<commit_message>
update lzs vocab namespace en conceptscheme base uri
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/luchtzuiveringssysteem/luchtzuiveringssysteem.xlsx
+++ b/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/luchtzuiveringssysteem/luchtzuiveringssysteem.xlsx
@@ -470,10 +470,10 @@
         <v>minValue</v>
       </c>
       <c r="W1" t="str">
-        <v>technishefiche</v>
+        <v>technischefiche</v>
       </c>
       <c r="X1" t="str">
-        <v>https://data\.omgeving\.vlaanderen\.be/ns/lzs#referentiewaardeType</v>
+        <v>referentiewaardeType</v>
       </c>
       <c r="Y1" t="str">
         <v>notation</v>
@@ -1255,13 +1255,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
       </c>
       <c r="H11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="I11" t="str">
         <v>Biobedspoelwaterproductie</v>
       </c>
       <c r="J11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="K11" t="str">
         <v>null</v>
@@ -1338,13 +1338,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0050</v>
       </c>
       <c r="H12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="I12" t="str">
         <v>Biobedspuiwaterproductie</v>
       </c>
       <c r="J12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="K12" t="str">
         <v>null</v>
@@ -1421,13 +1421,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0329</v>
       </c>
       <c r="H13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="I13" t="str">
         <v>Drukval over het systeem</v>
       </c>
       <c r="J13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="K13" t="str">
         <v>null</v>
@@ -1504,13 +1504,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0010</v>
       </c>
       <c r="H14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="I14" t="str">
         <v>Geleidbaarheid van het waswater</v>
       </c>
       <c r="J14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="K14" t="str">
         <v>null</v>
@@ -1587,13 +1587,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0050</v>
       </c>
       <c r="H15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="I15" t="str">
         <v>Spuiwaterproductie</v>
       </c>
       <c r="J15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="K15" t="str">
         <v>null</v>
@@ -1670,13 +1670,13 @@
         <v>null</v>
       </c>
       <c r="H16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="I16" t="str">
         <v>Stalbezetting</v>
       </c>
       <c r="J16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="K16" t="str">
         <v>null</v>
@@ -1753,13 +1753,13 @@
         <v>null</v>
       </c>
       <c r="H17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="I17" t="str">
         <v>SysteemStatus</v>
       </c>
       <c r="J17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="K17" t="str">
         <v>null</v>
@@ -1836,13 +1836,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
       </c>
       <c r="H18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="I18" t="str">
         <v>Waswaterdebiet over het waspakket</v>
       </c>
       <c r="J18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="K18" t="str">
         <v>null</v>
@@ -1919,13 +1919,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
       </c>
       <c r="H19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="I19" t="str">
         <v>Waswaterdebiet van de bevloeiing van het vulmateriaal</v>
       </c>
       <c r="J19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="K19" t="str">
         <v>null</v>
@@ -2002,13 +2002,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
       </c>
       <c r="H20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="I20" t="str">
         <v>Waswaterdebiet van de voorbevochtiging van de ingaande stallucht</v>
       </c>
       <c r="J20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="K20" t="str">
         <v>null</v>
@@ -2085,13 +2085,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0076</v>
       </c>
       <c r="H21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="I21" t="str">
         <v>Zuurtegraad van het waswater</v>
       </c>
       <c r="J21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="K21" t="str">
         <v>null</v>
@@ -2168,7 +2168,7 @@
         <v>null</v>
       </c>
       <c r="H22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs</v>
       </c>
       <c r="I22" t="str">
         <v>Luchtwassysteem</v>
@@ -2251,13 +2251,13 @@
         <v>null</v>
       </c>
       <c r="H23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs</v>
       </c>
       <c r="I23" t="str">
         <v>Luchtzuiveringssysteem</v>
       </c>
       <c r="J23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs</v>
       </c>
       <c r="K23" t="str">
         <v>null</v>
@@ -2334,13 +2334,13 @@
         <v>null</v>
       </c>
       <c r="H24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="I24" t="str">
         <v>Het elektronisch monitoringssysteem</v>
       </c>
       <c r="J24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="K24" t="str">
         <v>null</v>
@@ -2417,13 +2417,13 @@
         <v>null</v>
       </c>
       <c r="H25" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="I25" t="str">
         <v>Lucht</v>
       </c>
       <c r="J25" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="K25" t="str">
         <v>null</v>
@@ -2500,13 +2500,13 @@
         <v>null</v>
       </c>
       <c r="H26" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="I26" t="str">
         <v>Spuiwater</v>
       </c>
       <c r="J26" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="K26" t="str">
         <v>null</v>
@@ -2583,13 +2583,13 @@
         <v>null</v>
       </c>
       <c r="H27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="I27" t="str">
         <v>Stal</v>
       </c>
       <c r="J27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="K27" t="str">
         <v>null</v>
@@ -2666,13 +2666,13 @@
         <v>null</v>
       </c>
       <c r="H28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="I28" t="str">
         <v>Waswater</v>
       </c>
       <c r="J28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="K28" t="str">
         <v>null</v>
@@ -2749,13 +2749,13 @@
         <v>null</v>
       </c>
       <c r="H29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I29" t="str">
         <v>Zuurtegraad waswater &lt; 6 (S1 systeem)</v>
       </c>
       <c r="J29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K29" t="str">
         <v>null</v>
@@ -2832,13 +2832,13 @@
         <v>null</v>
       </c>
       <c r="H30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I30" t="str">
         <v>Waswaterdebiet afwijking naar beneden &gt; 20% (S2 systeem)</v>
       </c>
       <c r="J30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K30" t="str">
         <v>null</v>
@@ -2915,13 +2915,13 @@
         <v>null</v>
       </c>
       <c r="H31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I31" t="str">
         <v>Spuiwaterdebiet afwijking naar beneden &gt; 10% (S2 systeem)</v>
       </c>
       <c r="J31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K31" t="str">
         <v>null</v>
@@ -2998,13 +2998,13 @@
         <v>null</v>
       </c>
       <c r="H32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I32" t="str">
         <v>Drukval afwijking naar beneden &gt; 40% (S2 systeem)</v>
       </c>
       <c r="J32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K32" t="str">
         <v>null</v>
@@ -3081,13 +3081,13 @@
         <v>null</v>
       </c>
       <c r="H33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I33" t="str">
         <v>Drukval afwijking naar boven &gt; 40% (S2 systeem)</v>
       </c>
       <c r="J33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K33" t="str">
         <v>null</v>
@@ -3164,13 +3164,13 @@
         <v>null</v>
       </c>
       <c r="H34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I34" t="str">
         <v>Waswaterdebiet voorbevochtiging afwijking naar beneden &gt; 20% (S3 systeem)</v>
       </c>
       <c r="J34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K34" t="str">
         <v>null</v>
@@ -3247,13 +3247,13 @@
         <v>null</v>
       </c>
       <c r="H35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I35" t="str">
         <v>Waswaterdebiet bevloeiing afwijking naar beneden &gt; 20% (S3 systeem)</v>
       </c>
       <c r="J35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K35" t="str">
         <v>null</v>
@@ -3330,13 +3330,13 @@
         <v>null</v>
       </c>
       <c r="H36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I36" t="str">
         <v>Drukval afwijking naar boven &gt; 50 Pa (S3 systeem)</v>
       </c>
       <c r="J36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K36" t="str">
         <v>null</v>
@@ -3413,13 +3413,13 @@
         <v>null</v>
       </c>
       <c r="H37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I37" t="str">
         <v>Zuurtegraad waswater &gt; 8,5 (S1 systeem)</v>
       </c>
       <c r="J37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K37" t="str">
         <v>null</v>
@@ -3496,13 +3496,13 @@
         <v>null</v>
       </c>
       <c r="H38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I38" t="str">
         <v>Geleidbaarheid waswater &gt; maximale waarde (S1 systeem)</v>
       </c>
       <c r="J38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K38" t="str">
         <v>null</v>
@@ -3579,13 +3579,13 @@
         <v>null</v>
       </c>
       <c r="H39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I39" t="str">
         <v>Waswaterdebiet afwijking naar beneden &gt; 20% (S1 systeem)</v>
       </c>
       <c r="J39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K39" t="str">
         <v>null</v>
@@ -3662,13 +3662,13 @@
         <v>null</v>
       </c>
       <c r="H40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I40" t="str">
         <v>Spuiwaterdebiet afwijking naar beneden &gt; 10% (S1 systeem)</v>
       </c>
       <c r="J40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K40" t="str">
         <v>null</v>
@@ -3745,13 +3745,13 @@
         <v>null</v>
       </c>
       <c r="H41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I41" t="str">
         <v>Drukval afwijking naar beneden &gt; 40% (S1 systeem)</v>
       </c>
       <c r="J41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K41" t="str">
         <v>null</v>
@@ -3828,13 +3828,13 @@
         <v>null</v>
       </c>
       <c r="H42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I42" t="str">
         <v>Drukval afwijking naar boven &gt; 40% (S1 systeem)</v>
       </c>
       <c r="J42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K42" t="str">
         <v>null</v>
@@ -3911,13 +3911,13 @@
         <v>null</v>
       </c>
       <c r="H43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I43" t="str">
         <v>Zuurtegraad waswater afwijking naar boven &gt; 1 pH-eenheid (S2 systeem)</v>
       </c>
       <c r="J43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K43" t="str">
         <v>null</v>
@@ -3994,13 +3994,13 @@
         <v>null</v>
       </c>
       <c r="H44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="I44" t="str">
         <v>Geleidbaarheid waswater &gt; maximale waarde (S2 systeem)</v>
       </c>
       <c r="J44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="K44" t="str">
         <v>null</v>
@@ -4077,13 +4077,13 @@
         <v>null</v>
       </c>
       <c r="H45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I45" t="str">
         <v>Zuurtegraad waswater S1 systeem</v>
       </c>
       <c r="J45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K45" t="str">
         <v>null</v>
@@ -4160,13 +4160,13 @@
         <v>null</v>
       </c>
       <c r="H46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I46" t="str">
         <v>Drukval S2 systeem</v>
       </c>
       <c r="J46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K46" t="str">
         <v>null</v>
@@ -4243,13 +4243,13 @@
         <v>null</v>
       </c>
       <c r="H47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I47" t="str">
         <v>Waswaterdebiet voorbevochtiging S3 systeem</v>
       </c>
       <c r="J47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K47" t="str">
         <v>null</v>
@@ -4326,13 +4326,13 @@
         <v>null</v>
       </c>
       <c r="H48" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I48" t="str">
         <v>Waswaterdebiet bevloeiing S3 systeem</v>
       </c>
       <c r="J48" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K48" t="str">
         <v>null</v>
@@ -4409,13 +4409,13 @@
         <v>null</v>
       </c>
       <c r="H49" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I49" t="str">
         <v>Biobedspuiwaterproductie S3 systeem</v>
       </c>
       <c r="J49" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K49" t="str">
         <v>null</v>
@@ -4492,13 +4492,13 @@
         <v>null</v>
       </c>
       <c r="H50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I50" t="str">
         <v>Biobedspoelwaterproductie S3 systeem</v>
       </c>
       <c r="J50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K50" t="str">
         <v>null</v>
@@ -4575,13 +4575,13 @@
         <v>null</v>
       </c>
       <c r="H51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I51" t="str">
         <v>Drukval S3 systeem</v>
       </c>
       <c r="J51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K51" t="str">
         <v>null</v>
@@ -4658,13 +4658,13 @@
         <v>null</v>
       </c>
       <c r="H52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I52" t="str">
         <v>Geleidbaarheid waswater S1 systeem</v>
       </c>
       <c r="J52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K52" t="str">
         <v>null</v>
@@ -4741,13 +4741,13 @@
         <v>null</v>
       </c>
       <c r="H53" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I53" t="str">
         <v>Waswaterdebiet S1 systeem</v>
       </c>
       <c r="J53" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K53" t="str">
         <v>null</v>
@@ -4824,13 +4824,13 @@
         <v>null</v>
       </c>
       <c r="H54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I54" t="str">
         <v>Spuiwaterdebiet S1 systeem</v>
       </c>
       <c r="J54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K54" t="str">
         <v>null</v>
@@ -4907,13 +4907,13 @@
         <v>null</v>
       </c>
       <c r="H55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I55" t="str">
         <v>Drukval S1 systeem</v>
       </c>
       <c r="J55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K55" t="str">
         <v>null</v>
@@ -4990,13 +4990,13 @@
         <v>null</v>
       </c>
       <c r="H56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I56" t="str">
         <v>Zuurtegraad waswater S2 systeem</v>
       </c>
       <c r="J56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K56" t="str">
         <v>null</v>
@@ -5073,13 +5073,13 @@
         <v>null</v>
       </c>
       <c r="H57" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I57" t="str">
         <v>Geleidbaarheid waswater S2 systeem</v>
       </c>
       <c r="J57" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K57" t="str">
         <v>null</v>
@@ -5156,13 +5156,13 @@
         <v>null</v>
       </c>
       <c r="H58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I58" t="str">
         <v>Waswaterdebiet S2 systeem</v>
       </c>
       <c r="J58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K58" t="str">
         <v>null</v>
@@ -5239,13 +5239,13 @@
         <v>null</v>
       </c>
       <c r="H59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="I59" t="str">
         <v>Spuiwaterdebiet S2 systeem</v>
       </c>
       <c r="J59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="K59" t="str">
         <v>null</v>
@@ -5322,7 +5322,7 @@
         <v>null</v>
       </c>
       <c r="H60" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs</v>
       </c>
       <c r="I60" t="str">
         <v>Biologisch luchtwassysteem</v>
@@ -5405,7 +5405,7 @@
         <v>null</v>
       </c>
       <c r="H61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs</v>
       </c>
       <c r="I61" t="str">
         <v>Chemisch luchtwassysteem</v>
@@ -5488,7 +5488,7 @@
         <v>null</v>
       </c>
       <c r="H62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs</v>
       </c>
       <c r="I62" t="str">
         <v>Biobed</v>
@@ -5571,13 +5571,13 @@
         <v>null</v>
       </c>
       <c r="H63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsst</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
       </c>
       <c r="I63" t="str">
         <v>Stal in gebruik, dieren aanwezig.</v>
       </c>
       <c r="J63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsst</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
       </c>
       <c r="K63" t="str">
         <v>null</v>
@@ -5654,13 +5654,13 @@
         <v>null</v>
       </c>
       <c r="H64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsst</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
       </c>
       <c r="I64" t="str">
         <v>Lege stal</v>
       </c>
       <c r="J64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsst</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
       </c>
       <c r="K64" t="str">
         <v>null</v>
@@ -5737,13 +5737,13 @@
         <v>null</v>
       </c>
       <c r="H65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzss</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="I65" t="str">
         <v>In onderhoud</v>
       </c>
       <c r="J65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzss</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="K65" t="str">
         <v>null</v>
@@ -5820,13 +5820,13 @@
         <v>null</v>
       </c>
       <c r="H66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzss</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="I66" t="str">
         <v>Operationeel</v>
       </c>
       <c r="J66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzss</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="K66" t="str">
         <v>null</v>
@@ -5903,13 +5903,13 @@
         <v>null</v>
       </c>
       <c r="H67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzss</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="I67" t="str">
         <v>Storing</v>
       </c>
       <c r="J67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzss</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="K67" t="str">
         <v>null</v>
@@ -5965,7 +5965,7 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs</v>
       </c>
       <c r="B68" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6048,7 +6048,7 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="B69" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6131,7 +6131,7 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="B70" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6214,7 +6214,7 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="B71" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6297,7 +6297,7 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzss</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="B72" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6380,7 +6380,7 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzsst</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
       </c>
       <c r="B73" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6463,7 +6463,7 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="B74" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>

</xml_diff>

<commit_message>
Add qudt:relevantUnit and lzsns:relevantDataType to concepts of conceptscheme:lzs-param-norm. Change conceptscheme:lzs to conceptscheme:lzstype. Add lzsns:relevantProperty to concepts of conceptscheme:lzstype. New concept lzss:gereinigd. New conceptscheme:bedrijfsklasse.
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/luchtzuiveringssysteem/luchtzuiveringssysteem.xlsx
+++ b/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/luchtzuiveringssysteem/luchtzuiveringssysteem.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA74"/>
+  <dimension ref="A1:AA79"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -413,22 +413,22 @@
         <v>applicableUnit</v>
       </c>
       <c r="D1" t="str">
+        <v>inScheme</v>
+      </c>
+      <c r="E1" t="str">
+        <v>prefLabel</v>
+      </c>
+      <c r="F1" t="str">
+        <v>topConceptOf</v>
+      </c>
+      <c r="G1" t="str">
         <v>subject</v>
       </c>
-      <c r="E1" t="str">
+      <c r="H1" t="str">
         <v>relevantQuantityKind</v>
       </c>
-      <c r="F1" t="str">
+      <c r="I1" t="str">
         <v>seeAlso</v>
-      </c>
-      <c r="G1" t="str">
-        <v>inScheme</v>
-      </c>
-      <c r="H1" t="str">
-        <v>prefLabel</v>
-      </c>
-      <c r="I1" t="str">
-        <v>topConceptOf</v>
       </c>
       <c r="J1" t="str">
         <v>relevantLZS</v>
@@ -1234,34 +1234,34 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/bedrijfklasse/1</v>
       </c>
       <c r="B11" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C11" t="str">
         <v>null</v>
       </c>
       <c r="D11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/bedrijfsklasse</v>
       </c>
       <c r="E11" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Volume</v>
+        <v>Klasse 1</v>
       </c>
       <c r="F11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/bedrijfsklasse</v>
       </c>
       <c r="G11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>null</v>
       </c>
       <c r="H11" t="str">
-        <v>Biobedspoelwaterproductie</v>
+        <v>null</v>
       </c>
       <c r="I11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>null</v>
       </c>
       <c r="J11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>null</v>
       </c>
       <c r="K11" t="str">
         <v>null</v>
@@ -1317,34 +1317,34 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/bedrijfklasse/2</v>
       </c>
       <c r="B12" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C12" t="str">
         <v>null</v>
       </c>
       <c r="D12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/bedrijfsklasse</v>
       </c>
       <c r="E12" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Volume</v>
+        <v>Klasse 2</v>
       </c>
       <c r="F12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0050</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/bedrijfsklasse</v>
       </c>
       <c r="G12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>null</v>
       </c>
       <c r="H12" t="str">
-        <v>Biobedspuiwaterproductie</v>
+        <v>null</v>
       </c>
       <c r="I12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>null</v>
       </c>
       <c r="J12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>null</v>
       </c>
       <c r="K12" t="str">
         <v>null</v>
@@ -1400,34 +1400,34 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/bedrijfklasse/3</v>
       </c>
       <c r="B13" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C13" t="str">
         <v>null</v>
       </c>
       <c r="D13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/lucht</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/bedrijfsklasse</v>
       </c>
       <c r="E13" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Fugacity|http://qudt.org/vocab/quantitykind/VaporPressure</v>
+        <v>Klasse 3</v>
       </c>
       <c r="F13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0329</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/bedrijfsklasse</v>
       </c>
       <c r="G13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>null</v>
       </c>
       <c r="H13" t="str">
-        <v>Drukval over het systeem</v>
+        <v>null</v>
       </c>
       <c r="I13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>null</v>
       </c>
       <c r="J13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>null</v>
       </c>
       <c r="K13" t="str">
         <v>null</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie</v>
       </c>
       <c r="B14" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -1492,25 +1492,25 @@
         <v>null</v>
       </c>
       <c r="D14" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Biobedspoelwaterproductie</v>
+      </c>
+      <c r="F14" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+      </c>
+      <c r="G14" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
       </c>
-      <c r="E14" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Conductivity</v>
-      </c>
-      <c r="F14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0010</v>
-      </c>
-      <c r="G14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
-      </c>
       <c r="H14" t="str">
-        <v>Geleidbaarheid van het waswater</v>
+        <v>http://qudt.org/vocab/quantitykind/Volume</v>
       </c>
       <c r="I14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
       </c>
       <c r="J14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K14" t="str">
         <v>null</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie</v>
       </c>
       <c r="B15" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -1575,25 +1575,25 @@
         <v>null</v>
       </c>
       <c r="D15" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Biobedspuiwaterproductie</v>
+      </c>
+      <c r="F15" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+      </c>
+      <c r="G15" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater</v>
       </c>
-      <c r="E15" t="str">
+      <c r="H15" t="str">
         <v>http://qudt.org/vocab/quantitykind/Volume</v>
       </c>
-      <c r="F15" t="str">
+      <c r="I15" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0050</v>
       </c>
-      <c r="G15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
-      </c>
-      <c r="H15" t="str">
-        <v>Spuiwaterproductie</v>
-      </c>
-      <c r="I15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
-      </c>
       <c r="J15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K15" t="str">
         <v>null</v>
@@ -1649,7 +1649,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="B16" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -1658,22 +1658,22 @@
         <v>null</v>
       </c>
       <c r="D16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/stal</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="E16" t="str">
-        <v>null</v>
+        <v>Drukval over het systeem</v>
       </c>
       <c r="F16" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="G16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/lucht</v>
       </c>
       <c r="H16" t="str">
-        <v>Stalbezetting</v>
+        <v>http://qudt.org/vocab/quantitykind/Fugacity|http://qudt.org/vocab/quantitykind/VaporPressure</v>
       </c>
       <c r="I16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0329</v>
       </c>
       <c r="J16" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
@@ -1732,7 +1732,7 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="B17" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -1741,25 +1741,25 @@
         <v>null</v>
       </c>
       <c r="D17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/hetelektronischmonitoringssysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="E17" t="str">
-        <v>null</v>
+        <v>Geleidbaarheid van het waswater</v>
       </c>
       <c r="F17" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="G17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
       </c>
       <c r="H17" t="str">
-        <v>SysteemStatus</v>
+        <v>http://qudt.org/vocab/quantitykind/Conductivity</v>
       </c>
       <c r="I17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0010</v>
       </c>
       <c r="J17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K17" t="str">
         <v>null</v>
@@ -1815,7 +1815,7 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
       </c>
       <c r="B18" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -1824,22 +1824,22 @@
         <v>null</v>
       </c>
       <c r="D18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="E18" t="str">
-        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate|http://qudt.org/vocab/quantitykind/VolumePerTime</v>
+        <v>Spuiwaterproductie</v>
       </c>
       <c r="F18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="G18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater</v>
       </c>
       <c r="H18" t="str">
-        <v>Waswaterdebiet over het waspakket</v>
+        <v>http://qudt.org/vocab/quantitykind/Volume</v>
       </c>
       <c r="I18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0050</v>
       </c>
       <c r="J18" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
@@ -1898,7 +1898,7 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting</v>
       </c>
       <c r="B19" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -1907,25 +1907,25 @@
         <v>null</v>
       </c>
       <c r="D19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="E19" t="str">
-        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate|http://qudt.org/vocab/quantitykind/VolumePerTime</v>
+        <v>Stalbezetting</v>
       </c>
       <c r="F19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="G19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/stal</v>
       </c>
       <c r="H19" t="str">
-        <v>Waswaterdebiet van de bevloeiing van het vulmateriaal</v>
+        <v>null</v>
       </c>
       <c r="I19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>null</v>
       </c>
       <c r="J19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K19" t="str">
         <v>null</v>
@@ -1981,7 +1981,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus</v>
       </c>
       <c r="B20" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -1990,25 +1990,25 @@
         <v>null</v>
       </c>
       <c r="D20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="E20" t="str">
-        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate|http://qudt.org/vocab/quantitykind/VolumePerTime</v>
+        <v>SysteemStatus</v>
       </c>
       <c r="F20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="G20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/hetelektronischmonitoringssysteem</v>
       </c>
       <c r="H20" t="str">
-        <v>Waswaterdebiet van de voorbevochtiging van de ingaande stallucht</v>
+        <v>null</v>
       </c>
       <c r="I20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>null</v>
       </c>
       <c r="J20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K20" t="str">
         <v>null</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
       </c>
       <c r="B21" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -2073,22 +2073,22 @@
         <v>null</v>
       </c>
       <c r="D21" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Waswaterdebiet over het waspakket</v>
+      </c>
+      <c r="F21" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+      </c>
+      <c r="G21" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
       </c>
-      <c r="E21" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Acidity|http://qudt.org/vocab/quantitykind/Basicity</v>
-      </c>
-      <c r="F21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0076</v>
-      </c>
-      <c r="G21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
-      </c>
       <c r="H21" t="str">
-        <v>Zuurtegraad van het waswater</v>
+        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate|http://qudt.org/vocab/quantitykind/VolumePerTime</v>
       </c>
       <c r="I21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
       </c>
       <c r="J21" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
@@ -2147,34 +2147,34 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/hetelektronischmonitoringssysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing</v>
       </c>
       <c r="B22" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
       </c>
       <c r="C22" t="str">
         <v>null</v>
       </c>
       <c r="D22" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="E22" t="str">
-        <v>null</v>
+        <v>Waswaterdebiet van de bevloeiing van het vulmateriaal</v>
       </c>
       <c r="F22" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="G22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
       </c>
       <c r="H22" t="str">
-        <v>Het elektronisch monitoringssysteem</v>
+        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate|http://qudt.org/vocab/quantitykind/VolumePerTime</v>
       </c>
       <c r="I22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
       </c>
       <c r="J22" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K22" t="str">
         <v>null</v>
@@ -2230,34 +2230,34 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/lucht</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
       </c>
       <c r="B23" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
       </c>
       <c r="C23" t="str">
         <v>null</v>
       </c>
       <c r="D23" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="E23" t="str">
-        <v>null</v>
+        <v>Waswaterdebiet van de voorbevochtiging van de ingaande stallucht</v>
       </c>
       <c r="F23" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="G23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
       </c>
       <c r="H23" t="str">
-        <v>Lucht</v>
+        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate|http://qudt.org/vocab/quantitykind/VolumePerTime</v>
       </c>
       <c r="I23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
       </c>
       <c r="J23" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K23" t="str">
         <v>null</v>
@@ -2313,34 +2313,34 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="B24" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
       </c>
       <c r="C24" t="str">
         <v>null</v>
       </c>
       <c r="D24" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="E24" t="str">
-        <v>null</v>
+        <v>Zuurtegraad van het waswater</v>
       </c>
       <c r="F24" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="G24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
       </c>
       <c r="H24" t="str">
-        <v>Spuiwater</v>
+        <v>http://qudt.org/vocab/quantitykind/Acidity|http://qudt.org/vocab/quantitykind/Basicity</v>
       </c>
       <c r="I24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0076</v>
       </c>
       <c r="J24" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K24" t="str">
         <v>null</v>
@@ -2396,7 +2396,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/stal</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/hetelektronischmonitoringssysteem</v>
       </c>
       <c r="B25" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
@@ -2405,22 +2405,22 @@
         <v>null</v>
       </c>
       <c r="D25" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="E25" t="str">
-        <v>null</v>
+        <v>Het elektronisch monitoringssysteem</v>
       </c>
       <c r="F25" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="G25" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>null</v>
       </c>
       <c r="H25" t="str">
-        <v>Stal</v>
+        <v>null</v>
       </c>
       <c r="I25" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>null</v>
       </c>
       <c r="J25" t="str">
         <v>null</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/lucht</v>
       </c>
       <c r="B26" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
@@ -2488,22 +2488,22 @@
         <v>null</v>
       </c>
       <c r="D26" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="E26" t="str">
-        <v>null</v>
+        <v>Lucht</v>
       </c>
       <c r="F26" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="G26" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>null</v>
       </c>
       <c r="H26" t="str">
-        <v>Waswater</v>
+        <v>null</v>
       </c>
       <c r="I26" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>null</v>
       </c>
       <c r="J26" t="str">
         <v>null</v>
@@ -2562,49 +2562,49 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater</v>
       </c>
       <c r="B27" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
       </c>
       <c r="C27" t="str">
         <v>null</v>
       </c>
       <c r="D27" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="E27" t="str">
-        <v>null</v>
+        <v>Spuiwater</v>
       </c>
       <c r="F27" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="G27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H27" t="str">
-        <v>Zuurtegraad waswater &lt; 6 (S1 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>null</v>
       </c>
       <c r="K27" t="str">
-        <v>De zuurtegraad van het waswater is kleiner dan 6</v>
+        <v>null</v>
       </c>
       <c r="L27" t="str">
-        <v>De zuurtegraad van het waswater is kleiner dan 6|&lt; 6</v>
+        <v>null</v>
       </c>
       <c r="M27" t="str">
-        <v>&lt; 6</v>
+        <v>null</v>
       </c>
       <c r="N27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>null</v>
       </c>
       <c r="O27" t="str">
-        <v>6</v>
+        <v>null</v>
       </c>
       <c r="P27" t="str">
         <v>null</v>
@@ -2645,52 +2645,52 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/10</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/stal</v>
       </c>
       <c r="B28" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
       </c>
       <c r="C28" t="str">
         <v>null</v>
       </c>
       <c r="D28" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="E28" t="str">
-        <v>null</v>
+        <v>Stal</v>
       </c>
       <c r="F28" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="G28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H28" t="str">
-        <v>Waswaterdebiet afwijking naar beneden &gt; 20% (S2 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>null</v>
       </c>
       <c r="K28" t="str">
-        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>null</v>
       </c>
       <c r="L28" t="str">
-        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>null</v>
       </c>
       <c r="M28" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>null</v>
       </c>
       <c r="N28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
+        <v>null</v>
       </c>
       <c r="O28" t="str">
-        <v>0.8</v>
+        <v>null</v>
       </c>
       <c r="P28" t="str">
-        <v>product</v>
+        <v>null</v>
       </c>
       <c r="Q28" t="str">
         <v>null</v>
@@ -2728,52 +2728,52 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/11</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
       </c>
       <c r="B29" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
       </c>
       <c r="C29" t="str">
         <v>null</v>
       </c>
       <c r="D29" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="E29" t="str">
-        <v>null</v>
+        <v>Waswater</v>
       </c>
       <c r="F29" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="G29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H29" t="str">
-        <v>Spuiwaterdebiet afwijking naar beneden &gt; 10% (S2 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>null</v>
       </c>
       <c r="K29" t="str">
-        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>null</v>
       </c>
       <c r="L29" t="str">
-        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
+        <v>null</v>
       </c>
       <c r="M29" t="str">
-        <v>&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
+        <v>null</v>
       </c>
       <c r="N29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
+        <v>null</v>
       </c>
       <c r="O29" t="str">
-        <v>0.9</v>
+        <v>null</v>
       </c>
       <c r="P29" t="str">
-        <v>product</v>
+        <v>null</v>
       </c>
       <c r="Q29" t="str">
         <v>null</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/12</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/1</v>
       </c>
       <c r="B30" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2820,43 +2820,43 @@
         <v>null</v>
       </c>
       <c r="D30" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E30" t="str">
-        <v>null</v>
+        <v>Zuurtegraad waswater &lt; 6 (S1 systeem)</v>
       </c>
       <c r="F30" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H30" t="str">
-        <v>Drukval afwijking naar beneden &gt; 40% (S2 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K30" t="str">
-        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De zuurtegraad van het waswater is kleiner dan 6</v>
       </c>
       <c r="L30" t="str">
-        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>De zuurtegraad van het waswater is kleiner dan 6|&lt; 6</v>
       </c>
       <c r="M30" t="str">
-        <v>&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>&lt; 6</v>
       </c>
       <c r="N30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="O30" t="str">
-        <v>0.6</v>
+        <v>6</v>
       </c>
       <c r="P30" t="str">
-        <v>product</v>
+        <v>null</v>
       </c>
       <c r="Q30" t="str">
         <v>null</v>
@@ -2894,7 +2894,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/13</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/10</v>
       </c>
       <c r="B31" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2903,46 +2903,46 @@
         <v>null</v>
       </c>
       <c r="D31" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E31" t="str">
-        <v>null</v>
+        <v>Waswaterdebiet afwijking naar beneden &gt; 20% (S2 systeem)</v>
       </c>
       <c r="F31" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H31" t="str">
-        <v>Drukval afwijking naar boven &gt; 40% (S2 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J31" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K31" t="str">
-        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L31" t="str">
-        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="M31" t="str">
-        <v>&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="N31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
       </c>
       <c r="O31" t="str">
-        <v>null</v>
+        <v>0.8</v>
       </c>
       <c r="P31" t="str">
         <v>product</v>
       </c>
       <c r="Q31" t="str">
-        <v>1.4</v>
+        <v>null</v>
       </c>
       <c r="R31" t="str">
         <v>null</v>
@@ -2977,7 +2977,7 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/14</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/11</v>
       </c>
       <c r="B32" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2986,40 +2986,40 @@
         <v>null</v>
       </c>
       <c r="D32" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E32" t="str">
-        <v>null</v>
+        <v>Spuiwaterdebiet afwijking naar beneden &gt; 10% (S2 systeem)</v>
       </c>
       <c r="F32" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H32" t="str">
-        <v>Waswaterdebiet voorbevochtiging afwijking naar beneden &gt; 20% (S3 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K32" t="str">
-        <v>Het waswaterdebiet van de voorbevochtiging wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L32" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)|Het waswaterdebiet van de voorbevochtiging wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
       </c>
       <c r="M32" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
       </c>
       <c r="N32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
       </c>
       <c r="O32" t="str">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="P32" t="str">
         <v>product</v>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/15</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/12</v>
       </c>
       <c r="B33" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3069,40 +3069,40 @@
         <v>null</v>
       </c>
       <c r="D33" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E33" t="str">
-        <v>null</v>
+        <v>Drukval afwijking naar beneden &gt; 40% (S2 systeem)</v>
       </c>
       <c r="F33" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H33" t="str">
-        <v>Waswaterdebiet bevloeiing afwijking naar beneden &gt; 20% (S3 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K33" t="str">
-        <v>Het waswaterdebiet van de bevloeiing wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L33" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)|Het waswaterdebiet van de bevloeiing wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="M33" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="N33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="O33" t="str">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="P33" t="str">
         <v>product</v>
@@ -3143,7 +3143,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/16</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/13</v>
       </c>
       <c r="B34" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3152,34 +3152,34 @@
         <v>null</v>
       </c>
       <c r="D34" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E34" t="str">
-        <v>null</v>
+        <v>Drukval afwijking naar boven &gt; 40% (S2 systeem)</v>
       </c>
       <c r="F34" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H34" t="str">
-        <v>Drukval afwijking naar boven &gt; 50 Pa (S3 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K34" t="str">
-        <v>De drukval wijkt meer dan 50 Pa naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L34" t="str">
-        <v>De drukval wijkt meer dan 50 Pa naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 50 Pa + waarde technische fiche (afwijking &gt; 50 Pa)</v>
+        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="M34" t="str">
-        <v>&gt; 50 Pa + waarde technische fiche (afwijking &gt; 50 Pa)</v>
+        <v>&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="N34" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
@@ -3188,10 +3188,10 @@
         <v>null</v>
       </c>
       <c r="P34" t="str">
-        <v>som</v>
+        <v>product</v>
       </c>
       <c r="Q34" t="str">
-        <v>50</v>
+        <v>1.4</v>
       </c>
       <c r="R34" t="str">
         <v>null</v>
@@ -3226,7 +3226,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/14</v>
       </c>
       <c r="B35" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3235,46 +3235,46 @@
         <v>null</v>
       </c>
       <c r="D35" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E35" t="str">
-        <v>null</v>
+        <v>Waswaterdebiet voorbevochtiging afwijking naar beneden &gt; 20% (S3 systeem)</v>
       </c>
       <c r="F35" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H35" t="str">
-        <v>Zuurtegraad waswater &gt; 8,5 (S1 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K35" t="str">
-        <v>De zuurtegraad van het waswater is groter dan 8,5</v>
+        <v>Het waswaterdebiet van de voorbevochtiging wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L35" t="str">
-        <v>De zuurtegraad van het waswater is groter dan 8,5|&gt; 8,5</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)|Het waswaterdebiet van de voorbevochtiging wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="M35" t="str">
-        <v>&gt; 8,5</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="N35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
       </c>
       <c r="O35" t="str">
-        <v>null</v>
+        <v>0.8</v>
       </c>
       <c r="P35" t="str">
-        <v>null</v>
+        <v>product</v>
       </c>
       <c r="Q35" t="str">
-        <v>8.5</v>
+        <v>null</v>
       </c>
       <c r="R35" t="str">
         <v>null</v>
@@ -3309,7 +3309,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/15</v>
       </c>
       <c r="B36" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3318,46 +3318,46 @@
         <v>null</v>
       </c>
       <c r="D36" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E36" t="str">
-        <v>null</v>
+        <v>Waswaterdebiet bevloeiing afwijking naar beneden &gt; 20% (S3 systeem)</v>
       </c>
       <c r="F36" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H36" t="str">
-        <v>Geleidbaarheid waswater &gt; maximale waarde (S1 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K36" t="str">
-        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het waswaterdebiet van de bevloeiing wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L36" t="str">
-        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.|&gt; waarde technische fiche</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)|Het waswaterdebiet van de bevloeiing wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="M36" t="str">
-        <v>&gt; waarde technische fiche</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="N36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing</v>
       </c>
       <c r="O36" t="str">
-        <v>null</v>
+        <v>0.8</v>
       </c>
       <c r="P36" t="str">
-        <v>som</v>
+        <v>product</v>
       </c>
       <c r="Q36" t="str">
-        <v>0</v>
+        <v>null</v>
       </c>
       <c r="R36" t="str">
         <v>null</v>
@@ -3392,7 +3392,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/4</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/16</v>
       </c>
       <c r="B37" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3401,46 +3401,46 @@
         <v>null</v>
       </c>
       <c r="D37" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E37" t="str">
-        <v>null</v>
+        <v>Drukval afwijking naar boven &gt; 50 Pa (S3 systeem)</v>
       </c>
       <c r="F37" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H37" t="str">
-        <v>Waswaterdebiet afwijking naar beneden &gt; 20% (S1 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K37" t="str">
-        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De drukval wijkt meer dan 50 Pa naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L37" t="str">
-        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>De drukval wijkt meer dan 50 Pa naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 50 Pa + waarde technische fiche (afwijking &gt; 50 Pa)</v>
       </c>
       <c r="M37" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>&gt; 50 Pa + waarde technische fiche (afwijking &gt; 50 Pa)</v>
       </c>
       <c r="N37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="O37" t="str">
-        <v>0.8</v>
+        <v>null</v>
       </c>
       <c r="P37" t="str">
-        <v>product</v>
+        <v>som</v>
       </c>
       <c r="Q37" t="str">
-        <v>null</v>
+        <v>50</v>
       </c>
       <c r="R37" t="str">
         <v>null</v>
@@ -3475,7 +3475,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/5</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/2</v>
       </c>
       <c r="B38" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3484,46 +3484,46 @@
         <v>null</v>
       </c>
       <c r="D38" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E38" t="str">
-        <v>null</v>
+        <v>Zuurtegraad waswater &gt; 8,5 (S1 systeem)</v>
       </c>
       <c r="F38" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H38" t="str">
-        <v>Spuiwaterdebiet afwijking naar beneden &gt; 10% (S1 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J38" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K38" t="str">
-        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De zuurtegraad van het waswater is groter dan 8,5</v>
       </c>
       <c r="L38" t="str">
-        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
+        <v>De zuurtegraad van het waswater is groter dan 8,5|&gt; 8,5</v>
       </c>
       <c r="M38" t="str">
-        <v>&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
+        <v>&gt; 8,5</v>
       </c>
       <c r="N38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="O38" t="str">
-        <v>0.9</v>
+        <v>null</v>
       </c>
       <c r="P38" t="str">
-        <v>product</v>
+        <v>null</v>
       </c>
       <c r="Q38" t="str">
-        <v>null</v>
+        <v>8.5</v>
       </c>
       <c r="R38" t="str">
         <v>null</v>
@@ -3558,7 +3558,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/6</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/3</v>
       </c>
       <c r="B39" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3567,46 +3567,46 @@
         <v>null</v>
       </c>
       <c r="D39" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E39" t="str">
-        <v>null</v>
+        <v>Geleidbaarheid waswater &gt; maximale waarde (S1 systeem)</v>
       </c>
       <c r="F39" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H39" t="str">
-        <v>Drukval afwijking naar beneden &gt; 40% (S1 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J39" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K39" t="str">
-        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L39" t="str">
-        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.|&gt; waarde technische fiche</v>
       </c>
       <c r="M39" t="str">
-        <v>&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>&gt; waarde technische fiche</v>
       </c>
       <c r="N39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="O39" t="str">
-        <v>0.6</v>
+        <v>null</v>
       </c>
       <c r="P39" t="str">
-        <v>product</v>
+        <v>som</v>
       </c>
       <c r="Q39" t="str">
-        <v>null</v>
+        <v>0</v>
       </c>
       <c r="R39" t="str">
         <v>null</v>
@@ -3641,7 +3641,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/7</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/4</v>
       </c>
       <c r="B40" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3650,46 +3650,46 @@
         <v>null</v>
       </c>
       <c r="D40" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E40" t="str">
-        <v>null</v>
+        <v>Waswaterdebiet afwijking naar beneden &gt; 20% (S1 systeem)</v>
       </c>
       <c r="F40" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H40" t="str">
-        <v>Drukval afwijking naar boven &gt; 40% (S1 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J40" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K40" t="str">
-        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L40" t="str">
-        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="M40" t="str">
-        <v>&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="N40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
       </c>
       <c r="O40" t="str">
-        <v>null</v>
+        <v>0.8</v>
       </c>
       <c r="P40" t="str">
         <v>product</v>
       </c>
       <c r="Q40" t="str">
-        <v>1.4</v>
+        <v>null</v>
       </c>
       <c r="R40" t="str">
         <v>null</v>
@@ -3724,7 +3724,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/8</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/5</v>
       </c>
       <c r="B41" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3733,46 +3733,46 @@
         <v>null</v>
       </c>
       <c r="D41" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E41" t="str">
-        <v>null</v>
+        <v>Spuiwaterdebiet afwijking naar beneden &gt; 10% (S1 systeem)</v>
       </c>
       <c r="F41" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H41" t="str">
-        <v>Zuurtegraad waswater afwijking naar boven &gt; 1 pH-eenheid (S2 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K41" t="str">
-        <v>De zuurtegraad van het waswater wijkt meer dan 1 pH-eenheid naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L41" t="str">
-        <v>De zuurtegraad van het waswater wijkt meer dan 1 pH-eenheid naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1 pH + waarde technische fiche (afwijking &gt; 1pH)</v>
+        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
       </c>
       <c r="M41" t="str">
-        <v>&gt; 1 pH + waarde technische fiche (afwijking &gt; 1pH)</v>
+        <v>&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
       </c>
       <c r="N41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
       </c>
       <c r="O41" t="str">
-        <v>null</v>
+        <v>0.9</v>
       </c>
       <c r="P41" t="str">
-        <v>som</v>
+        <v>product</v>
       </c>
       <c r="Q41" t="str">
-        <v>1</v>
+        <v>null</v>
       </c>
       <c r="R41" t="str">
         <v>null</v>
@@ -3807,7 +3807,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/9</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/6</v>
       </c>
       <c r="B42" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3816,46 +3816,46 @@
         <v>null</v>
       </c>
       <c r="D42" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E42" t="str">
-        <v>null</v>
+        <v>Drukval afwijking naar beneden &gt; 40% (S1 systeem)</v>
       </c>
       <c r="F42" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="H42" t="str">
-        <v>Geleidbaarheid waswater &gt; maximale waarde (S2 systeem)</v>
+        <v>null</v>
       </c>
       <c r="I42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="J42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K42" t="str">
-        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L42" t="str">
-        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.|&gt; waarde technische fiche</v>
+        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="M42" t="str">
-        <v>&gt; waarde technische fiche</v>
+        <v>&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="N42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="O42" t="str">
-        <v>null</v>
+        <v>0.6</v>
       </c>
       <c r="P42" t="str">
-        <v>som</v>
+        <v>product</v>
       </c>
       <c r="Q42" t="str">
-        <v>0</v>
+        <v>null</v>
       </c>
       <c r="R42" t="str">
         <v>null</v>
@@ -3890,58 +3890,58 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/7</v>
       </c>
       <c r="B43" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C43" t="str">
-        <v>http://qudt.org/vocab/unit/PH</v>
+        <v>null</v>
       </c>
       <c r="D43" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E43" t="str">
-        <v>null</v>
+        <v>Drukval afwijking naar boven &gt; 40% (S1 systeem)</v>
       </c>
       <c r="F43" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H43" t="str">
-        <v>Zuurtegraad waswater S1 systeem</v>
+        <v>null</v>
       </c>
       <c r="I43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J43" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K43" t="str">
-        <v>null</v>
+        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L43" t="str">
-        <v>null</v>
+        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="M43" t="str">
-        <v>null</v>
+        <v>&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="N43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="O43" t="str">
         <v>null</v>
       </c>
       <c r="P43" t="str">
-        <v>null</v>
+        <v>product</v>
       </c>
       <c r="Q43" t="str">
-        <v>null</v>
+        <v>1.4</v>
       </c>
       <c r="R43" t="str">
-        <v>false</v>
+        <v>null</v>
       </c>
       <c r="S43" t="str">
         <v>null</v>
@@ -3973,61 +3973,61 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/10</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/8</v>
       </c>
       <c r="B44" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C44" t="str">
-        <v>http://qudt.org/vocab/unit/PA</v>
+        <v>null</v>
       </c>
       <c r="D44" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E44" t="str">
-        <v>null</v>
+        <v>Zuurtegraad waswater afwijking naar boven &gt; 1 pH-eenheid (S2 systeem)</v>
       </c>
       <c r="F44" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H44" t="str">
-        <v>Drukval S2 systeem</v>
+        <v>null</v>
       </c>
       <c r="I44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J44" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K44" t="str">
-        <v>null</v>
+        <v>De zuurtegraad van het waswater wijkt meer dan 1 pH-eenheid naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L44" t="str">
-        <v>null</v>
+        <v>De zuurtegraad van het waswater wijkt meer dan 1 pH-eenheid naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1 pH + waarde technische fiche (afwijking &gt; 1pH)</v>
       </c>
       <c r="M44" t="str">
-        <v>null</v>
+        <v>&gt; 1 pH + waarde technische fiche (afwijking &gt; 1pH)</v>
       </c>
       <c r="N44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="O44" t="str">
         <v>null</v>
       </c>
       <c r="P44" t="str">
-        <v>null</v>
+        <v>som</v>
       </c>
       <c r="Q44" t="str">
-        <v>null</v>
+        <v>1</v>
       </c>
       <c r="R44" t="str">
-        <v>true</v>
+        <v>null</v>
       </c>
       <c r="S44" t="str">
-        <v>exact</v>
+        <v>null</v>
       </c>
       <c r="T44" t="str">
         <v>null</v>
@@ -4056,61 +4056,61 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/11</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/9</v>
       </c>
       <c r="B45" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C45" t="str">
-        <v>http://qudt.org/vocab/unit/M3-PER-HR</v>
+        <v>null</v>
       </c>
       <c r="D45" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="E45" t="str">
-        <v>null</v>
+        <v>Geleidbaarheid waswater &gt; maximale waarde (S2 systeem)</v>
       </c>
       <c r="F45" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="G45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H45" t="str">
-        <v>Waswaterdebiet voorbevochtiging S3 systeem</v>
+        <v>null</v>
       </c>
       <c r="I45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K45" t="str">
-        <v>null</v>
+        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L45" t="str">
-        <v>null</v>
+        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.|&gt; waarde technische fiche</v>
       </c>
       <c r="M45" t="str">
-        <v>null</v>
+        <v>&gt; waarde technische fiche</v>
       </c>
       <c r="N45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="O45" t="str">
         <v>null</v>
       </c>
       <c r="P45" t="str">
-        <v>null</v>
+        <v>som</v>
       </c>
       <c r="Q45" t="str">
-        <v>null</v>
+        <v>0</v>
       </c>
       <c r="R45" t="str">
-        <v>true</v>
+        <v>null</v>
       </c>
       <c r="S45" t="str">
-        <v>minimum</v>
+        <v>null</v>
       </c>
       <c r="T45" t="str">
         <v>null</v>
@@ -4139,34 +4139,34 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/12</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/1</v>
       </c>
       <c r="B46" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C46" t="str">
-        <v>http://qudt.org/vocab/unit/M3-PER-HR</v>
+        <v>null</v>
       </c>
       <c r="D46" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E46" t="str">
-        <v>null</v>
+        <v>Zuurtegraad waswater S1 systeem</v>
       </c>
       <c r="F46" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H46" t="str">
-        <v>Waswaterdebiet bevloeiing S3 systeem</v>
+        <v>null</v>
       </c>
       <c r="I46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K46" t="str">
         <v>null</v>
@@ -4178,7 +4178,7 @@
         <v>null</v>
       </c>
       <c r="N46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="O46" t="str">
         <v>null</v>
@@ -4190,10 +4190,10 @@
         <v>null</v>
       </c>
       <c r="R46" t="str">
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="S46" t="str">
-        <v>minimum</v>
+        <v>null</v>
       </c>
       <c r="T46" t="str">
         <v>null</v>
@@ -4222,34 +4222,34 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/13</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/10</v>
       </c>
       <c r="B47" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C47" t="str">
-        <v>http://qudt.org/vocab/unit/M3</v>
+        <v>null</v>
       </c>
       <c r="D47" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E47" t="str">
-        <v>null</v>
+        <v>Drukval S2 systeem</v>
       </c>
       <c r="F47" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H47" t="str">
-        <v>Biobedspuiwaterproductie S3 systeem</v>
+        <v>null</v>
       </c>
       <c r="I47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K47" t="str">
         <v>null</v>
@@ -4261,7 +4261,7 @@
         <v>null</v>
       </c>
       <c r="N47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="O47" t="str">
         <v>null</v>
@@ -4276,7 +4276,7 @@
         <v>true</v>
       </c>
       <c r="S47" t="str">
-        <v>minimum</v>
+        <v>exact</v>
       </c>
       <c r="T47" t="str">
         <v>null</v>
@@ -4305,31 +4305,31 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/14</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/11</v>
       </c>
       <c r="B48" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C48" t="str">
-        <v>http://qudt.org/vocab/unit/M3</v>
+        <v>null</v>
       </c>
       <c r="D48" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E48" t="str">
-        <v>null</v>
+        <v>Waswaterdebiet voorbevochtiging S3 systeem</v>
       </c>
       <c r="F48" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G48" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H48" t="str">
-        <v>Biobedspoelwaterproductie S3 systeem</v>
+        <v>null</v>
       </c>
       <c r="I48" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J48" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
@@ -4344,7 +4344,7 @@
         <v>null</v>
       </c>
       <c r="N48" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
       </c>
       <c r="O48" t="str">
         <v>null</v>
@@ -4388,31 +4388,31 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/15</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/12</v>
       </c>
       <c r="B49" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C49" t="str">
-        <v>http://qudt.org/vocab/unit/PA</v>
+        <v>null</v>
       </c>
       <c r="D49" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E49" t="str">
-        <v>null</v>
+        <v>Waswaterdebiet bevloeiing S3 systeem</v>
       </c>
       <c r="F49" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G49" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H49" t="str">
-        <v>Drukval S3 systeem</v>
+        <v>null</v>
       </c>
       <c r="I49" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J49" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
@@ -4427,7 +4427,7 @@
         <v>null</v>
       </c>
       <c r="N49" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing</v>
       </c>
       <c r="O49" t="str">
         <v>null</v>
@@ -4442,7 +4442,7 @@
         <v>true</v>
       </c>
       <c r="S49" t="str">
-        <v>maximum</v>
+        <v>minimum</v>
       </c>
       <c r="T49" t="str">
         <v>null</v>
@@ -4471,34 +4471,34 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/13</v>
       </c>
       <c r="B50" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C50" t="str">
-        <v>http://qudt.org/vocab/unit/MilliS-PER-CentiM</v>
+        <v>null</v>
       </c>
       <c r="D50" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E50" t="str">
-        <v>null</v>
+        <v>Biobedspuiwaterproductie S3 systeem</v>
       </c>
       <c r="F50" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H50" t="str">
-        <v>Geleidbaarheid waswater S1 systeem</v>
+        <v>null</v>
       </c>
       <c r="I50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K50" t="str">
         <v>null</v>
@@ -4510,7 +4510,7 @@
         <v>null</v>
       </c>
       <c r="N50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie</v>
       </c>
       <c r="O50" t="str">
         <v>null</v>
@@ -4525,7 +4525,7 @@
         <v>true</v>
       </c>
       <c r="S50" t="str">
-        <v>maximum</v>
+        <v>minimum</v>
       </c>
       <c r="T50" t="str">
         <v>null</v>
@@ -4554,34 +4554,34 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/14</v>
       </c>
       <c r="B51" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C51" t="str">
-        <v>http://qudt.org/vocab/unit/M3-PER-HR</v>
+        <v>null</v>
       </c>
       <c r="D51" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E51" t="str">
-        <v>null</v>
+        <v>Biobedspoelwaterproductie S3 systeem</v>
       </c>
       <c r="F51" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H51" t="str">
-        <v>Waswaterdebiet S1 systeem</v>
+        <v>null</v>
       </c>
       <c r="I51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K51" t="str">
         <v>null</v>
@@ -4593,7 +4593,7 @@
         <v>null</v>
       </c>
       <c r="N51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie</v>
       </c>
       <c r="O51" t="str">
         <v>null</v>
@@ -4637,34 +4637,34 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/4</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/15</v>
       </c>
       <c r="B52" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C52" t="str">
-        <v>http://qudt.org/vocab/unit/M3</v>
+        <v>null</v>
       </c>
       <c r="D52" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E52" t="str">
-        <v>null</v>
+        <v>Drukval S3 systeem</v>
       </c>
       <c r="F52" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H52" t="str">
-        <v>Spuiwaterdebiet S1 systeem</v>
+        <v>null</v>
       </c>
       <c r="I52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K52" t="str">
         <v>null</v>
@@ -4676,7 +4676,7 @@
         <v>null</v>
       </c>
       <c r="N52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="O52" t="str">
         <v>null</v>
@@ -4691,7 +4691,7 @@
         <v>true</v>
       </c>
       <c r="S52" t="str">
-        <v>minimum</v>
+        <v>maximum</v>
       </c>
       <c r="T52" t="str">
         <v>null</v>
@@ -4720,31 +4720,31 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/5</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/2</v>
       </c>
       <c r="B53" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C53" t="str">
-        <v>http://qudt.org/vocab/unit/PA</v>
+        <v>null</v>
       </c>
       <c r="D53" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E53" t="str">
-        <v>null</v>
+        <v>Geleidbaarheid waswater S1 systeem</v>
       </c>
       <c r="F53" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G53" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H53" t="str">
-        <v>Drukval S1 systeem</v>
+        <v>null</v>
       </c>
       <c r="I53" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J53" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
@@ -4759,7 +4759,7 @@
         <v>null</v>
       </c>
       <c r="N53" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="O53" t="str">
         <v>null</v>
@@ -4774,7 +4774,7 @@
         <v>true</v>
       </c>
       <c r="S53" t="str">
-        <v>exact</v>
+        <v>maximum</v>
       </c>
       <c r="T53" t="str">
         <v>null</v>
@@ -4803,34 +4803,34 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/6</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/3</v>
       </c>
       <c r="B54" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C54" t="str">
-        <v>http://qudt.org/vocab/unit/PH</v>
+        <v>null</v>
       </c>
       <c r="D54" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E54" t="str">
-        <v>null</v>
+        <v>Waswaterdebiet S1 systeem</v>
       </c>
       <c r="F54" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H54" t="str">
-        <v>Zuurtegraad waswater S2 systeem</v>
+        <v>null</v>
       </c>
       <c r="I54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K54" t="str">
         <v>null</v>
@@ -4842,7 +4842,7 @@
         <v>null</v>
       </c>
       <c r="N54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
       </c>
       <c r="O54" t="str">
         <v>null</v>
@@ -4857,7 +4857,7 @@
         <v>true</v>
       </c>
       <c r="S54" t="str">
-        <v>maximum</v>
+        <v>minimum</v>
       </c>
       <c r="T54" t="str">
         <v>null</v>
@@ -4886,34 +4886,34 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/7</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/4</v>
       </c>
       <c r="B55" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C55" t="str">
-        <v>http://qudt.org/vocab/unit/MilliS-PER-CentiM</v>
+        <v>null</v>
       </c>
       <c r="D55" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E55" t="str">
-        <v>null</v>
+        <v>Spuiwaterdebiet S1 systeem</v>
       </c>
       <c r="F55" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H55" t="str">
-        <v>Geleidbaarheid waswater S2 systeem</v>
+        <v>null</v>
       </c>
       <c r="I55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K55" t="str">
         <v>null</v>
@@ -4925,7 +4925,7 @@
         <v>null</v>
       </c>
       <c r="N55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
       </c>
       <c r="O55" t="str">
         <v>null</v>
@@ -4940,7 +4940,7 @@
         <v>true</v>
       </c>
       <c r="S55" t="str">
-        <v>maximum</v>
+        <v>minimum</v>
       </c>
       <c r="T55" t="str">
         <v>null</v>
@@ -4969,34 +4969,34 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/8</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/5</v>
       </c>
       <c r="B56" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C56" t="str">
-        <v>http://qudt.org/vocab/unit/M3-PER-HR</v>
+        <v>null</v>
       </c>
       <c r="D56" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E56" t="str">
-        <v>null</v>
+        <v>Drukval S1 systeem</v>
       </c>
       <c r="F56" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H56" t="str">
-        <v>Waswaterdebiet S2 systeem</v>
+        <v>null</v>
       </c>
       <c r="I56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K56" t="str">
         <v>null</v>
@@ -5008,7 +5008,7 @@
         <v>null</v>
       </c>
       <c r="N56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="O56" t="str">
         <v>null</v>
@@ -5023,7 +5023,7 @@
         <v>true</v>
       </c>
       <c r="S56" t="str">
-        <v>minimum</v>
+        <v>exact</v>
       </c>
       <c r="T56" t="str">
         <v>null</v>
@@ -5052,31 +5052,31 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/9</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/6</v>
       </c>
       <c r="B57" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C57" t="str">
-        <v>http://qudt.org/vocab/unit/M3</v>
+        <v>null</v>
       </c>
       <c r="D57" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E57" t="str">
-        <v>null</v>
+        <v>Zuurtegraad waswater S2 systeem</v>
       </c>
       <c r="F57" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G57" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="H57" t="str">
-        <v>Spuiwaterdebiet S2 systeem</v>
+        <v>null</v>
       </c>
       <c r="I57" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="J57" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
@@ -5091,7 +5091,7 @@
         <v>null</v>
       </c>
       <c r="N57" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="O57" t="str">
         <v>null</v>
@@ -5106,7 +5106,7 @@
         <v>true</v>
       </c>
       <c r="S57" t="str">
-        <v>minimum</v>
+        <v>maximum</v>
       </c>
       <c r="T57" t="str">
         <v>null</v>
@@ -5135,7 +5135,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/in_gebruik</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/7</v>
       </c>
       <c r="B58" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5144,25 +5144,25 @@
         <v>null</v>
       </c>
       <c r="D58" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E58" t="str">
-        <v>null</v>
+        <v>Geleidbaarheid waswater S2 systeem</v>
       </c>
       <c r="F58" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
+        <v>null</v>
       </c>
       <c r="H58" t="str">
-        <v>Stal in gebruik, dieren aanwezig.</v>
+        <v>null</v>
       </c>
       <c r="I58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
+        <v>null</v>
       </c>
       <c r="J58" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K58" t="str">
         <v>null</v>
@@ -5174,7 +5174,7 @@
         <v>null</v>
       </c>
       <c r="N58" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="O58" t="str">
         <v>null</v>
@@ -5186,10 +5186,10 @@
         <v>null</v>
       </c>
       <c r="R58" t="str">
-        <v>null</v>
+        <v>true</v>
       </c>
       <c r="S58" t="str">
-        <v>null</v>
+        <v>maximum</v>
       </c>
       <c r="T58" t="str">
         <v>null</v>
@@ -5218,7 +5218,7 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/leeg</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/8</v>
       </c>
       <c r="B59" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5227,25 +5227,25 @@
         <v>null</v>
       </c>
       <c r="D59" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E59" t="str">
-        <v>null</v>
+        <v>Waswaterdebiet S2 systeem</v>
       </c>
       <c r="F59" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
+        <v>null</v>
       </c>
       <c r="H59" t="str">
-        <v>Lege stal</v>
+        <v>null</v>
       </c>
       <c r="I59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
+        <v>null</v>
       </c>
       <c r="J59" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K59" t="str">
         <v>null</v>
@@ -5257,7 +5257,7 @@
         <v>null</v>
       </c>
       <c r="N59" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
       </c>
       <c r="O59" t="str">
         <v>null</v>
@@ -5269,10 +5269,10 @@
         <v>null</v>
       </c>
       <c r="R59" t="str">
-        <v>null</v>
+        <v>true</v>
       </c>
       <c r="S59" t="str">
-        <v>null</v>
+        <v>minimum</v>
       </c>
       <c r="T59" t="str">
         <v>null</v>
@@ -5301,7 +5301,7 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/onderhoud</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/9</v>
       </c>
       <c r="B60" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5310,25 +5310,25 @@
         <v>null</v>
       </c>
       <c r="D60" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="E60" t="str">
-        <v>null</v>
+        <v>Spuiwaterdebiet S2 systeem</v>
       </c>
       <c r="F60" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="G60" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+        <v>null</v>
       </c>
       <c r="H60" t="str">
-        <v>In onderhoud</v>
+        <v>null</v>
       </c>
       <c r="I60" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+        <v>null</v>
       </c>
       <c r="J60" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K60" t="str">
         <v>null</v>
@@ -5340,7 +5340,7 @@
         <v>null</v>
       </c>
       <c r="N60" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
       </c>
       <c r="O60" t="str">
         <v>null</v>
@@ -5352,10 +5352,10 @@
         <v>null</v>
       </c>
       <c r="R60" t="str">
-        <v>null</v>
+        <v>true</v>
       </c>
       <c r="S60" t="str">
-        <v>null</v>
+        <v>minimum</v>
       </c>
       <c r="T60" t="str">
         <v>null</v>
@@ -5384,7 +5384,7 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/operationeel</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/in_gebruik</v>
       </c>
       <c r="B61" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5393,22 +5393,22 @@
         <v>null</v>
       </c>
       <c r="D61" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
       </c>
       <c r="E61" t="str">
-        <v>null</v>
+        <v>Stal in gebruik, dieren aanwezig.</v>
       </c>
       <c r="F61" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
       </c>
       <c r="G61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+        <v>null</v>
       </c>
       <c r="H61" t="str">
-        <v>Operationeel</v>
+        <v>null</v>
       </c>
       <c r="I61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+        <v>null</v>
       </c>
       <c r="J61" t="str">
         <v>null</v>
@@ -5467,7 +5467,7 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/storing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/leeg</v>
       </c>
       <c r="B62" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5476,22 +5476,22 @@
         <v>null</v>
       </c>
       <c r="D62" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
       </c>
       <c r="E62" t="str">
-        <v>null</v>
+        <v>Lege stal</v>
       </c>
       <c r="F62" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
       </c>
       <c r="G62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+        <v>null</v>
       </c>
       <c r="H62" t="str">
-        <v>Storing</v>
+        <v>null</v>
       </c>
       <c r="I62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+        <v>null</v>
       </c>
       <c r="J62" t="str">
         <v>null</v>
@@ -5550,7 +5550,7 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/gereinigd</v>
       </c>
       <c r="B63" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5559,19 +5559,19 @@
         <v>null</v>
       </c>
       <c r="D63" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="E63" t="str">
-        <v>null</v>
+        <v>Gereinigd</v>
       </c>
       <c r="F63" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="G63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs</v>
+        <v>null</v>
       </c>
       <c r="H63" t="str">
-        <v>Luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="I63" t="str">
         <v>null</v>
@@ -5607,19 +5607,19 @@
         <v>null</v>
       </c>
       <c r="T63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="U63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="V63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>null</v>
       </c>
       <c r="W63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>null</v>
       </c>
       <c r="X63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="Y63" t="str">
         <v>null</v>
@@ -5633,7 +5633,7 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/onderhoud</v>
       </c>
       <c r="B64" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5642,22 +5642,22 @@
         <v>null</v>
       </c>
       <c r="D64" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="E64" t="str">
-        <v>null</v>
+        <v>In onderhoud</v>
       </c>
       <c r="F64" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="G64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs</v>
+        <v>null</v>
       </c>
       <c r="H64" t="str">
-        <v>Luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="I64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs</v>
+        <v>null</v>
       </c>
       <c r="J64" t="str">
         <v>null</v>
@@ -5696,13 +5696,13 @@
         <v>null</v>
       </c>
       <c r="V64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="W64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="X64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="Y64" t="str">
         <v>null</v>
@@ -5716,7 +5716,7 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/operationeel</v>
       </c>
       <c r="B65" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5725,19 +5725,19 @@
         <v>null</v>
       </c>
       <c r="D65" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="E65" t="str">
-        <v>null</v>
+        <v>Operationeel</v>
       </c>
       <c r="F65" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="G65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs</v>
+        <v>null</v>
       </c>
       <c r="H65" t="str">
-        <v>Biologisch luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="I65" t="str">
         <v>null</v>
@@ -5773,10 +5773,10 @@
         <v>null</v>
       </c>
       <c r="T65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="U65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="V65" t="str">
         <v>null</v>
@@ -5785,10 +5785,10 @@
         <v>null</v>
       </c>
       <c r="X65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="Y65" t="str">
-        <v>S1</v>
+        <v>null</v>
       </c>
       <c r="Z65" t="str">
         <v>null</v>
@@ -5799,7 +5799,7 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/storing</v>
       </c>
       <c r="B66" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5808,19 +5808,19 @@
         <v>null</v>
       </c>
       <c r="D66" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="E66" t="str">
-        <v>null</v>
+        <v>Storing</v>
       </c>
       <c r="F66" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="G66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs</v>
+        <v>null</v>
       </c>
       <c r="H66" t="str">
-        <v>Chemisch luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="I66" t="str">
         <v>null</v>
@@ -5856,10 +5856,10 @@
         <v>null</v>
       </c>
       <c r="T66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="U66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="V66" t="str">
         <v>null</v>
@@ -5868,10 +5868,10 @@
         <v>null</v>
       </c>
       <c r="X66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="Y66" t="str">
-        <v>S2</v>
+        <v>null</v>
       </c>
       <c r="Z66" t="str">
         <v>null</v>
@@ -5882,7 +5882,7 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
       </c>
       <c r="B67" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5891,19 +5891,19 @@
         <v>null</v>
       </c>
       <c r="D67" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
       </c>
       <c r="E67" t="str">
-        <v>null</v>
+        <v>Luchtwassysteem</v>
       </c>
       <c r="F67" t="str">
         <v>null</v>
       </c>
       <c r="G67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs</v>
+        <v>null</v>
       </c>
       <c r="H67" t="str">
-        <v>Biobed</v>
+        <v>null</v>
       </c>
       <c r="I67" t="str">
         <v>null</v>
@@ -5945,16 +5945,16 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="V67" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="W67" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="X67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="Y67" t="str">
-        <v>S3</v>
+        <v>null</v>
       </c>
       <c r="Z67" t="str">
         <v>null</v>
@@ -5965,28 +5965,28 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="B68" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C68" t="str">
         <v>null</v>
       </c>
       <c r="D68" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
       </c>
       <c r="E68" t="str">
-        <v>null</v>
+        <v>Luchtzuiveringssysteem</v>
       </c>
       <c r="F68" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
       </c>
       <c r="G68" t="str">
         <v>null</v>
       </c>
       <c r="H68" t="str">
-        <v>conceptschema luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="I68" t="str">
         <v>null</v>
@@ -6028,19 +6028,19 @@
         <v>null</v>
       </c>
       <c r="V68" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
       </c>
       <c r="W68" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
       </c>
       <c r="X68" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
       </c>
       <c r="Y68" t="str">
         <v>null</v>
       </c>
       <c r="Z68" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="AA68" t="str">
         <v>null</v>
@@ -6048,19 +6048,19 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="B69" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C69" t="str">
         <v>null</v>
       </c>
       <c r="D69" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
       </c>
       <c r="E69" t="str">
-        <v>null</v>
+        <v>Biologisch luchtwassysteem</v>
       </c>
       <c r="F69" t="str">
         <v>null</v>
@@ -6069,7 +6069,7 @@
         <v>null</v>
       </c>
       <c r="H69" t="str">
-        <v>conceptschema luchtzuiveringssysteem parameter specificatie</v>
+        <v>null</v>
       </c>
       <c r="I69" t="str">
         <v>null</v>
@@ -6087,7 +6087,7 @@
         <v>null</v>
       </c>
       <c r="N69" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="O69" t="str">
         <v>null</v>
@@ -6105,10 +6105,10 @@
         <v>null</v>
       </c>
       <c r="T69" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
       </c>
       <c r="U69" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="V69" t="str">
         <v>null</v>
@@ -6117,13 +6117,13 @@
         <v>null</v>
       </c>
       <c r="X69" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="Y69" t="str">
-        <v>null</v>
+        <v>S1</v>
       </c>
       <c r="Z69" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/10|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/11|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/12|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/13|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/14|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/15|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/4|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/5|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/6|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/7|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/8|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/9</v>
+        <v>null</v>
       </c>
       <c r="AA69" t="str">
         <v>null</v>
@@ -6131,19 +6131,19 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="B70" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C70" t="str">
         <v>null</v>
       </c>
       <c r="D70" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
       </c>
       <c r="E70" t="str">
-        <v>null</v>
+        <v>Chemisch luchtwassysteem</v>
       </c>
       <c r="F70" t="str">
         <v>null</v>
@@ -6152,7 +6152,7 @@
         <v>null</v>
       </c>
       <c r="H70" t="str">
-        <v>conceptschema luchtzuiveringssysteem medium</v>
+        <v>null</v>
       </c>
       <c r="I70" t="str">
         <v>null</v>
@@ -6170,7 +6170,7 @@
         <v>null</v>
       </c>
       <c r="N70" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="O70" t="str">
         <v>null</v>
@@ -6188,10 +6188,10 @@
         <v>null</v>
       </c>
       <c r="T70" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
       </c>
       <c r="U70" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="V70" t="str">
         <v>null</v>
@@ -6200,13 +6200,13 @@
         <v>null</v>
       </c>
       <c r="X70" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="Y70" t="str">
-        <v>null</v>
+        <v>S2</v>
       </c>
       <c r="Z70" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/lucht|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/stal|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/hetelektronischmonitoringssysteem</v>
+        <v>null</v>
       </c>
       <c r="AA70" t="str">
         <v>null</v>
@@ -6214,19 +6214,19 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="B71" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C71" t="str">
         <v>null</v>
       </c>
       <c r="D71" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
       </c>
       <c r="E71" t="str">
-        <v>null</v>
+        <v>Biobed</v>
       </c>
       <c r="F71" t="str">
         <v>null</v>
@@ -6235,7 +6235,7 @@
         <v>null</v>
       </c>
       <c r="H71" t="str">
-        <v>conceptschema luchtzuiveringssysteem eigenschap</v>
+        <v>null</v>
       </c>
       <c r="I71" t="str">
         <v>null</v>
@@ -6253,7 +6253,7 @@
         <v>null</v>
       </c>
       <c r="N71" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
       </c>
       <c r="O71" t="str">
         <v>null</v>
@@ -6271,10 +6271,10 @@
         <v>null</v>
       </c>
       <c r="T71" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="U71" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="V71" t="str">
         <v>null</v>
@@ -6283,13 +6283,13 @@
         <v>null</v>
       </c>
       <c r="X71" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="Y71" t="str">
-        <v>null</v>
+        <v>S3</v>
       </c>
       <c r="Z71" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>null</v>
       </c>
       <c r="AA71" t="str">
         <v>null</v>
@@ -6297,7 +6297,7 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/bedrijfsklasse</v>
       </c>
       <c r="B72" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6309,7 +6309,7 @@
         <v>null</v>
       </c>
       <c r="E72" t="str">
-        <v>null</v>
+        <v>conceptschema iioa bedrijfsklassen</v>
       </c>
       <c r="F72" t="str">
         <v>null</v>
@@ -6318,7 +6318,7 @@
         <v>null</v>
       </c>
       <c r="H72" t="str">
-        <v>conceptschema luchtzuiveringssysteem status</v>
+        <v>null</v>
       </c>
       <c r="I72" t="str">
         <v>null</v>
@@ -6372,7 +6372,7 @@
         <v>null</v>
       </c>
       <c r="Z72" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/onderhoud|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/operationeel|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/storing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/bedrijfklasse/1|https://data.omgeving.vlaanderen.be/id/concept/bedrijfklasse/2|https://data.omgeving.vlaanderen.be/id/concept/bedrijfklasse/3</v>
       </c>
       <c r="AA72" t="str">
         <v>null</v>
@@ -6380,7 +6380,7 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="B73" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6392,7 +6392,7 @@
         <v>null</v>
       </c>
       <c r="E73" t="str">
-        <v>null</v>
+        <v>conceptschema luchtzuiveringssysteem parameter specificatie</v>
       </c>
       <c r="F73" t="str">
         <v>null</v>
@@ -6401,7 +6401,7 @@
         <v>null</v>
       </c>
       <c r="H73" t="str">
-        <v>conceptschema luchtzuiveringssysteem stalbezetting</v>
+        <v>null</v>
       </c>
       <c r="I73" t="str">
         <v>null</v>
@@ -6455,7 +6455,7 @@
         <v>null</v>
       </c>
       <c r="Z73" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/in_gebruik|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/leeg</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/10|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/11|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/12|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/13|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/14|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/15|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/4|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/5|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/6|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/7|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/8|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/9</v>
       </c>
       <c r="AA73" t="str">
         <v>null</v>
@@ -6463,7 +6463,7 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="B74" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6475,7 +6475,7 @@
         <v>null</v>
       </c>
       <c r="E74" t="str">
-        <v>null</v>
+        <v>conceptschema luchtzuiveringssysteem medium</v>
       </c>
       <c r="F74" t="str">
         <v>null</v>
@@ -6484,69 +6484,484 @@
         <v>null</v>
       </c>
       <c r="H74" t="str">
+        <v>null</v>
+      </c>
+      <c r="I74" t="str">
+        <v>null</v>
+      </c>
+      <c r="J74" t="str">
+        <v>null</v>
+      </c>
+      <c r="K74" t="str">
+        <v>null</v>
+      </c>
+      <c r="L74" t="str">
+        <v>null</v>
+      </c>
+      <c r="M74" t="str">
+        <v>null</v>
+      </c>
+      <c r="N74" t="str">
+        <v>null</v>
+      </c>
+      <c r="O74" t="str">
+        <v>null</v>
+      </c>
+      <c r="P74" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q74" t="str">
+        <v>null</v>
+      </c>
+      <c r="R74" t="str">
+        <v>null</v>
+      </c>
+      <c r="S74" t="str">
+        <v>null</v>
+      </c>
+      <c r="T74" t="str">
+        <v>null</v>
+      </c>
+      <c r="U74" t="str">
+        <v>null</v>
+      </c>
+      <c r="V74" t="str">
+        <v>null</v>
+      </c>
+      <c r="W74" t="str">
+        <v>null</v>
+      </c>
+      <c r="X74" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y74" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z74" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/lucht|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/stal|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/hetelektronischmonitoringssysteem</v>
+      </c>
+      <c r="AA74" t="str">
+        <v>null</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+      </c>
+      <c r="B75" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+      </c>
+      <c r="C75" t="str">
+        <v>null</v>
+      </c>
+      <c r="D75" t="str">
+        <v>null</v>
+      </c>
+      <c r="E75" t="str">
+        <v>conceptschema luchtzuiveringssysteem eigenschap</v>
+      </c>
+      <c r="F75" t="str">
+        <v>null</v>
+      </c>
+      <c r="G75" t="str">
+        <v>null</v>
+      </c>
+      <c r="H75" t="str">
+        <v>null</v>
+      </c>
+      <c r="I75" t="str">
+        <v>null</v>
+      </c>
+      <c r="J75" t="str">
+        <v>null</v>
+      </c>
+      <c r="K75" t="str">
+        <v>null</v>
+      </c>
+      <c r="L75" t="str">
+        <v>null</v>
+      </c>
+      <c r="M75" t="str">
+        <v>null</v>
+      </c>
+      <c r="N75" t="str">
+        <v>null</v>
+      </c>
+      <c r="O75" t="str">
+        <v>null</v>
+      </c>
+      <c r="P75" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q75" t="str">
+        <v>null</v>
+      </c>
+      <c r="R75" t="str">
+        <v>null</v>
+      </c>
+      <c r="S75" t="str">
+        <v>null</v>
+      </c>
+      <c r="T75" t="str">
+        <v>null</v>
+      </c>
+      <c r="U75" t="str">
+        <v>null</v>
+      </c>
+      <c r="V75" t="str">
+        <v>null</v>
+      </c>
+      <c r="W75" t="str">
+        <v>null</v>
+      </c>
+      <c r="X75" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y75" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z75" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+      </c>
+      <c r="AA75" t="str">
+        <v>null</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+      </c>
+      <c r="B76" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+      </c>
+      <c r="C76" t="str">
+        <v>null</v>
+      </c>
+      <c r="D76" t="str">
+        <v>null</v>
+      </c>
+      <c r="E76" t="str">
+        <v>conceptschema luchtzuiveringssysteem status</v>
+      </c>
+      <c r="F76" t="str">
+        <v>null</v>
+      </c>
+      <c r="G76" t="str">
+        <v>null</v>
+      </c>
+      <c r="H76" t="str">
+        <v>null</v>
+      </c>
+      <c r="I76" t="str">
+        <v>null</v>
+      </c>
+      <c r="J76" t="str">
+        <v>null</v>
+      </c>
+      <c r="K76" t="str">
+        <v>null</v>
+      </c>
+      <c r="L76" t="str">
+        <v>null</v>
+      </c>
+      <c r="M76" t="str">
+        <v>null</v>
+      </c>
+      <c r="N76" t="str">
+        <v>null</v>
+      </c>
+      <c r="O76" t="str">
+        <v>null</v>
+      </c>
+      <c r="P76" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q76" t="str">
+        <v>null</v>
+      </c>
+      <c r="R76" t="str">
+        <v>null</v>
+      </c>
+      <c r="S76" t="str">
+        <v>null</v>
+      </c>
+      <c r="T76" t="str">
+        <v>null</v>
+      </c>
+      <c r="U76" t="str">
+        <v>null</v>
+      </c>
+      <c r="V76" t="str">
+        <v>null</v>
+      </c>
+      <c r="W76" t="str">
+        <v>null</v>
+      </c>
+      <c r="X76" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y76" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z76" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/gereinigd|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/onderhoud|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/operationeel|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/storing</v>
+      </c>
+      <c r="AA76" t="str">
+        <v>null</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
+      </c>
+      <c r="B77" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+      </c>
+      <c r="C77" t="str">
+        <v>null</v>
+      </c>
+      <c r="D77" t="str">
+        <v>null</v>
+      </c>
+      <c r="E77" t="str">
+        <v>conceptschema luchtzuiveringssysteem stalbezetting</v>
+      </c>
+      <c r="F77" t="str">
+        <v>null</v>
+      </c>
+      <c r="G77" t="str">
+        <v>null</v>
+      </c>
+      <c r="H77" t="str">
+        <v>null</v>
+      </c>
+      <c r="I77" t="str">
+        <v>null</v>
+      </c>
+      <c r="J77" t="str">
+        <v>null</v>
+      </c>
+      <c r="K77" t="str">
+        <v>null</v>
+      </c>
+      <c r="L77" t="str">
+        <v>null</v>
+      </c>
+      <c r="M77" t="str">
+        <v>null</v>
+      </c>
+      <c r="N77" t="str">
+        <v>null</v>
+      </c>
+      <c r="O77" t="str">
+        <v>null</v>
+      </c>
+      <c r="P77" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q77" t="str">
+        <v>null</v>
+      </c>
+      <c r="R77" t="str">
+        <v>null</v>
+      </c>
+      <c r="S77" t="str">
+        <v>null</v>
+      </c>
+      <c r="T77" t="str">
+        <v>null</v>
+      </c>
+      <c r="U77" t="str">
+        <v>null</v>
+      </c>
+      <c r="V77" t="str">
+        <v>null</v>
+      </c>
+      <c r="W77" t="str">
+        <v>null</v>
+      </c>
+      <c r="X77" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y77" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z77" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/in_gebruik|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/leeg</v>
+      </c>
+      <c r="AA77" t="str">
+        <v>null</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
+      </c>
+      <c r="B78" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+      </c>
+      <c r="C78" t="str">
+        <v>null</v>
+      </c>
+      <c r="D78" t="str">
+        <v>null</v>
+      </c>
+      <c r="E78" t="str">
+        <v>conceptschema luchtzuiveringssysteem</v>
+      </c>
+      <c r="F78" t="str">
+        <v>null</v>
+      </c>
+      <c r="G78" t="str">
+        <v>null</v>
+      </c>
+      <c r="H78" t="str">
+        <v>null</v>
+      </c>
+      <c r="I78" t="str">
+        <v>null</v>
+      </c>
+      <c r="J78" t="str">
+        <v>null</v>
+      </c>
+      <c r="K78" t="str">
+        <v>null</v>
+      </c>
+      <c r="L78" t="str">
+        <v>null</v>
+      </c>
+      <c r="M78" t="str">
+        <v>null</v>
+      </c>
+      <c r="N78" t="str">
+        <v>null</v>
+      </c>
+      <c r="O78" t="str">
+        <v>null</v>
+      </c>
+      <c r="P78" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q78" t="str">
+        <v>null</v>
+      </c>
+      <c r="R78" t="str">
+        <v>null</v>
+      </c>
+      <c r="S78" t="str">
+        <v>null</v>
+      </c>
+      <c r="T78" t="str">
+        <v>null</v>
+      </c>
+      <c r="U78" t="str">
+        <v>null</v>
+      </c>
+      <c r="V78" t="str">
+        <v>null</v>
+      </c>
+      <c r="W78" t="str">
+        <v>null</v>
+      </c>
+      <c r="X78" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y78" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z78" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+      </c>
+      <c r="AA78" t="str">
+        <v>null</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+      </c>
+      <c r="B79" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+      </c>
+      <c r="C79" t="str">
+        <v>null</v>
+      </c>
+      <c r="D79" t="str">
+        <v>null</v>
+      </c>
+      <c r="E79" t="str">
         <v>conceptschema luchtzuiveringssysteem normbandbreedte</v>
       </c>
-      <c r="I74" t="str">
-        <v>null</v>
-      </c>
-      <c r="J74" t="str">
-        <v>null</v>
-      </c>
-      <c r="K74" t="str">
-        <v>null</v>
-      </c>
-      <c r="L74" t="str">
-        <v>null</v>
-      </c>
-      <c r="M74" t="str">
-        <v>null</v>
-      </c>
-      <c r="N74" t="str">
-        <v>null</v>
-      </c>
-      <c r="O74" t="str">
-        <v>null</v>
-      </c>
-      <c r="P74" t="str">
-        <v>null</v>
-      </c>
-      <c r="Q74" t="str">
-        <v>null</v>
-      </c>
-      <c r="R74" t="str">
-        <v>null</v>
-      </c>
-      <c r="S74" t="str">
-        <v>null</v>
-      </c>
-      <c r="T74" t="str">
-        <v>null</v>
-      </c>
-      <c r="U74" t="str">
-        <v>null</v>
-      </c>
-      <c r="V74" t="str">
-        <v>null</v>
-      </c>
-      <c r="W74" t="str">
-        <v>null</v>
-      </c>
-      <c r="X74" t="str">
-        <v>null</v>
-      </c>
-      <c r="Y74" t="str">
-        <v>null</v>
-      </c>
-      <c r="Z74" t="str">
+      <c r="F79" t="str">
+        <v>null</v>
+      </c>
+      <c r="G79" t="str">
+        <v>null</v>
+      </c>
+      <c r="H79" t="str">
+        <v>null</v>
+      </c>
+      <c r="I79" t="str">
+        <v>null</v>
+      </c>
+      <c r="J79" t="str">
+        <v>null</v>
+      </c>
+      <c r="K79" t="str">
+        <v>null</v>
+      </c>
+      <c r="L79" t="str">
+        <v>null</v>
+      </c>
+      <c r="M79" t="str">
+        <v>null</v>
+      </c>
+      <c r="N79" t="str">
+        <v>null</v>
+      </c>
+      <c r="O79" t="str">
+        <v>null</v>
+      </c>
+      <c r="P79" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q79" t="str">
+        <v>null</v>
+      </c>
+      <c r="R79" t="str">
+        <v>null</v>
+      </c>
+      <c r="S79" t="str">
+        <v>null</v>
+      </c>
+      <c r="T79" t="str">
+        <v>null</v>
+      </c>
+      <c r="U79" t="str">
+        <v>null</v>
+      </c>
+      <c r="V79" t="str">
+        <v>null</v>
+      </c>
+      <c r="W79" t="str">
+        <v>null</v>
+      </c>
+      <c r="X79" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y79" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z79" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/10|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/11|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/12|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/13|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/14|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/15|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/16|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/4|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/5|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/6|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/7|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/8|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/9</v>
       </c>
-      <c r="AA74" t="str">
+      <c r="AA79" t="str">
         <v>Ranges</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AA74"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AA79"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
uri's conceptscheme en concepten vlarem klasse aangepast uri's param normen aangepast
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/luchtzuiveringssysteem/luchtzuiveringssysteem.xlsx
+++ b/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/luchtzuiveringssysteem/luchtzuiveringssysteem.xlsx
@@ -413,22 +413,22 @@
         <v>applicableUnit</v>
       </c>
       <c r="D1" t="str">
+        <v>subject</v>
+      </c>
+      <c r="E1" t="str">
+        <v>relevantQuantityKind</v>
+      </c>
+      <c r="F1" t="str">
+        <v>seeAlso</v>
+      </c>
+      <c r="G1" t="str">
         <v>inScheme</v>
       </c>
-      <c r="E1" t="str">
+      <c r="H1" t="str">
         <v>prefLabel</v>
       </c>
-      <c r="F1" t="str">
+      <c r="I1" t="str">
         <v>topConceptOf</v>
-      </c>
-      <c r="G1" t="str">
-        <v>subject</v>
-      </c>
-      <c r="H1" t="str">
-        <v>relevantQuantityKind</v>
-      </c>
-      <c r="I1" t="str">
-        <v>seeAlso</v>
       </c>
       <c r="J1" t="str">
         <v>relevantLZS</v>
@@ -479,10 +479,10 @@
         <v>notation</v>
       </c>
       <c r="Z1" t="str">
+        <v>altLabel</v>
+      </c>
+      <c r="AA1" t="str">
         <v>hasTopConcept</v>
-      </c>
-      <c r="AA1" t="str">
-        <v>altLabel</v>
       </c>
     </row>
     <row r="2">
@@ -1234,34 +1234,34 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/bedrijfklasse/1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie</v>
       </c>
       <c r="B11" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
       </c>
       <c r="C11" t="str">
         <v>null</v>
       </c>
       <c r="D11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/bedrijfsklasse</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
       </c>
       <c r="E11" t="str">
-        <v>Klasse 1</v>
+        <v>http://qudt.org/vocab/quantitykind/Volume</v>
       </c>
       <c r="F11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/bedrijfsklasse</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
       </c>
       <c r="G11" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="H11" t="str">
-        <v>null</v>
+        <v>Biobedspoelwaterproductie</v>
       </c>
       <c r="I11" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="J11" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K11" t="str">
         <v>null</v>
@@ -1317,34 +1317,34 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/bedrijfklasse/2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie</v>
       </c>
       <c r="B12" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
       </c>
       <c r="C12" t="str">
         <v>null</v>
       </c>
       <c r="D12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/bedrijfsklasse</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater</v>
       </c>
       <c r="E12" t="str">
-        <v>Klasse 2</v>
+        <v>http://qudt.org/vocab/quantitykind/Volume</v>
       </c>
       <c r="F12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/bedrijfsklasse</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0050</v>
       </c>
       <c r="G12" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="H12" t="str">
-        <v>null</v>
+        <v>Biobedspuiwaterproductie</v>
       </c>
       <c r="I12" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="J12" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K12" t="str">
         <v>null</v>
@@ -1400,34 +1400,34 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/bedrijfklasse/3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="B13" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
       </c>
       <c r="C13" t="str">
         <v>null</v>
       </c>
       <c r="D13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/bedrijfsklasse</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/lucht</v>
       </c>
       <c r="E13" t="str">
-        <v>Klasse 3</v>
+        <v>http://qudt.org/vocab/quantitykind/Fugacity|http://qudt.org/vocab/quantitykind/VaporPressure</v>
       </c>
       <c r="F13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/bedrijfsklasse</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0329</v>
       </c>
       <c r="G13" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="H13" t="str">
-        <v>null</v>
+        <v>Drukval over het systeem</v>
       </c>
       <c r="I13" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="J13" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K13" t="str">
         <v>null</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="B14" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -1492,25 +1492,25 @@
         <v>null</v>
       </c>
       <c r="D14" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
+      </c>
+      <c r="E14" t="str">
+        <v>http://qudt.org/vocab/quantitykind/Conductivity</v>
+      </c>
+      <c r="F14" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0010</v>
+      </c>
+      <c r="G14" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
-      <c r="E14" t="str">
-        <v>Biobedspoelwaterproductie</v>
-      </c>
-      <c r="F14" t="str">
+      <c r="H14" t="str">
+        <v>Geleidbaarheid van het waswater</v>
+      </c>
+      <c r="I14" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
-      <c r="G14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
-      </c>
-      <c r="H14" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Volume</v>
-      </c>
-      <c r="I14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
-      </c>
       <c r="J14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K14" t="str">
         <v>null</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
       </c>
       <c r="B15" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -1575,25 +1575,25 @@
         <v>null</v>
       </c>
       <c r="D15" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater</v>
+      </c>
+      <c r="E15" t="str">
+        <v>http://qudt.org/vocab/quantitykind/Volume</v>
+      </c>
+      <c r="F15" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0050</v>
+      </c>
+      <c r="G15" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
-      <c r="E15" t="str">
-        <v>Biobedspuiwaterproductie</v>
-      </c>
-      <c r="F15" t="str">
+      <c r="H15" t="str">
+        <v>Spuiwaterproductie</v>
+      </c>
+      <c r="I15" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
-      <c r="G15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater</v>
-      </c>
-      <c r="H15" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Volume</v>
-      </c>
-      <c r="I15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0050</v>
-      </c>
       <c r="J15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K15" t="str">
         <v>null</v>
@@ -1649,7 +1649,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting</v>
       </c>
       <c r="B16" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -1658,22 +1658,22 @@
         <v>null</v>
       </c>
       <c r="D16" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/stal</v>
+      </c>
+      <c r="E16" t="str">
+        <v>null</v>
+      </c>
+      <c r="F16" t="str">
+        <v>null</v>
+      </c>
+      <c r="G16" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
-      <c r="E16" t="str">
-        <v>Drukval over het systeem</v>
-      </c>
-      <c r="F16" t="str">
+      <c r="H16" t="str">
+        <v>Stalbezetting</v>
+      </c>
+      <c r="I16" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
-      </c>
-      <c r="G16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/lucht</v>
-      </c>
-      <c r="H16" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Fugacity|http://qudt.org/vocab/quantitykind/VaporPressure</v>
-      </c>
-      <c r="I16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0329</v>
       </c>
       <c r="J16" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
@@ -1732,7 +1732,7 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus</v>
       </c>
       <c r="B17" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -1741,25 +1741,25 @@
         <v>null</v>
       </c>
       <c r="D17" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/hetelektronischmonitoringssysteem</v>
+      </c>
+      <c r="E17" t="str">
+        <v>null</v>
+      </c>
+      <c r="F17" t="str">
+        <v>null</v>
+      </c>
+      <c r="G17" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
-      <c r="E17" t="str">
-        <v>Geleidbaarheid van het waswater</v>
-      </c>
-      <c r="F17" t="str">
+      <c r="H17" t="str">
+        <v>SysteemStatus</v>
+      </c>
+      <c r="I17" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
-      <c r="G17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
-      </c>
-      <c r="H17" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Conductivity</v>
-      </c>
-      <c r="I17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0010</v>
-      </c>
       <c r="J17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K17" t="str">
         <v>null</v>
@@ -1815,7 +1815,7 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
       </c>
       <c r="B18" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -1824,22 +1824,22 @@
         <v>null</v>
       </c>
       <c r="D18" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
+      </c>
+      <c r="E18" t="str">
+        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate|http://qudt.org/vocab/quantitykind/VolumePerTime</v>
+      </c>
+      <c r="F18" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
+      </c>
+      <c r="G18" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
-      <c r="E18" t="str">
-        <v>Spuiwaterproductie</v>
-      </c>
-      <c r="F18" t="str">
+      <c r="H18" t="str">
+        <v>Waswaterdebiet over het waspakket</v>
+      </c>
+      <c r="I18" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
-      </c>
-      <c r="G18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater</v>
-      </c>
-      <c r="H18" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Volume</v>
-      </c>
-      <c r="I18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0050</v>
       </c>
       <c r="J18" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
@@ -1898,7 +1898,7 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing</v>
       </c>
       <c r="B19" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -1907,25 +1907,25 @@
         <v>null</v>
       </c>
       <c r="D19" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
+      </c>
+      <c r="E19" t="str">
+        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate|http://qudt.org/vocab/quantitykind/VolumePerTime</v>
+      </c>
+      <c r="F19" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
+      </c>
+      <c r="G19" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
-      <c r="E19" t="str">
-        <v>Stalbezetting</v>
-      </c>
-      <c r="F19" t="str">
+      <c r="H19" t="str">
+        <v>Waswaterdebiet van de bevloeiing van het vulmateriaal</v>
+      </c>
+      <c r="I19" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
-      <c r="G19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/stal</v>
-      </c>
-      <c r="H19" t="str">
-        <v>null</v>
-      </c>
-      <c r="I19" t="str">
-        <v>null</v>
-      </c>
       <c r="J19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K19" t="str">
         <v>null</v>
@@ -1981,7 +1981,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
       </c>
       <c r="B20" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -1990,25 +1990,25 @@
         <v>null</v>
       </c>
       <c r="D20" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
+      </c>
+      <c r="E20" t="str">
+        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate|http://qudt.org/vocab/quantitykind/VolumePerTime</v>
+      </c>
+      <c r="F20" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
+      </c>
+      <c r="G20" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
-      <c r="E20" t="str">
-        <v>SysteemStatus</v>
-      </c>
-      <c r="F20" t="str">
+      <c r="H20" t="str">
+        <v>Waswaterdebiet van de voorbevochtiging van de ingaande stallucht</v>
+      </c>
+      <c r="I20" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
-      <c r="G20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/hetelektronischmonitoringssysteem</v>
-      </c>
-      <c r="H20" t="str">
-        <v>null</v>
-      </c>
-      <c r="I20" t="str">
-        <v>null</v>
-      </c>
       <c r="J20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K20" t="str">
         <v>null</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="B21" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -2073,22 +2073,22 @@
         <v>null</v>
       </c>
       <c r="D21" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
+      </c>
+      <c r="E21" t="str">
+        <v>http://qudt.org/vocab/quantitykind/Acidity|http://qudt.org/vocab/quantitykind/Basicity</v>
+      </c>
+      <c r="F21" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0076</v>
+      </c>
+      <c r="G21" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
-      <c r="E21" t="str">
-        <v>Waswaterdebiet over het waspakket</v>
-      </c>
-      <c r="F21" t="str">
+      <c r="H21" t="str">
+        <v>Zuurtegraad van het waswater</v>
+      </c>
+      <c r="I21" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
-      </c>
-      <c r="G21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
-      </c>
-      <c r="H21" t="str">
-        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate|http://qudt.org/vocab/quantitykind/VolumePerTime</v>
-      </c>
-      <c r="I21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
       </c>
       <c r="J21" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
@@ -2147,34 +2147,34 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/hetelektronischmonitoringssysteem</v>
       </c>
       <c r="B22" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
       </c>
       <c r="C22" t="str">
         <v>null</v>
       </c>
       <c r="D22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>null</v>
       </c>
       <c r="E22" t="str">
-        <v>Waswaterdebiet van de bevloeiing van het vulmateriaal</v>
+        <v>null</v>
       </c>
       <c r="F22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>null</v>
       </c>
       <c r="G22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="H22" t="str">
-        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate|http://qudt.org/vocab/quantitykind/VolumePerTime</v>
+        <v>Het elektronisch monitoringssysteem</v>
       </c>
       <c r="I22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="J22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>null</v>
       </c>
       <c r="K22" t="str">
         <v>null</v>
@@ -2230,34 +2230,34 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/lucht</v>
       </c>
       <c r="B23" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
       </c>
       <c r="C23" t="str">
         <v>null</v>
       </c>
       <c r="D23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>null</v>
       </c>
       <c r="E23" t="str">
-        <v>Waswaterdebiet van de voorbevochtiging van de ingaande stallucht</v>
+        <v>null</v>
       </c>
       <c r="F23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>null</v>
       </c>
       <c r="G23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="H23" t="str">
-        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate|http://qudt.org/vocab/quantitykind/VolumePerTime</v>
+        <v>Lucht</v>
       </c>
       <c r="I23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="J23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>null</v>
       </c>
       <c r="K23" t="str">
         <v>null</v>
@@ -2313,34 +2313,34 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater</v>
       </c>
       <c r="B24" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
       </c>
       <c r="C24" t="str">
         <v>null</v>
       </c>
       <c r="D24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>null</v>
       </c>
       <c r="E24" t="str">
-        <v>Zuurtegraad van het waswater</v>
+        <v>null</v>
       </c>
       <c r="F24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>null</v>
       </c>
       <c r="G24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="H24" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Acidity|http://qudt.org/vocab/quantitykind/Basicity</v>
+        <v>Spuiwater</v>
       </c>
       <c r="I24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0076</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="J24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>null</v>
       </c>
       <c r="K24" t="str">
         <v>null</v>
@@ -2396,7 +2396,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/hetelektronischmonitoringssysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/stal</v>
       </c>
       <c r="B25" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
@@ -2405,22 +2405,22 @@
         <v>null</v>
       </c>
       <c r="D25" t="str">
+        <v>null</v>
+      </c>
+      <c r="E25" t="str">
+        <v>null</v>
+      </c>
+      <c r="F25" t="str">
+        <v>null</v>
+      </c>
+      <c r="G25" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
-      <c r="E25" t="str">
-        <v>Het elektronisch monitoringssysteem</v>
-      </c>
-      <c r="F25" t="str">
+      <c r="H25" t="str">
+        <v>Stal</v>
+      </c>
+      <c r="I25" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
-      </c>
-      <c r="G25" t="str">
-        <v>null</v>
-      </c>
-      <c r="H25" t="str">
-        <v>null</v>
-      </c>
-      <c r="I25" t="str">
-        <v>null</v>
       </c>
       <c r="J25" t="str">
         <v>null</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/lucht</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
       </c>
       <c r="B26" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
@@ -2488,22 +2488,22 @@
         <v>null</v>
       </c>
       <c r="D26" t="str">
+        <v>null</v>
+      </c>
+      <c r="E26" t="str">
+        <v>null</v>
+      </c>
+      <c r="F26" t="str">
+        <v>null</v>
+      </c>
+      <c r="G26" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
-      <c r="E26" t="str">
-        <v>Lucht</v>
-      </c>
-      <c r="F26" t="str">
+      <c r="H26" t="str">
+        <v>Waswater</v>
+      </c>
+      <c r="I26" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
-      </c>
-      <c r="G26" t="str">
-        <v>null</v>
-      </c>
-      <c r="H26" t="str">
-        <v>null</v>
-      </c>
-      <c r="I26" t="str">
-        <v>null</v>
       </c>
       <c r="J26" t="str">
         <v>null</v>
@@ -2562,49 +2562,49 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/1</v>
       </c>
       <c r="B27" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C27" t="str">
         <v>null</v>
       </c>
       <c r="D27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>null</v>
       </c>
       <c r="E27" t="str">
-        <v>Spuiwater</v>
+        <v>null</v>
       </c>
       <c r="F27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>null</v>
       </c>
       <c r="G27" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="H27" t="str">
-        <v>null</v>
+        <v>Zuurtegraad waswater &lt; 6 (S1 systeem)</v>
       </c>
       <c r="I27" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="J27" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K27" t="str">
-        <v>null</v>
+        <v>De zuurtegraad van het waswater is kleiner dan 6</v>
       </c>
       <c r="L27" t="str">
-        <v>null</v>
+        <v>De zuurtegraad van het waswater is kleiner dan 6|&lt; 6</v>
       </c>
       <c r="M27" t="str">
-        <v>null</v>
+        <v>&lt; 6</v>
       </c>
       <c r="N27" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="O27" t="str">
-        <v>null</v>
+        <v>6</v>
       </c>
       <c r="P27" t="str">
         <v>null</v>
@@ -2645,52 +2645,52 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/stal</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/10</v>
       </c>
       <c r="B28" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C28" t="str">
         <v>null</v>
       </c>
       <c r="D28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>null</v>
       </c>
       <c r="E28" t="str">
-        <v>Stal</v>
+        <v>null</v>
       </c>
       <c r="F28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>null</v>
       </c>
       <c r="G28" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="H28" t="str">
-        <v>null</v>
+        <v>Waswaterdebiet afwijking naar beneden &gt; 20% (S2 systeem)</v>
       </c>
       <c r="I28" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="J28" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K28" t="str">
-        <v>null</v>
+        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L28" t="str">
-        <v>null</v>
+        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="M28" t="str">
-        <v>null</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="N28" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
       </c>
       <c r="O28" t="str">
-        <v>null</v>
+        <v>0.8</v>
       </c>
       <c r="P28" t="str">
-        <v>null</v>
+        <v>product</v>
       </c>
       <c r="Q28" t="str">
         <v>null</v>
@@ -2728,52 +2728,52 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/11</v>
       </c>
       <c r="B29" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/2000/01/rdf-schema#Resource</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C29" t="str">
         <v>null</v>
       </c>
       <c r="D29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>null</v>
       </c>
       <c r="E29" t="str">
-        <v>Waswater</v>
+        <v>null</v>
       </c>
       <c r="F29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>null</v>
       </c>
       <c r="G29" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="H29" t="str">
-        <v>null</v>
+        <v>Spuiwaterdebiet afwijking naar beneden &gt; 10% (S2 systeem)</v>
       </c>
       <c r="I29" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="J29" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K29" t="str">
-        <v>null</v>
+        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L29" t="str">
-        <v>null</v>
+        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
       </c>
       <c r="M29" t="str">
-        <v>null</v>
+        <v>&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
       </c>
       <c r="N29" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
       </c>
       <c r="O29" t="str">
-        <v>null</v>
+        <v>0.9</v>
       </c>
       <c r="P29" t="str">
-        <v>null</v>
+        <v>product</v>
       </c>
       <c r="Q29" t="str">
         <v>null</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/12</v>
       </c>
       <c r="B30" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2820,43 +2820,43 @@
         <v>null</v>
       </c>
       <c r="D30" t="str">
+        <v>null</v>
+      </c>
+      <c r="E30" t="str">
+        <v>null</v>
+      </c>
+      <c r="F30" t="str">
+        <v>null</v>
+      </c>
+      <c r="G30" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="E30" t="str">
-        <v>Zuurtegraad waswater &lt; 6 (S1 systeem)</v>
-      </c>
-      <c r="F30" t="str">
+      <c r="H30" t="str">
+        <v>Drukval afwijking naar beneden &gt; 40% (S2 systeem)</v>
+      </c>
+      <c r="I30" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="G30" t="str">
-        <v>null</v>
-      </c>
-      <c r="H30" t="str">
-        <v>null</v>
-      </c>
-      <c r="I30" t="str">
-        <v>null</v>
-      </c>
       <c r="J30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K30" t="str">
-        <v>De zuurtegraad van het waswater is kleiner dan 6</v>
+        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L30" t="str">
-        <v>De zuurtegraad van het waswater is kleiner dan 6|&lt; 6</v>
+        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="M30" t="str">
-        <v>&lt; 6</v>
+        <v>&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="N30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="O30" t="str">
-        <v>6</v>
+        <v>0.6</v>
       </c>
       <c r="P30" t="str">
-        <v>null</v>
+        <v>product</v>
       </c>
       <c r="Q30" t="str">
         <v>null</v>
@@ -2894,7 +2894,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/10</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/13</v>
       </c>
       <c r="B31" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2903,46 +2903,46 @@
         <v>null</v>
       </c>
       <c r="D31" t="str">
+        <v>null</v>
+      </c>
+      <c r="E31" t="str">
+        <v>null</v>
+      </c>
+      <c r="F31" t="str">
+        <v>null</v>
+      </c>
+      <c r="G31" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="E31" t="str">
-        <v>Waswaterdebiet afwijking naar beneden &gt; 20% (S2 systeem)</v>
-      </c>
-      <c r="F31" t="str">
+      <c r="H31" t="str">
+        <v>Drukval afwijking naar boven &gt; 40% (S2 systeem)</v>
+      </c>
+      <c r="I31" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
-      </c>
-      <c r="G31" t="str">
-        <v>null</v>
-      </c>
-      <c r="H31" t="str">
-        <v>null</v>
-      </c>
-      <c r="I31" t="str">
-        <v>null</v>
       </c>
       <c r="J31" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K31" t="str">
-        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L31" t="str">
-        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="M31" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="N31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="O31" t="str">
-        <v>0.8</v>
+        <v>null</v>
       </c>
       <c r="P31" t="str">
         <v>product</v>
       </c>
       <c r="Q31" t="str">
-        <v>null</v>
+        <v>1.4</v>
       </c>
       <c r="R31" t="str">
         <v>null</v>
@@ -2977,7 +2977,7 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/11</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/14</v>
       </c>
       <c r="B32" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2986,40 +2986,40 @@
         <v>null</v>
       </c>
       <c r="D32" t="str">
+        <v>null</v>
+      </c>
+      <c r="E32" t="str">
+        <v>null</v>
+      </c>
+      <c r="F32" t="str">
+        <v>null</v>
+      </c>
+      <c r="G32" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="E32" t="str">
-        <v>Spuiwaterdebiet afwijking naar beneden &gt; 10% (S2 systeem)</v>
-      </c>
-      <c r="F32" t="str">
+      <c r="H32" t="str">
+        <v>Waswaterdebiet voorbevochtiging afwijking naar beneden &gt; 20% (S3 systeem)</v>
+      </c>
+      <c r="I32" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="G32" t="str">
-        <v>null</v>
-      </c>
-      <c r="H32" t="str">
-        <v>null</v>
-      </c>
-      <c r="I32" t="str">
-        <v>null</v>
-      </c>
       <c r="J32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K32" t="str">
-        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het waswaterdebiet van de voorbevochtiging wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L32" t="str">
-        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)|Het waswaterdebiet van de voorbevochtiging wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="M32" t="str">
-        <v>&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="N32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
       </c>
       <c r="O32" t="str">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="P32" t="str">
         <v>product</v>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/12</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/15</v>
       </c>
       <c r="B33" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3069,40 +3069,40 @@
         <v>null</v>
       </c>
       <c r="D33" t="str">
+        <v>null</v>
+      </c>
+      <c r="E33" t="str">
+        <v>null</v>
+      </c>
+      <c r="F33" t="str">
+        <v>null</v>
+      </c>
+      <c r="G33" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="E33" t="str">
-        <v>Drukval afwijking naar beneden &gt; 40% (S2 systeem)</v>
-      </c>
-      <c r="F33" t="str">
+      <c r="H33" t="str">
+        <v>Waswaterdebiet bevloeiing afwijking naar beneden &gt; 20% (S3 systeem)</v>
+      </c>
+      <c r="I33" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="G33" t="str">
-        <v>null</v>
-      </c>
-      <c r="H33" t="str">
-        <v>null</v>
-      </c>
-      <c r="I33" t="str">
-        <v>null</v>
-      </c>
       <c r="J33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K33" t="str">
-        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het waswaterdebiet van de bevloeiing wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L33" t="str">
-        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)|Het waswaterdebiet van de bevloeiing wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="M33" t="str">
-        <v>&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="N33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing</v>
       </c>
       <c r="O33" t="str">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="P33" t="str">
         <v>product</v>
@@ -3143,7 +3143,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/13</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/16</v>
       </c>
       <c r="B34" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3152,34 +3152,34 @@
         <v>null</v>
       </c>
       <c r="D34" t="str">
+        <v>null</v>
+      </c>
+      <c r="E34" t="str">
+        <v>null</v>
+      </c>
+      <c r="F34" t="str">
+        <v>null</v>
+      </c>
+      <c r="G34" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="E34" t="str">
-        <v>Drukval afwijking naar boven &gt; 40% (S2 systeem)</v>
-      </c>
-      <c r="F34" t="str">
+      <c r="H34" t="str">
+        <v>Drukval afwijking naar boven &gt; 50 Pa (S3 systeem)</v>
+      </c>
+      <c r="I34" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="G34" t="str">
-        <v>null</v>
-      </c>
-      <c r="H34" t="str">
-        <v>null</v>
-      </c>
-      <c r="I34" t="str">
-        <v>null</v>
-      </c>
       <c r="J34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K34" t="str">
-        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De drukval wijkt meer dan 50 Pa naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L34" t="str">
-        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>De drukval wijkt meer dan 50 Pa naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 50 Pa + waarde technische fiche (afwijking &gt; 50 Pa)</v>
       </c>
       <c r="M34" t="str">
-        <v>&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>&gt; 50 Pa + waarde technische fiche (afwijking &gt; 50 Pa)</v>
       </c>
       <c r="N34" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
@@ -3188,10 +3188,10 @@
         <v>null</v>
       </c>
       <c r="P34" t="str">
-        <v>product</v>
+        <v>som</v>
       </c>
       <c r="Q34" t="str">
-        <v>1.4</v>
+        <v>50</v>
       </c>
       <c r="R34" t="str">
         <v>null</v>
@@ -3226,7 +3226,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/14</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/2</v>
       </c>
       <c r="B35" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3235,46 +3235,46 @@
         <v>null</v>
       </c>
       <c r="D35" t="str">
+        <v>null</v>
+      </c>
+      <c r="E35" t="str">
+        <v>null</v>
+      </c>
+      <c r="F35" t="str">
+        <v>null</v>
+      </c>
+      <c r="G35" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="E35" t="str">
-        <v>Waswaterdebiet voorbevochtiging afwijking naar beneden &gt; 20% (S3 systeem)</v>
-      </c>
-      <c r="F35" t="str">
+      <c r="H35" t="str">
+        <v>Zuurtegraad waswater &gt; 8,5 (S1 systeem)</v>
+      </c>
+      <c r="I35" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="G35" t="str">
-        <v>null</v>
-      </c>
-      <c r="H35" t="str">
-        <v>null</v>
-      </c>
-      <c r="I35" t="str">
-        <v>null</v>
-      </c>
       <c r="J35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K35" t="str">
-        <v>Het waswaterdebiet van de voorbevochtiging wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De zuurtegraad van het waswater is groter dan 8,5</v>
       </c>
       <c r="L35" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)|Het waswaterdebiet van de voorbevochtiging wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De zuurtegraad van het waswater is groter dan 8,5|&gt; 8,5</v>
       </c>
       <c r="M35" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>&gt; 8,5</v>
       </c>
       <c r="N35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="O35" t="str">
-        <v>0.8</v>
+        <v>null</v>
       </c>
       <c r="P35" t="str">
-        <v>product</v>
+        <v>null</v>
       </c>
       <c r="Q35" t="str">
-        <v>null</v>
+        <v>8.5</v>
       </c>
       <c r="R35" t="str">
         <v>null</v>
@@ -3309,7 +3309,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/15</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/3</v>
       </c>
       <c r="B36" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3318,46 +3318,46 @@
         <v>null</v>
       </c>
       <c r="D36" t="str">
+        <v>null</v>
+      </c>
+      <c r="E36" t="str">
+        <v>null</v>
+      </c>
+      <c r="F36" t="str">
+        <v>null</v>
+      </c>
+      <c r="G36" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="E36" t="str">
-        <v>Waswaterdebiet bevloeiing afwijking naar beneden &gt; 20% (S3 systeem)</v>
-      </c>
-      <c r="F36" t="str">
+      <c r="H36" t="str">
+        <v>Geleidbaarheid waswater &gt; maximale waarde (S1 systeem)</v>
+      </c>
+      <c r="I36" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="G36" t="str">
-        <v>null</v>
-      </c>
-      <c r="H36" t="str">
-        <v>null</v>
-      </c>
-      <c r="I36" t="str">
-        <v>null</v>
-      </c>
       <c r="J36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K36" t="str">
-        <v>Het waswaterdebiet van de bevloeiing wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L36" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)|Het waswaterdebiet van de bevloeiing wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.|&gt; waarde technische fiche</v>
       </c>
       <c r="M36" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>&gt; waarde technische fiche</v>
       </c>
       <c r="N36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="O36" t="str">
-        <v>0.8</v>
+        <v>null</v>
       </c>
       <c r="P36" t="str">
-        <v>product</v>
+        <v>som</v>
       </c>
       <c r="Q36" t="str">
-        <v>null</v>
+        <v>0</v>
       </c>
       <c r="R36" t="str">
         <v>null</v>
@@ -3392,7 +3392,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/16</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/4</v>
       </c>
       <c r="B37" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3401,46 +3401,46 @@
         <v>null</v>
       </c>
       <c r="D37" t="str">
+        <v>null</v>
+      </c>
+      <c r="E37" t="str">
+        <v>null</v>
+      </c>
+      <c r="F37" t="str">
+        <v>null</v>
+      </c>
+      <c r="G37" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="E37" t="str">
-        <v>Drukval afwijking naar boven &gt; 50 Pa (S3 systeem)</v>
-      </c>
-      <c r="F37" t="str">
+      <c r="H37" t="str">
+        <v>Waswaterdebiet afwijking naar beneden &gt; 20% (S1 systeem)</v>
+      </c>
+      <c r="I37" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="G37" t="str">
-        <v>null</v>
-      </c>
-      <c r="H37" t="str">
-        <v>null</v>
-      </c>
-      <c r="I37" t="str">
-        <v>null</v>
-      </c>
       <c r="J37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K37" t="str">
-        <v>De drukval wijkt meer dan 50 Pa naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L37" t="str">
-        <v>De drukval wijkt meer dan 50 Pa naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 50 Pa + waarde technische fiche (afwijking &gt; 50 Pa)</v>
+        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="M37" t="str">
-        <v>&gt; 50 Pa + waarde technische fiche (afwijking &gt; 50 Pa)</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="N37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
       </c>
       <c r="O37" t="str">
-        <v>null</v>
+        <v>0.8</v>
       </c>
       <c r="P37" t="str">
-        <v>som</v>
+        <v>product</v>
       </c>
       <c r="Q37" t="str">
-        <v>50</v>
+        <v>null</v>
       </c>
       <c r="R37" t="str">
         <v>null</v>
@@ -3475,7 +3475,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/5</v>
       </c>
       <c r="B38" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3484,46 +3484,46 @@
         <v>null</v>
       </c>
       <c r="D38" t="str">
+        <v>null</v>
+      </c>
+      <c r="E38" t="str">
+        <v>null</v>
+      </c>
+      <c r="F38" t="str">
+        <v>null</v>
+      </c>
+      <c r="G38" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="E38" t="str">
-        <v>Zuurtegraad waswater &gt; 8,5 (S1 systeem)</v>
-      </c>
-      <c r="F38" t="str">
+      <c r="H38" t="str">
+        <v>Spuiwaterdebiet afwijking naar beneden &gt; 10% (S1 systeem)</v>
+      </c>
+      <c r="I38" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
-      </c>
-      <c r="G38" t="str">
-        <v>null</v>
-      </c>
-      <c r="H38" t="str">
-        <v>null</v>
-      </c>
-      <c r="I38" t="str">
-        <v>null</v>
       </c>
       <c r="J38" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K38" t="str">
-        <v>De zuurtegraad van het waswater is groter dan 8,5</v>
+        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L38" t="str">
-        <v>De zuurtegraad van het waswater is groter dan 8,5|&gt; 8,5</v>
+        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
       </c>
       <c r="M38" t="str">
-        <v>&gt; 8,5</v>
+        <v>&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
       </c>
       <c r="N38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
       </c>
       <c r="O38" t="str">
-        <v>null</v>
+        <v>0.9</v>
       </c>
       <c r="P38" t="str">
-        <v>null</v>
+        <v>product</v>
       </c>
       <c r="Q38" t="str">
-        <v>8.5</v>
+        <v>null</v>
       </c>
       <c r="R38" t="str">
         <v>null</v>
@@ -3558,7 +3558,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/6</v>
       </c>
       <c r="B39" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3567,46 +3567,46 @@
         <v>null</v>
       </c>
       <c r="D39" t="str">
+        <v>null</v>
+      </c>
+      <c r="E39" t="str">
+        <v>null</v>
+      </c>
+      <c r="F39" t="str">
+        <v>null</v>
+      </c>
+      <c r="G39" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="E39" t="str">
-        <v>Geleidbaarheid waswater &gt; maximale waarde (S1 systeem)</v>
-      </c>
-      <c r="F39" t="str">
+      <c r="H39" t="str">
+        <v>Drukval afwijking naar beneden &gt; 40% (S1 systeem)</v>
+      </c>
+      <c r="I39" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
-      </c>
-      <c r="G39" t="str">
-        <v>null</v>
-      </c>
-      <c r="H39" t="str">
-        <v>null</v>
-      </c>
-      <c r="I39" t="str">
-        <v>null</v>
       </c>
       <c r="J39" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K39" t="str">
-        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L39" t="str">
-        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.|&gt; waarde technische fiche</v>
+        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="M39" t="str">
-        <v>&gt; waarde technische fiche</v>
+        <v>&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="N39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="O39" t="str">
-        <v>null</v>
+        <v>0.6</v>
       </c>
       <c r="P39" t="str">
-        <v>som</v>
+        <v>product</v>
       </c>
       <c r="Q39" t="str">
-        <v>0</v>
+        <v>null</v>
       </c>
       <c r="R39" t="str">
         <v>null</v>
@@ -3641,7 +3641,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/4</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/7</v>
       </c>
       <c r="B40" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3650,46 +3650,46 @@
         <v>null</v>
       </c>
       <c r="D40" t="str">
+        <v>null</v>
+      </c>
+      <c r="E40" t="str">
+        <v>null</v>
+      </c>
+      <c r="F40" t="str">
+        <v>null</v>
+      </c>
+      <c r="G40" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="E40" t="str">
-        <v>Waswaterdebiet afwijking naar beneden &gt; 20% (S1 systeem)</v>
-      </c>
-      <c r="F40" t="str">
+      <c r="H40" t="str">
+        <v>Drukval afwijking naar boven &gt; 40% (S1 systeem)</v>
+      </c>
+      <c r="I40" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
-      </c>
-      <c r="G40" t="str">
-        <v>null</v>
-      </c>
-      <c r="H40" t="str">
-        <v>null</v>
-      </c>
-      <c r="I40" t="str">
-        <v>null</v>
       </c>
       <c r="J40" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K40" t="str">
-        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L40" t="str">
-        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="M40" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="N40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="O40" t="str">
-        <v>0.8</v>
+        <v>null</v>
       </c>
       <c r="P40" t="str">
         <v>product</v>
       </c>
       <c r="Q40" t="str">
-        <v>null</v>
+        <v>1.4</v>
       </c>
       <c r="R40" t="str">
         <v>null</v>
@@ -3724,7 +3724,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/5</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/8</v>
       </c>
       <c r="B41" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3733,46 +3733,46 @@
         <v>null</v>
       </c>
       <c r="D41" t="str">
+        <v>null</v>
+      </c>
+      <c r="E41" t="str">
+        <v>null</v>
+      </c>
+      <c r="F41" t="str">
+        <v>null</v>
+      </c>
+      <c r="G41" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="E41" t="str">
-        <v>Spuiwaterdebiet afwijking naar beneden &gt; 10% (S1 systeem)</v>
-      </c>
-      <c r="F41" t="str">
+      <c r="H41" t="str">
+        <v>Zuurtegraad waswater afwijking naar boven &gt; 1 pH-eenheid (S2 systeem)</v>
+      </c>
+      <c r="I41" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="G41" t="str">
-        <v>null</v>
-      </c>
-      <c r="H41" t="str">
-        <v>null</v>
-      </c>
-      <c r="I41" t="str">
-        <v>null</v>
-      </c>
       <c r="J41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K41" t="str">
-        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De zuurtegraad van het waswater wijkt meer dan 1 pH-eenheid naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L41" t="str">
-        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
+        <v>De zuurtegraad van het waswater wijkt meer dan 1 pH-eenheid naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1 pH + waarde technische fiche (afwijking &gt; 1pH)</v>
       </c>
       <c r="M41" t="str">
-        <v>&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
+        <v>&gt; 1 pH + waarde technische fiche (afwijking &gt; 1pH)</v>
       </c>
       <c r="N41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="O41" t="str">
-        <v>0.9</v>
+        <v>null</v>
       </c>
       <c r="P41" t="str">
-        <v>product</v>
+        <v>som</v>
       </c>
       <c r="Q41" t="str">
-        <v>null</v>
+        <v>1</v>
       </c>
       <c r="R41" t="str">
         <v>null</v>
@@ -3807,7 +3807,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/6</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/9</v>
       </c>
       <c r="B42" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3816,46 +3816,46 @@
         <v>null</v>
       </c>
       <c r="D42" t="str">
+        <v>null</v>
+      </c>
+      <c r="E42" t="str">
+        <v>null</v>
+      </c>
+      <c r="F42" t="str">
+        <v>null</v>
+      </c>
+      <c r="G42" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="E42" t="str">
-        <v>Drukval afwijking naar beneden &gt; 40% (S1 systeem)</v>
-      </c>
-      <c r="F42" t="str">
+      <c r="H42" t="str">
+        <v>Geleidbaarheid waswater &gt; maximale waarde (S2 systeem)</v>
+      </c>
+      <c r="I42" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
-      <c r="G42" t="str">
-        <v>null</v>
-      </c>
-      <c r="H42" t="str">
-        <v>null</v>
-      </c>
-      <c r="I42" t="str">
-        <v>null</v>
-      </c>
       <c r="J42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K42" t="str">
-        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="L42" t="str">
-        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.|&gt; waarde technische fiche</v>
       </c>
       <c r="M42" t="str">
-        <v>&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>&gt; waarde technische fiche</v>
       </c>
       <c r="N42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="O42" t="str">
-        <v>0.6</v>
+        <v>null</v>
       </c>
       <c r="P42" t="str">
-        <v>product</v>
+        <v>som</v>
       </c>
       <c r="Q42" t="str">
-        <v>null</v>
+        <v>0</v>
       </c>
       <c r="R42" t="str">
         <v>null</v>
@@ -3890,7 +3890,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/7</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_1</v>
       </c>
       <c r="B43" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3899,49 +3899,49 @@
         <v>null</v>
       </c>
       <c r="D43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="E43" t="str">
-        <v>Drukval afwijking naar boven &gt; 40% (S1 systeem)</v>
+        <v>null</v>
       </c>
       <c r="F43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="G43" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="H43" t="str">
-        <v>null</v>
+        <v>Zuurtegraad waswater S1 systeem</v>
       </c>
       <c r="I43" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="J43" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K43" t="str">
-        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>null</v>
       </c>
       <c r="L43" t="str">
-        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>null</v>
       </c>
       <c r="M43" t="str">
-        <v>&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>null</v>
       </c>
       <c r="N43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="O43" t="str">
         <v>null</v>
       </c>
       <c r="P43" t="str">
-        <v>product</v>
+        <v>null</v>
       </c>
       <c r="Q43" t="str">
-        <v>1.4</v>
+        <v>null</v>
       </c>
       <c r="R43" t="str">
-        <v>null</v>
+        <v>false</v>
       </c>
       <c r="S43" t="str">
         <v>null</v>
@@ -3973,7 +3973,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/8</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_10</v>
       </c>
       <c r="B44" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3982,52 +3982,52 @@
         <v>null</v>
       </c>
       <c r="D44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="E44" t="str">
-        <v>Zuurtegraad waswater afwijking naar boven &gt; 1 pH-eenheid (S2 systeem)</v>
+        <v>null</v>
       </c>
       <c r="F44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="G44" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="H44" t="str">
-        <v>null</v>
+        <v>Drukval S2 systeem</v>
       </c>
       <c r="I44" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="J44" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K44" t="str">
-        <v>De zuurtegraad van het waswater wijkt meer dan 1 pH-eenheid naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>null</v>
       </c>
       <c r="L44" t="str">
-        <v>De zuurtegraad van het waswater wijkt meer dan 1 pH-eenheid naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1 pH + waarde technische fiche (afwijking &gt; 1pH)</v>
+        <v>null</v>
       </c>
       <c r="M44" t="str">
-        <v>&gt; 1 pH + waarde technische fiche (afwijking &gt; 1pH)</v>
+        <v>null</v>
       </c>
       <c r="N44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="O44" t="str">
         <v>null</v>
       </c>
       <c r="P44" t="str">
-        <v>som</v>
+        <v>null</v>
       </c>
       <c r="Q44" t="str">
-        <v>1</v>
+        <v>null</v>
       </c>
       <c r="R44" t="str">
-        <v>null</v>
+        <v>true</v>
       </c>
       <c r="S44" t="str">
-        <v>null</v>
+        <v>exact</v>
       </c>
       <c r="T44" t="str">
         <v>null</v>
@@ -4056,7 +4056,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/9</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_11</v>
       </c>
       <c r="B45" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4065,52 +4065,52 @@
         <v>null</v>
       </c>
       <c r="D45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="E45" t="str">
-        <v>Geleidbaarheid waswater &gt; maximale waarde (S2 systeem)</v>
+        <v>null</v>
       </c>
       <c r="F45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>null</v>
       </c>
       <c r="G45" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="H45" t="str">
-        <v>null</v>
+        <v>Waswaterdebiet voorbevochtiging S3 systeem</v>
       </c>
       <c r="I45" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="J45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K45" t="str">
-        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>null</v>
       </c>
       <c r="L45" t="str">
-        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.|&gt; waarde technische fiche</v>
+        <v>null</v>
       </c>
       <c r="M45" t="str">
-        <v>&gt; waarde technische fiche</v>
+        <v>null</v>
       </c>
       <c r="N45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
       </c>
       <c r="O45" t="str">
         <v>null</v>
       </c>
       <c r="P45" t="str">
-        <v>som</v>
+        <v>null</v>
       </c>
       <c r="Q45" t="str">
-        <v>0</v>
+        <v>null</v>
       </c>
       <c r="R45" t="str">
-        <v>null</v>
+        <v>true</v>
       </c>
       <c r="S45" t="str">
-        <v>null</v>
+        <v>minimum</v>
       </c>
       <c r="T45" t="str">
         <v>null</v>
@@ -4139,7 +4139,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_12</v>
       </c>
       <c r="B46" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4148,25 +4148,25 @@
         <v>null</v>
       </c>
       <c r="D46" t="str">
+        <v>null</v>
+      </c>
+      <c r="E46" t="str">
+        <v>null</v>
+      </c>
+      <c r="F46" t="str">
+        <v>null</v>
+      </c>
+      <c r="G46" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="E46" t="str">
-        <v>Zuurtegraad waswater S1 systeem</v>
-      </c>
-      <c r="F46" t="str">
+      <c r="H46" t="str">
+        <v>Waswaterdebiet bevloeiing S3 systeem</v>
+      </c>
+      <c r="I46" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="G46" t="str">
-        <v>null</v>
-      </c>
-      <c r="H46" t="str">
-        <v>null</v>
-      </c>
-      <c r="I46" t="str">
-        <v>null</v>
-      </c>
       <c r="J46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K46" t="str">
         <v>null</v>
@@ -4178,7 +4178,7 @@
         <v>null</v>
       </c>
       <c r="N46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing</v>
       </c>
       <c r="O46" t="str">
         <v>null</v>
@@ -4190,10 +4190,10 @@
         <v>null</v>
       </c>
       <c r="R46" t="str">
-        <v>false</v>
+        <v>true</v>
       </c>
       <c r="S46" t="str">
-        <v>null</v>
+        <v>minimum</v>
       </c>
       <c r="T46" t="str">
         <v>null</v>
@@ -4222,7 +4222,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/10</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_13</v>
       </c>
       <c r="B47" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4231,25 +4231,25 @@
         <v>null</v>
       </c>
       <c r="D47" t="str">
+        <v>null</v>
+      </c>
+      <c r="E47" t="str">
+        <v>null</v>
+      </c>
+      <c r="F47" t="str">
+        <v>null</v>
+      </c>
+      <c r="G47" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="E47" t="str">
-        <v>Drukval S2 systeem</v>
-      </c>
-      <c r="F47" t="str">
+      <c r="H47" t="str">
+        <v>Biobedspuiwaterproductie S3 systeem</v>
+      </c>
+      <c r="I47" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="G47" t="str">
-        <v>null</v>
-      </c>
-      <c r="H47" t="str">
-        <v>null</v>
-      </c>
-      <c r="I47" t="str">
-        <v>null</v>
-      </c>
       <c r="J47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="K47" t="str">
         <v>null</v>
@@ -4261,7 +4261,7 @@
         <v>null</v>
       </c>
       <c r="N47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie</v>
       </c>
       <c r="O47" t="str">
         <v>null</v>
@@ -4276,7 +4276,7 @@
         <v>true</v>
       </c>
       <c r="S47" t="str">
-        <v>exact</v>
+        <v>minimum</v>
       </c>
       <c r="T47" t="str">
         <v>null</v>
@@ -4305,7 +4305,7 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/11</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_14</v>
       </c>
       <c r="B48" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4314,22 +4314,22 @@
         <v>null</v>
       </c>
       <c r="D48" t="str">
+        <v>null</v>
+      </c>
+      <c r="E48" t="str">
+        <v>null</v>
+      </c>
+      <c r="F48" t="str">
+        <v>null</v>
+      </c>
+      <c r="G48" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="E48" t="str">
-        <v>Waswaterdebiet voorbevochtiging S3 systeem</v>
-      </c>
-      <c r="F48" t="str">
+      <c r="H48" t="str">
+        <v>Biobedspoelwaterproductie S3 systeem</v>
+      </c>
+      <c r="I48" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
-      </c>
-      <c r="G48" t="str">
-        <v>null</v>
-      </c>
-      <c r="H48" t="str">
-        <v>null</v>
-      </c>
-      <c r="I48" t="str">
-        <v>null</v>
       </c>
       <c r="J48" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
@@ -4344,7 +4344,7 @@
         <v>null</v>
       </c>
       <c r="N48" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie</v>
       </c>
       <c r="O48" t="str">
         <v>null</v>
@@ -4388,7 +4388,7 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/12</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_15</v>
       </c>
       <c r="B49" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4397,22 +4397,22 @@
         <v>null</v>
       </c>
       <c r="D49" t="str">
+        <v>null</v>
+      </c>
+      <c r="E49" t="str">
+        <v>null</v>
+      </c>
+      <c r="F49" t="str">
+        <v>null</v>
+      </c>
+      <c r="G49" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="E49" t="str">
-        <v>Waswaterdebiet bevloeiing S3 systeem</v>
-      </c>
-      <c r="F49" t="str">
+      <c r="H49" t="str">
+        <v>Drukval S3 systeem</v>
+      </c>
+      <c r="I49" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
-      </c>
-      <c r="G49" t="str">
-        <v>null</v>
-      </c>
-      <c r="H49" t="str">
-        <v>null</v>
-      </c>
-      <c r="I49" t="str">
-        <v>null</v>
       </c>
       <c r="J49" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
@@ -4427,7 +4427,7 @@
         <v>null</v>
       </c>
       <c r="N49" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="O49" t="str">
         <v>null</v>
@@ -4442,7 +4442,7 @@
         <v>true</v>
       </c>
       <c r="S49" t="str">
-        <v>minimum</v>
+        <v>maximum</v>
       </c>
       <c r="T49" t="str">
         <v>null</v>
@@ -4471,7 +4471,7 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/13</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_2</v>
       </c>
       <c r="B50" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4480,25 +4480,25 @@
         <v>null</v>
       </c>
       <c r="D50" t="str">
+        <v>null</v>
+      </c>
+      <c r="E50" t="str">
+        <v>null</v>
+      </c>
+      <c r="F50" t="str">
+        <v>null</v>
+      </c>
+      <c r="G50" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="E50" t="str">
-        <v>Biobedspuiwaterproductie S3 systeem</v>
-      </c>
-      <c r="F50" t="str">
+      <c r="H50" t="str">
+        <v>Geleidbaarheid waswater S1 systeem</v>
+      </c>
+      <c r="I50" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="G50" t="str">
-        <v>null</v>
-      </c>
-      <c r="H50" t="str">
-        <v>null</v>
-      </c>
-      <c r="I50" t="str">
-        <v>null</v>
-      </c>
       <c r="J50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K50" t="str">
         <v>null</v>
@@ -4510,7 +4510,7 @@
         <v>null</v>
       </c>
       <c r="N50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="O50" t="str">
         <v>null</v>
@@ -4525,7 +4525,7 @@
         <v>true</v>
       </c>
       <c r="S50" t="str">
-        <v>minimum</v>
+        <v>maximum</v>
       </c>
       <c r="T50" t="str">
         <v>null</v>
@@ -4554,7 +4554,7 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/14</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_3</v>
       </c>
       <c r="B51" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4563,25 +4563,25 @@
         <v>null</v>
       </c>
       <c r="D51" t="str">
+        <v>null</v>
+      </c>
+      <c r="E51" t="str">
+        <v>null</v>
+      </c>
+      <c r="F51" t="str">
+        <v>null</v>
+      </c>
+      <c r="G51" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="E51" t="str">
-        <v>Biobedspoelwaterproductie S3 systeem</v>
-      </c>
-      <c r="F51" t="str">
+      <c r="H51" t="str">
+        <v>Waswaterdebiet S1 systeem</v>
+      </c>
+      <c r="I51" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="G51" t="str">
-        <v>null</v>
-      </c>
-      <c r="H51" t="str">
-        <v>null</v>
-      </c>
-      <c r="I51" t="str">
-        <v>null</v>
-      </c>
       <c r="J51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K51" t="str">
         <v>null</v>
@@ -4593,7 +4593,7 @@
         <v>null</v>
       </c>
       <c r="N51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
       </c>
       <c r="O51" t="str">
         <v>null</v>
@@ -4637,7 +4637,7 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/15</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_4</v>
       </c>
       <c r="B52" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4646,25 +4646,25 @@
         <v>null</v>
       </c>
       <c r="D52" t="str">
+        <v>null</v>
+      </c>
+      <c r="E52" t="str">
+        <v>null</v>
+      </c>
+      <c r="F52" t="str">
+        <v>null</v>
+      </c>
+      <c r="G52" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="E52" t="str">
-        <v>Drukval S3 systeem</v>
-      </c>
-      <c r="F52" t="str">
+      <c r="H52" t="str">
+        <v>Spuiwaterdebiet S1 systeem</v>
+      </c>
+      <c r="I52" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="G52" t="str">
-        <v>null</v>
-      </c>
-      <c r="H52" t="str">
-        <v>null</v>
-      </c>
-      <c r="I52" t="str">
-        <v>null</v>
-      </c>
       <c r="J52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="K52" t="str">
         <v>null</v>
@@ -4676,7 +4676,7 @@
         <v>null</v>
       </c>
       <c r="N52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
       </c>
       <c r="O52" t="str">
         <v>null</v>
@@ -4691,7 +4691,7 @@
         <v>true</v>
       </c>
       <c r="S52" t="str">
-        <v>maximum</v>
+        <v>minimum</v>
       </c>
       <c r="T52" t="str">
         <v>null</v>
@@ -4720,7 +4720,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_5</v>
       </c>
       <c r="B53" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4729,22 +4729,22 @@
         <v>null</v>
       </c>
       <c r="D53" t="str">
+        <v>null</v>
+      </c>
+      <c r="E53" t="str">
+        <v>null</v>
+      </c>
+      <c r="F53" t="str">
+        <v>null</v>
+      </c>
+      <c r="G53" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="E53" t="str">
-        <v>Geleidbaarheid waswater S1 systeem</v>
-      </c>
-      <c r="F53" t="str">
+      <c r="H53" t="str">
+        <v>Drukval S1 systeem</v>
+      </c>
+      <c r="I53" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
-      </c>
-      <c r="G53" t="str">
-        <v>null</v>
-      </c>
-      <c r="H53" t="str">
-        <v>null</v>
-      </c>
-      <c r="I53" t="str">
-        <v>null</v>
       </c>
       <c r="J53" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
@@ -4759,7 +4759,7 @@
         <v>null</v>
       </c>
       <c r="N53" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
       </c>
       <c r="O53" t="str">
         <v>null</v>
@@ -4774,7 +4774,7 @@
         <v>true</v>
       </c>
       <c r="S53" t="str">
-        <v>maximum</v>
+        <v>exact</v>
       </c>
       <c r="T53" t="str">
         <v>null</v>
@@ -4803,7 +4803,7 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_6</v>
       </c>
       <c r="B54" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4812,25 +4812,25 @@
         <v>null</v>
       </c>
       <c r="D54" t="str">
+        <v>null</v>
+      </c>
+      <c r="E54" t="str">
+        <v>null</v>
+      </c>
+      <c r="F54" t="str">
+        <v>null</v>
+      </c>
+      <c r="G54" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="E54" t="str">
-        <v>Waswaterdebiet S1 systeem</v>
-      </c>
-      <c r="F54" t="str">
+      <c r="H54" t="str">
+        <v>Zuurtegraad waswater S2 systeem</v>
+      </c>
+      <c r="I54" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="G54" t="str">
-        <v>null</v>
-      </c>
-      <c r="H54" t="str">
-        <v>null</v>
-      </c>
-      <c r="I54" t="str">
-        <v>null</v>
-      </c>
       <c r="J54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K54" t="str">
         <v>null</v>
@@ -4842,7 +4842,7 @@
         <v>null</v>
       </c>
       <c r="N54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="O54" t="str">
         <v>null</v>
@@ -4857,7 +4857,7 @@
         <v>true</v>
       </c>
       <c r="S54" t="str">
-        <v>minimum</v>
+        <v>maximum</v>
       </c>
       <c r="T54" t="str">
         <v>null</v>
@@ -4886,7 +4886,7 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/4</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_7</v>
       </c>
       <c r="B55" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4895,25 +4895,25 @@
         <v>null</v>
       </c>
       <c r="D55" t="str">
+        <v>null</v>
+      </c>
+      <c r="E55" t="str">
+        <v>null</v>
+      </c>
+      <c r="F55" t="str">
+        <v>null</v>
+      </c>
+      <c r="G55" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="E55" t="str">
-        <v>Spuiwaterdebiet S1 systeem</v>
-      </c>
-      <c r="F55" t="str">
+      <c r="H55" t="str">
+        <v>Geleidbaarheid waswater S2 systeem</v>
+      </c>
+      <c r="I55" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="G55" t="str">
-        <v>null</v>
-      </c>
-      <c r="H55" t="str">
-        <v>null</v>
-      </c>
-      <c r="I55" t="str">
-        <v>null</v>
-      </c>
       <c r="J55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K55" t="str">
         <v>null</v>
@@ -4925,7 +4925,7 @@
         <v>null</v>
       </c>
       <c r="N55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="O55" t="str">
         <v>null</v>
@@ -4940,7 +4940,7 @@
         <v>true</v>
       </c>
       <c r="S55" t="str">
-        <v>minimum</v>
+        <v>maximum</v>
       </c>
       <c r="T55" t="str">
         <v>null</v>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/5</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_8</v>
       </c>
       <c r="B56" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4978,25 +4978,25 @@
         <v>null</v>
       </c>
       <c r="D56" t="str">
+        <v>null</v>
+      </c>
+      <c r="E56" t="str">
+        <v>null</v>
+      </c>
+      <c r="F56" t="str">
+        <v>null</v>
+      </c>
+      <c r="G56" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="E56" t="str">
-        <v>Drukval S1 systeem</v>
-      </c>
-      <c r="F56" t="str">
+      <c r="H56" t="str">
+        <v>Waswaterdebiet S2 systeem</v>
+      </c>
+      <c r="I56" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="G56" t="str">
-        <v>null</v>
-      </c>
-      <c r="H56" t="str">
-        <v>null</v>
-      </c>
-      <c r="I56" t="str">
-        <v>null</v>
-      </c>
       <c r="J56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="K56" t="str">
         <v>null</v>
@@ -5008,7 +5008,7 @@
         <v>null</v>
       </c>
       <c r="N56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
       </c>
       <c r="O56" t="str">
         <v>null</v>
@@ -5023,7 +5023,7 @@
         <v>true</v>
       </c>
       <c r="S56" t="str">
-        <v>exact</v>
+        <v>minimum</v>
       </c>
       <c r="T56" t="str">
         <v>null</v>
@@ -5052,7 +5052,7 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/6</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_9</v>
       </c>
       <c r="B57" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5061,22 +5061,22 @@
         <v>null</v>
       </c>
       <c r="D57" t="str">
+        <v>null</v>
+      </c>
+      <c r="E57" t="str">
+        <v>null</v>
+      </c>
+      <c r="F57" t="str">
+        <v>null</v>
+      </c>
+      <c r="G57" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
-      <c r="E57" t="str">
-        <v>Zuurtegraad waswater S2 systeem</v>
-      </c>
-      <c r="F57" t="str">
+      <c r="H57" t="str">
+        <v>Spuiwaterdebiet S2 systeem</v>
+      </c>
+      <c r="I57" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
-      </c>
-      <c r="G57" t="str">
-        <v>null</v>
-      </c>
-      <c r="H57" t="str">
-        <v>null</v>
-      </c>
-      <c r="I57" t="str">
-        <v>null</v>
       </c>
       <c r="J57" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
@@ -5091,7 +5091,7 @@
         <v>null</v>
       </c>
       <c r="N57" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
       </c>
       <c r="O57" t="str">
         <v>null</v>
@@ -5106,7 +5106,7 @@
         <v>true</v>
       </c>
       <c r="S57" t="str">
-        <v>maximum</v>
+        <v>minimum</v>
       </c>
       <c r="T57" t="str">
         <v>null</v>
@@ -5135,7 +5135,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/7</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/in_gebruik</v>
       </c>
       <c r="B58" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5144,25 +5144,25 @@
         <v>null</v>
       </c>
       <c r="D58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="E58" t="str">
-        <v>Geleidbaarheid waswater S2 systeem</v>
+        <v>null</v>
       </c>
       <c r="F58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="G58" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
       </c>
       <c r="H58" t="str">
-        <v>null</v>
+        <v>Stal in gebruik, dieren aanwezig.</v>
       </c>
       <c r="I58" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
       </c>
       <c r="J58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>null</v>
       </c>
       <c r="K58" t="str">
         <v>null</v>
@@ -5174,7 +5174,7 @@
         <v>null</v>
       </c>
       <c r="N58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater</v>
+        <v>null</v>
       </c>
       <c r="O58" t="str">
         <v>null</v>
@@ -5186,10 +5186,10 @@
         <v>null</v>
       </c>
       <c r="R58" t="str">
-        <v>true</v>
+        <v>null</v>
       </c>
       <c r="S58" t="str">
-        <v>maximum</v>
+        <v>null</v>
       </c>
       <c r="T58" t="str">
         <v>null</v>
@@ -5218,7 +5218,7 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/8</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/leeg</v>
       </c>
       <c r="B59" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5227,25 +5227,25 @@
         <v>null</v>
       </c>
       <c r="D59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="E59" t="str">
-        <v>Waswaterdebiet S2 systeem</v>
+        <v>null</v>
       </c>
       <c r="F59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="G59" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
       </c>
       <c r="H59" t="str">
-        <v>null</v>
+        <v>Lege stal</v>
       </c>
       <c r="I59" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
       </c>
       <c r="J59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>null</v>
       </c>
       <c r="K59" t="str">
         <v>null</v>
@@ -5257,7 +5257,7 @@
         <v>null</v>
       </c>
       <c r="N59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet</v>
+        <v>null</v>
       </c>
       <c r="O59" t="str">
         <v>null</v>
@@ -5269,10 +5269,10 @@
         <v>null</v>
       </c>
       <c r="R59" t="str">
-        <v>true</v>
+        <v>null</v>
       </c>
       <c r="S59" t="str">
-        <v>minimum</v>
+        <v>null</v>
       </c>
       <c r="T59" t="str">
         <v>null</v>
@@ -5301,7 +5301,7 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/9</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/gereinigd</v>
       </c>
       <c r="B60" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5310,25 +5310,25 @@
         <v>null</v>
       </c>
       <c r="D60" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="E60" t="str">
-        <v>Spuiwaterdebiet S2 systeem</v>
+        <v>null</v>
       </c>
       <c r="F60" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>null</v>
       </c>
       <c r="G60" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="H60" t="str">
-        <v>null</v>
+        <v>Gereinigd</v>
       </c>
       <c r="I60" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="J60" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>null</v>
       </c>
       <c r="K60" t="str">
         <v>null</v>
@@ -5340,7 +5340,7 @@
         <v>null</v>
       </c>
       <c r="N60" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie</v>
+        <v>null</v>
       </c>
       <c r="O60" t="str">
         <v>null</v>
@@ -5352,10 +5352,10 @@
         <v>null</v>
       </c>
       <c r="R60" t="str">
-        <v>true</v>
+        <v>null</v>
       </c>
       <c r="S60" t="str">
-        <v>minimum</v>
+        <v>null</v>
       </c>
       <c r="T60" t="str">
         <v>null</v>
@@ -5384,7 +5384,7 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/in_gebruik</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/onderhoud</v>
       </c>
       <c r="B61" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5393,22 +5393,22 @@
         <v>null</v>
       </c>
       <c r="D61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
+        <v>null</v>
       </c>
       <c r="E61" t="str">
-        <v>Stal in gebruik, dieren aanwezig.</v>
+        <v>null</v>
       </c>
       <c r="F61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
+        <v>null</v>
       </c>
       <c r="G61" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="H61" t="str">
-        <v>null</v>
+        <v>In onderhoud</v>
       </c>
       <c r="I61" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="J61" t="str">
         <v>null</v>
@@ -5467,7 +5467,7 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/leeg</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/operationeel</v>
       </c>
       <c r="B62" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5476,22 +5476,22 @@
         <v>null</v>
       </c>
       <c r="D62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
+        <v>null</v>
       </c>
       <c r="E62" t="str">
-        <v>Lege stal</v>
+        <v>null</v>
       </c>
       <c r="F62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
+        <v>null</v>
       </c>
       <c r="G62" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="H62" t="str">
-        <v>null</v>
+        <v>Operationeel</v>
       </c>
       <c r="I62" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="J62" t="str">
         <v>null</v>
@@ -5550,7 +5550,7 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/gereinigd</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/storing</v>
       </c>
       <c r="B63" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5559,22 +5559,22 @@
         <v>null</v>
       </c>
       <c r="D63" t="str">
+        <v>null</v>
+      </c>
+      <c r="E63" t="str">
+        <v>null</v>
+      </c>
+      <c r="F63" t="str">
+        <v>null</v>
+      </c>
+      <c r="G63" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
-      <c r="E63" t="str">
-        <v>Gereinigd</v>
-      </c>
-      <c r="F63" t="str">
+      <c r="H63" t="str">
+        <v>Storing</v>
+      </c>
+      <c r="I63" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
-      </c>
-      <c r="G63" t="str">
-        <v>null</v>
-      </c>
-      <c r="H63" t="str">
-        <v>null</v>
-      </c>
-      <c r="I63" t="str">
-        <v>null</v>
       </c>
       <c r="J63" t="str">
         <v>null</v>
@@ -5633,7 +5633,7 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/onderhoud</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
       </c>
       <c r="B64" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5642,19 +5642,19 @@
         <v>null</v>
       </c>
       <c r="D64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+        <v>null</v>
       </c>
       <c r="E64" t="str">
-        <v>In onderhoud</v>
+        <v>null</v>
       </c>
       <c r="F64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+        <v>null</v>
       </c>
       <c r="G64" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
       </c>
       <c r="H64" t="str">
-        <v>null</v>
+        <v>Luchtwassysteem</v>
       </c>
       <c r="I64" t="str">
         <v>null</v>
@@ -5690,19 +5690,19 @@
         <v>null</v>
       </c>
       <c r="T64" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="U64" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="V64" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="W64" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="X64" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="Y64" t="str">
         <v>null</v>
@@ -5716,7 +5716,7 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/operationeel</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="B65" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5725,22 +5725,22 @@
         <v>null</v>
       </c>
       <c r="D65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+        <v>null</v>
       </c>
       <c r="E65" t="str">
-        <v>Operationeel</v>
+        <v>null</v>
       </c>
       <c r="F65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+        <v>null</v>
       </c>
       <c r="G65" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
       </c>
       <c r="H65" t="str">
-        <v>null</v>
+        <v>Luchtzuiveringssysteem</v>
       </c>
       <c r="I65" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
       </c>
       <c r="J65" t="str">
         <v>null</v>
@@ -5779,13 +5779,13 @@
         <v>null</v>
       </c>
       <c r="V65" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
       </c>
       <c r="W65" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
       </c>
       <c r="X65" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
       </c>
       <c r="Y65" t="str">
         <v>null</v>
@@ -5799,7 +5799,7 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/storing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
       </c>
       <c r="B66" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5808,19 +5808,19 @@
         <v>null</v>
       </c>
       <c r="D66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+        <v>null</v>
       </c>
       <c r="E66" t="str">
-        <v>Storing</v>
+        <v>null</v>
       </c>
       <c r="F66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+        <v>null</v>
       </c>
       <c r="G66" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
       </c>
       <c r="H66" t="str">
-        <v>null</v>
+        <v>Biologisch luchtwassysteem</v>
       </c>
       <c r="I66" t="str">
         <v>null</v>
@@ -5838,7 +5838,7 @@
         <v>null</v>
       </c>
       <c r="N66" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="O66" t="str">
         <v>null</v>
@@ -5856,10 +5856,10 @@
         <v>null</v>
       </c>
       <c r="T66" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
       </c>
       <c r="U66" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="V66" t="str">
         <v>null</v>
@@ -5868,10 +5868,10 @@
         <v>null</v>
       </c>
       <c r="X66" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="Y66" t="str">
-        <v>null</v>
+        <v>S1</v>
       </c>
       <c r="Z66" t="str">
         <v>null</v>
@@ -5882,7 +5882,7 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
       </c>
       <c r="B67" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5891,19 +5891,19 @@
         <v>null</v>
       </c>
       <c r="D67" t="str">
+        <v>null</v>
+      </c>
+      <c r="E67" t="str">
+        <v>null</v>
+      </c>
+      <c r="F67" t="str">
+        <v>null</v>
+      </c>
+      <c r="G67" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
       </c>
-      <c r="E67" t="str">
-        <v>Luchtwassysteem</v>
-      </c>
-      <c r="F67" t="str">
-        <v>null</v>
-      </c>
-      <c r="G67" t="str">
-        <v>null</v>
-      </c>
       <c r="H67" t="str">
-        <v>null</v>
+        <v>Chemisch luchtwassysteem</v>
       </c>
       <c r="I67" t="str">
         <v>null</v>
@@ -5921,7 +5921,7 @@
         <v>null</v>
       </c>
       <c r="N67" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
       <c r="O67" t="str">
         <v>null</v>
@@ -5939,22 +5939,22 @@
         <v>null</v>
       </c>
       <c r="T67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
       </c>
       <c r="U67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="V67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>null</v>
       </c>
       <c r="W67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>null</v>
       </c>
       <c r="X67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="Y67" t="str">
-        <v>null</v>
+        <v>S2</v>
       </c>
       <c r="Z67" t="str">
         <v>null</v>
@@ -5965,7 +5965,7 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
       </c>
       <c r="B68" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5974,19 +5974,19 @@
         <v>null</v>
       </c>
       <c r="D68" t="str">
+        <v>null</v>
+      </c>
+      <c r="E68" t="str">
+        <v>null</v>
+      </c>
+      <c r="F68" t="str">
+        <v>null</v>
+      </c>
+      <c r="G68" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
       </c>
-      <c r="E68" t="str">
-        <v>Luchtzuiveringssysteem</v>
-      </c>
-      <c r="F68" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
-      </c>
-      <c r="G68" t="str">
-        <v>null</v>
-      </c>
       <c r="H68" t="str">
-        <v>null</v>
+        <v>Biobed</v>
       </c>
       <c r="I68" t="str">
         <v>null</v>
@@ -6004,7 +6004,7 @@
         <v>null</v>
       </c>
       <c r="N68" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
       </c>
       <c r="O68" t="str">
         <v>null</v>
@@ -6022,22 +6022,22 @@
         <v>null</v>
       </c>
       <c r="T68" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="U68" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="V68" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="W68" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="X68" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
       <c r="Y68" t="str">
-        <v>null</v>
+        <v>S3</v>
       </c>
       <c r="Z68" t="str">
         <v>null</v>
@@ -6048,7 +6048,7 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k1</v>
       </c>
       <c r="B69" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -6057,37 +6057,37 @@
         <v>null</v>
       </c>
       <c r="D69" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
+        <v>null</v>
       </c>
       <c r="E69" t="str">
-        <v>Biologisch luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="F69" t="str">
         <v>null</v>
       </c>
       <c r="G69" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
       </c>
       <c r="H69" t="str">
-        <v>null</v>
+        <v>Klasse 1</v>
       </c>
       <c r="I69" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
       </c>
       <c r="J69" t="str">
         <v>null</v>
       </c>
       <c r="K69" t="str">
-        <v>null</v>
+        <v>Indelingsklasse voor inrichtingen met de grootste milieu-impact. Voor deze activiteiten geldt een omgevingsvergunning klasse 1 (zwaarste procedure).</v>
       </c>
       <c r="L69" t="str">
-        <v>null</v>
+        <v>Indelingsklasse voor inrichtingen met de grootste milieu-impact. Voor deze activiteiten geldt een omgevingsvergunning klasse 1 (zwaarste procedure).</v>
       </c>
       <c r="M69" t="str">
         <v>null</v>
       </c>
       <c r="N69" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>null</v>
       </c>
       <c r="O69" t="str">
         <v>null</v>
@@ -6105,10 +6105,10 @@
         <v>null</v>
       </c>
       <c r="T69" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="U69" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="V69" t="str">
         <v>null</v>
@@ -6117,13 +6117,13 @@
         <v>null</v>
       </c>
       <c r="X69" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="Y69" t="str">
-        <v>S1</v>
+        <v>null</v>
       </c>
       <c r="Z69" t="str">
-        <v>null</v>
+        <v>VLAREM klasse 1</v>
       </c>
       <c r="AA69" t="str">
         <v>null</v>
@@ -6131,7 +6131,7 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k2</v>
       </c>
       <c r="B70" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -6140,37 +6140,37 @@
         <v>null</v>
       </c>
       <c r="D70" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
+        <v>null</v>
       </c>
       <c r="E70" t="str">
-        <v>Chemisch luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="F70" t="str">
         <v>null</v>
       </c>
       <c r="G70" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
       </c>
       <c r="H70" t="str">
-        <v>null</v>
+        <v>Klasse 2</v>
       </c>
       <c r="I70" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
       </c>
       <c r="J70" t="str">
         <v>null</v>
       </c>
       <c r="K70" t="str">
-        <v>null</v>
+        <v>Indelingsklasse voor inrichtingen met een middelgrote milieu-impact. Voor deze activiteiten geldt een omgevingsvergunning klasse 2.</v>
       </c>
       <c r="L70" t="str">
-        <v>null</v>
+        <v>Indelingsklasse voor inrichtingen met een middelgrote milieu-impact. Voor deze activiteiten geldt een omgevingsvergunning klasse 2.</v>
       </c>
       <c r="M70" t="str">
         <v>null</v>
       </c>
       <c r="N70" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>null</v>
       </c>
       <c r="O70" t="str">
         <v>null</v>
@@ -6188,10 +6188,10 @@
         <v>null</v>
       </c>
       <c r="T70" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="U70" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="V70" t="str">
         <v>null</v>
@@ -6200,13 +6200,13 @@
         <v>null</v>
       </c>
       <c r="X70" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="Y70" t="str">
-        <v>S2</v>
+        <v>null</v>
       </c>
       <c r="Z70" t="str">
-        <v>null</v>
+        <v>VLAREM klasse 2</v>
       </c>
       <c r="AA70" t="str">
         <v>null</v>
@@ -6214,7 +6214,7 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k3</v>
       </c>
       <c r="B71" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -6223,37 +6223,37 @@
         <v>null</v>
       </c>
       <c r="D71" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
+        <v>null</v>
       </c>
       <c r="E71" t="str">
-        <v>Biobed</v>
+        <v>null</v>
       </c>
       <c r="F71" t="str">
         <v>null</v>
       </c>
       <c r="G71" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
       </c>
       <c r="H71" t="str">
-        <v>null</v>
+        <v>Klasse 3</v>
       </c>
       <c r="I71" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
       </c>
       <c r="J71" t="str">
         <v>null</v>
       </c>
       <c r="K71" t="str">
-        <v>null</v>
+        <v>Indelingsklasse voor inrichtingen met een beperkte milieu-impact. Voor deze activiteiten geldt een meldingsplicht (klasse 3).</v>
       </c>
       <c r="L71" t="str">
-        <v>null</v>
+        <v>Indelingsklasse voor inrichtingen met een beperkte milieu-impact. Voor deze activiteiten geldt een meldingsplicht (klasse 3).</v>
       </c>
       <c r="M71" t="str">
         <v>null</v>
       </c>
       <c r="N71" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging</v>
+        <v>null</v>
       </c>
       <c r="O71" t="str">
         <v>null</v>
@@ -6271,10 +6271,10 @@
         <v>null</v>
       </c>
       <c r="T71" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="U71" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="V71" t="str">
         <v>null</v>
@@ -6283,13 +6283,13 @@
         <v>null</v>
       </c>
       <c r="X71" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="Y71" t="str">
-        <v>S3</v>
+        <v>null</v>
       </c>
       <c r="Z71" t="str">
-        <v>null</v>
+        <v>VLAREM klasse 3</v>
       </c>
       <c r="AA71" t="str">
         <v>null</v>
@@ -6297,7 +6297,7 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/bedrijfsklasse</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
       </c>
       <c r="B72" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6309,7 +6309,7 @@
         <v>null</v>
       </c>
       <c r="E72" t="str">
-        <v>conceptschema iioa bedrijfsklassen</v>
+        <v>null</v>
       </c>
       <c r="F72" t="str">
         <v>null</v>
@@ -6318,7 +6318,7 @@
         <v>null</v>
       </c>
       <c r="H72" t="str">
-        <v>null</v>
+        <v>conceptschema luchtzuiveringssysteem parameter specificatie</v>
       </c>
       <c r="I72" t="str">
         <v>null</v>
@@ -6327,10 +6327,10 @@
         <v>null</v>
       </c>
       <c r="K72" t="str">
-        <v>null</v>
+        <v>Het schema van indelingsklassen (1, 2, 3) zoals vastgelegd in de Vlaamse milieuregelgeving (VLAREM).</v>
       </c>
       <c r="L72" t="str">
-        <v>null</v>
+        <v>Het schema van indelingsklassen (1, 2, 3) zoals vastgelegd in de Vlaamse milieuregelgeving (VLAREM).</v>
       </c>
       <c r="M72" t="str">
         <v>null</v>
@@ -6372,15 +6372,15 @@
         <v>null</v>
       </c>
       <c r="Z72" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/bedrijfklasse/1|https://data.omgeving.vlaanderen.be/id/concept/bedrijfklasse/2|https://data.omgeving.vlaanderen.be/id/concept/bedrijfklasse/3</v>
+        <v>null</v>
       </c>
       <c r="AA72" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_10|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_11|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_12|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_13|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_14|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_15|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_4|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_5|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_6|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_7|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_8|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/_9</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzs-param-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
       </c>
       <c r="B73" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6392,7 +6392,7 @@
         <v>null</v>
       </c>
       <c r="E73" t="str">
-        <v>conceptschema luchtzuiveringssysteem parameter specificatie</v>
+        <v>null</v>
       </c>
       <c r="F73" t="str">
         <v>null</v>
@@ -6401,7 +6401,7 @@
         <v>null</v>
       </c>
       <c r="H73" t="str">
-        <v>null</v>
+        <v>conceptschema luchtzuiveringssysteem medium</v>
       </c>
       <c r="I73" t="str">
         <v>null</v>
@@ -6455,15 +6455,15 @@
         <v>null</v>
       </c>
       <c r="Z73" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/10|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/11|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/12|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/13|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/14|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/15|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/4|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/5|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/6|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/7|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/8|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/parameter_norm/9</v>
+        <v>null</v>
       </c>
       <c r="AA73" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/lucht|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/stal|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/hetelektronischmonitoringssysteem</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
       </c>
       <c r="B74" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6475,7 +6475,7 @@
         <v>null</v>
       </c>
       <c r="E74" t="str">
-        <v>conceptschema luchtzuiveringssysteem medium</v>
+        <v>null</v>
       </c>
       <c r="F74" t="str">
         <v>null</v>
@@ -6484,7 +6484,7 @@
         <v>null</v>
       </c>
       <c r="H74" t="str">
-        <v>null</v>
+        <v>conceptschema luchtzuiveringssysteem eigenschap</v>
       </c>
       <c r="I74" t="str">
         <v>null</v>
@@ -6538,15 +6538,15 @@
         <v>null</v>
       </c>
       <c r="Z74" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/waswater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/spuiwater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/lucht|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/stal|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/medium/hetelektronischmonitoringssysteem</v>
+        <v>null</v>
       </c>
       <c r="AA74" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsp</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
       </c>
       <c r="B75" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6558,7 +6558,7 @@
         <v>null</v>
       </c>
       <c r="E75" t="str">
-        <v>conceptschema luchtzuiveringssysteem eigenschap</v>
+        <v>null</v>
       </c>
       <c r="F75" t="str">
         <v>null</v>
@@ -6567,7 +6567,7 @@
         <v>null</v>
       </c>
       <c r="H75" t="str">
-        <v>null</v>
+        <v>conceptschema luchtzuiveringssysteem status</v>
       </c>
       <c r="I75" t="str">
         <v>null</v>
@@ -6621,15 +6621,15 @@
         <v>null</v>
       </c>
       <c r="Z75" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspoelwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/biobedspuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/systeemstatus|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietbevloeiing|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/waswaterdebietvoorbevochtiging|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/eigenschap/zuurtegraadwaswater</v>
+        <v>null</v>
       </c>
       <c r="AA75" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/gereinigd|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/onderhoud|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/operationeel|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/storing</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzss</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
       </c>
       <c r="B76" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6641,7 +6641,7 @@
         <v>null</v>
       </c>
       <c r="E76" t="str">
-        <v>conceptschema luchtzuiveringssysteem status</v>
+        <v>null</v>
       </c>
       <c r="F76" t="str">
         <v>null</v>
@@ -6650,7 +6650,7 @@
         <v>null</v>
       </c>
       <c r="H76" t="str">
-        <v>null</v>
+        <v>conceptschema luchtzuiveringssysteem stalbezetting</v>
       </c>
       <c r="I76" t="str">
         <v>null</v>
@@ -6704,15 +6704,15 @@
         <v>null</v>
       </c>
       <c r="Z76" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/gereinigd|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/onderhoud|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/operationeel|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/status/storing</v>
+        <v>null</v>
       </c>
       <c r="AA76" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/in_gebruik|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/leeg</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzsst</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
       </c>
       <c r="B77" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6724,7 +6724,7 @@
         <v>null</v>
       </c>
       <c r="E77" t="str">
-        <v>conceptschema luchtzuiveringssysteem stalbezetting</v>
+        <v>null</v>
       </c>
       <c r="F77" t="str">
         <v>null</v>
@@ -6733,7 +6733,7 @@
         <v>null</v>
       </c>
       <c r="H77" t="str">
-        <v>null</v>
+        <v>conceptschema luchtzuiveringssysteem</v>
       </c>
       <c r="I77" t="str">
         <v>null</v>
@@ -6787,15 +6787,15 @@
         <v>null</v>
       </c>
       <c r="Z77" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/in_gebruik|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/stalgebruik/leeg</v>
+        <v>null</v>
       </c>
       <c r="AA77" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/lzstype</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
       </c>
       <c r="B78" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6807,7 +6807,7 @@
         <v>null</v>
       </c>
       <c r="E78" t="str">
-        <v>conceptschema luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="F78" t="str">
         <v>null</v>
@@ -6816,7 +6816,7 @@
         <v>null</v>
       </c>
       <c r="H78" t="str">
-        <v>null</v>
+        <v>conceptschema luchtzuiveringssysteem normbandbreedte</v>
       </c>
       <c r="I78" t="str">
         <v>null</v>
@@ -6870,15 +6870,15 @@
         <v>null</v>
       </c>
       <c r="Z78" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/type/luchtzuiveringssysteem</v>
+        <v>Ranges</v>
       </c>
       <c r="AA78" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/10|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/11|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/12|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/13|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/14|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/15|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/16|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/4|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/5|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/6|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/7|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/8|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/9</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm_bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
       </c>
       <c r="B79" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -6890,7 +6890,7 @@
         <v>null</v>
       </c>
       <c r="E79" t="str">
-        <v>conceptschema luchtzuiveringssysteem normbandbreedte</v>
+        <v>null</v>
       </c>
       <c r="F79" t="str">
         <v>null</v>
@@ -6899,7 +6899,7 @@
         <v>null</v>
       </c>
       <c r="H79" t="str">
-        <v>null</v>
+        <v>VLAREM indelingsklassen</v>
       </c>
       <c r="I79" t="str">
         <v>null</v>
@@ -6953,10 +6953,10 @@
         <v>null</v>
       </c>
       <c r="Z79" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/10|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/11|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/12|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/13|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/14|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/15|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/16|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/1|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/2|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/3|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/4|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/5|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/6|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/7|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/8|https://data.omgeving.vlaanderen.be/id/concept/luchtzuiveringssysteem/norm_bandbreedte/9</v>
+        <v>null</v>
       </c>
       <c r="AA79" t="str">
-        <v>Ranges</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k1|https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k2|https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nieuw type lely sphere. Nieuwe parameter elektriciteitsverbruik. Grenswaarden technische fiche.
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/luchtzuiveringssysteem/luchtzuiveringssysteem.xlsx
+++ b/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/luchtzuiveringssysteem/luchtzuiveringssysteem.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC76"/>
+  <dimension ref="A1:AC83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -464,10 +464,10 @@
         <v>relevantCodeList</v>
       </c>
       <c r="U1" t="str">
+        <v>referentiewaardeType</v>
+      </c>
+      <c r="V1" t="str">
         <v>technischefiche</v>
-      </c>
-      <c r="V1" t="str">
-        <v>referentiewaardeType</v>
       </c>
       <c r="W1" t="str">
         <v>broader</v>
@@ -476,16 +476,16 @@
         <v>broaderTransitive</v>
       </c>
       <c r="Y1" t="str">
+        <v>code</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>semanticRelation</v>
+      </c>
+      <c r="AA1" t="str">
         <v>narrower</v>
       </c>
-      <c r="Z1" t="str">
+      <c r="AB1" t="str">
         <v>narrowerTransitive</v>
-      </c>
-      <c r="AA1" t="str">
-        <v>semanticRelation</v>
-      </c>
-      <c r="AB1" t="str">
-        <v>code</v>
       </c>
       <c r="AC1" t="str">
         <v>hasTopConcept</v>
@@ -760,16 +760,16 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>http://qudt.org/vocab/quantitykind/VaporPressure</v>
+        <v>http://qudt.org/vocab/quantitykind/Energy</v>
       </c>
       <c r="B5" t="str">
         <v>http://qudt.org/schema/qudt/QuantityKind</v>
       </c>
       <c r="C5" t="str">
-        <v>http://qudt.org/vocab/unit/PA</v>
+        <v>http://qudt.org/vocab/unit/KiloW-HR</v>
       </c>
       <c r="D5" t="str">
-        <v>Dampdruk</v>
+        <v>Vermogen</v>
       </c>
       <c r="E5" t="str">
         <v>null</v>
@@ -849,16 +849,16 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Volume</v>
+        <v>http://qudt.org/vocab/quantitykind/VaporPressure</v>
       </c>
       <c r="B6" t="str">
         <v>http://qudt.org/schema/qudt/QuantityKind</v>
       </c>
       <c r="C6" t="str">
-        <v>http://qudt.org/vocab/unit/M3</v>
+        <v>http://qudt.org/vocab/unit/PA</v>
       </c>
       <c r="D6" t="str">
-        <v>Volume</v>
+        <v>Dampdruk</v>
       </c>
       <c r="E6" t="str">
         <v>null</v>
@@ -938,16 +938,16 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate</v>
+        <v>http://qudt.org/vocab/quantitykind/Volume</v>
       </c>
       <c r="B7" t="str">
         <v>http://qudt.org/schema/qudt/QuantityKind</v>
       </c>
       <c r="C7" t="str">
-        <v>http://qudt.org/vocab/unit/M3-PER-HR</v>
+        <v>http://qudt.org/vocab/unit/M3</v>
       </c>
       <c r="D7" t="str">
-        <v>Volume per tijdseenheid</v>
+        <v>Volume</v>
       </c>
       <c r="E7" t="str">
         <v>null</v>
@@ -1027,25 +1027,25 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/hetelektronischmonitoringssysteem</v>
+        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate</v>
       </c>
       <c r="B8" t="str">
-        <v>http://www.w3.org/2000/01/rdf-schema#Resource|http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://qudt.org/schema/qudt/QuantityKind</v>
       </c>
       <c r="C8" t="str">
-        <v>null</v>
+        <v>http://qudt.org/vocab/unit/M3-PER-HR</v>
       </c>
       <c r="D8" t="str">
-        <v>null</v>
+        <v>Volume per tijdseenheid</v>
       </c>
       <c r="E8" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/medium</v>
+        <v>null</v>
       </c>
       <c r="F8" t="str">
-        <v>Het elektronisch monitoringssysteem</v>
+        <v>null</v>
       </c>
       <c r="G8" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/medium</v>
+        <v>null</v>
       </c>
       <c r="H8" t="str">
         <v>null</v>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/lucht</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/hetelektronischmonitoringssysteem</v>
       </c>
       <c r="B9" t="str">
         <v>http://www.w3.org/2000/01/rdf-schema#Resource|http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1131,7 +1131,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/medium</v>
       </c>
       <c r="F9" t="str">
-        <v>Lucht</v>
+        <v>Het elektronisch monitoringssysteem</v>
       </c>
       <c r="G9" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/medium</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/spuiwater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/lucht</v>
       </c>
       <c r="B10" t="str">
         <v>http://www.w3.org/2000/01/rdf-schema#Resource|http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1220,7 +1220,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/medium</v>
       </c>
       <c r="F10" t="str">
-        <v>Spuiwater</v>
+        <v>Lucht</v>
       </c>
       <c r="G10" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/medium</v>
@@ -1294,7 +1294,7 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/stal</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/spuiwater</v>
       </c>
       <c r="B11" t="str">
         <v>http://www.w3.org/2000/01/rdf-schema#Resource|http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1309,7 +1309,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/medium</v>
       </c>
       <c r="F11" t="str">
-        <v>Stal</v>
+        <v>Spuiwater</v>
       </c>
       <c r="G11" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/medium</v>
@@ -1383,7 +1383,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/waswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/stal</v>
       </c>
       <c r="B12" t="str">
         <v>http://www.w3.org/2000/01/rdf-schema#Resource|http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1398,7 +1398,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/medium</v>
       </c>
       <c r="F12" t="str">
-        <v>Waswater</v>
+        <v>Stal</v>
       </c>
       <c r="G12" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/medium</v>
@@ -1472,10 +1472,10 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/waswater</v>
       </c>
       <c r="B13" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://www.w3.org/2000/01/rdf-schema#Resource|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C13" t="str">
         <v>null</v>
@@ -1484,34 +1484,34 @@
         <v>null</v>
       </c>
       <c r="E13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/medium</v>
       </c>
       <c r="F13" t="str">
-        <v>Zuurtegraad waswater &lt; 6 (S1 systeem)</v>
+        <v>Waswater</v>
       </c>
       <c r="G13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/medium</v>
       </c>
       <c r="H13" t="str">
-        <v>Onder minimum grenswaarde</v>
+        <v>null</v>
       </c>
       <c r="I13" t="str">
-        <v>De zuurtegraad van het waswater is kleiner dan 6</v>
+        <v>null</v>
       </c>
       <c r="J13" t="str">
-        <v>De zuurtegraad van het waswater is kleiner dan 6|&lt; 6</v>
+        <v>null</v>
       </c>
       <c r="K13" t="str">
-        <v>&lt; 6</v>
+        <v>null</v>
       </c>
       <c r="L13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>null</v>
       </c>
       <c r="M13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater</v>
+        <v>null</v>
       </c>
       <c r="N13" t="str">
-        <v>6</v>
+        <v>null</v>
       </c>
       <c r="O13" t="str">
         <v>null</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_10</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_1</v>
       </c>
       <c r="B14" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1576,7 +1576,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F14" t="str">
-        <v>Waswaterdebiet afwijking naar beneden &gt; 20% (S2 systeem)</v>
+        <v>Zuurtegraad waswater &lt; 6 (S1 systeem)</v>
       </c>
       <c r="G14" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
@@ -1585,25 +1585,25 @@
         <v>Onder minimum grenswaarde</v>
       </c>
       <c r="I14" t="str">
-        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De zuurtegraad van het waswater is kleiner dan 6</v>
       </c>
       <c r="J14" t="str">
-        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>De zuurtegraad van het waswater is kleiner dan 6|&lt; 6</v>
       </c>
       <c r="K14" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>&lt; 6</v>
       </c>
       <c r="L14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater</v>
       </c>
       <c r="N14" t="str">
-        <v>0.8</v>
+        <v>6</v>
       </c>
       <c r="O14" t="str">
-        <v>product</v>
+        <v>null</v>
       </c>
       <c r="P14" t="str">
         <v>null</v>
@@ -1650,7 +1650,7 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_11</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_10</v>
       </c>
       <c r="B15" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1665,7 +1665,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F15" t="str">
-        <v>Spuiwaterdebiet afwijking naar beneden &gt; 10% (S2 systeem)</v>
+        <v>Waswaterdebiet afwijking naar beneden &gt; 20% (S2 systeem)</v>
       </c>
       <c r="G15" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
@@ -1674,22 +1674,22 @@
         <v>Onder minimum grenswaarde</v>
       </c>
       <c r="I15" t="str">
-        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="J15" t="str">
-        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
+        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="K15" t="str">
-        <v>&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="L15" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
       </c>
       <c r="M15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet</v>
       </c>
       <c r="N15" t="str">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="O15" t="str">
         <v>product</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_12</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_11</v>
       </c>
       <c r="B16" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1754,7 +1754,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F16" t="str">
-        <v>Drukval afwijking naar beneden &gt; 40% (S2 systeem)</v>
+        <v>Spuiwaterdebiet afwijking naar beneden &gt; 10% (S2 systeem)</v>
       </c>
       <c r="G16" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
@@ -1763,22 +1763,22 @@
         <v>Onder minimum grenswaarde</v>
       </c>
       <c r="I16" t="str">
-        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="J16" t="str">
-        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
       </c>
       <c r="K16" t="str">
-        <v>&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
       </c>
       <c r="L16" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
       </c>
       <c r="M16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie</v>
       </c>
       <c r="N16" t="str">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="O16" t="str">
         <v>product</v>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_13</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_12</v>
       </c>
       <c r="B17" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1843,22 +1843,22 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F17" t="str">
-        <v>Drukval afwijking naar boven &gt; 40% (S2 systeem)</v>
+        <v>Drukval afwijking naar beneden &gt; 40% (S2 systeem)</v>
       </c>
       <c r="G17" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="H17" t="str">
-        <v>Boven maximum grenswaarde</v>
+        <v>Onder minimum grenswaarde</v>
       </c>
       <c r="I17" t="str">
-        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="J17" t="str">
-        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="K17" t="str">
-        <v>&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="L17" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
@@ -1867,13 +1867,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
       </c>
       <c r="N17" t="str">
-        <v>null</v>
+        <v>0.6</v>
       </c>
       <c r="O17" t="str">
         <v>product</v>
       </c>
       <c r="P17" t="str">
-        <v>1.4</v>
+        <v>null</v>
       </c>
       <c r="Q17" t="str">
         <v>null</v>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_14</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_13</v>
       </c>
       <c r="B18" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1932,37 +1932,37 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F18" t="str">
-        <v>Waswaterdebiet voorbevochtiging afwijking naar beneden &gt; 20% (S3 systeem)</v>
+        <v>Drukval afwijking naar boven &gt; 40% (S2 systeem)</v>
       </c>
       <c r="G18" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="H18" t="str">
-        <v>Onder minimum grenswaarde</v>
+        <v>Boven maximum grenswaarde</v>
       </c>
       <c r="I18" t="str">
-        <v>Het waswaterdebiet van de voorbevochtiging wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="J18" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)|Het waswaterdebiet van de voorbevochtiging wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="K18" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="L18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
       </c>
       <c r="M18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietvoorbevochtiging</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
       </c>
       <c r="N18" t="str">
-        <v>0.8</v>
+        <v>null</v>
       </c>
       <c r="O18" t="str">
         <v>product</v>
       </c>
       <c r="P18" t="str">
-        <v>null</v>
+        <v>1.4</v>
       </c>
       <c r="Q18" t="str">
         <v>null</v>
@@ -2006,7 +2006,7 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_15</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_14</v>
       </c>
       <c r="B19" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2021,7 +2021,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F19" t="str">
-        <v>Waswaterdebiet bevloeiing afwijking naar beneden &gt; 20% (S3 systeem)</v>
+        <v>Waswaterdebiet voorbevochtiging afwijking naar beneden &gt; 20% (S3 systeem)</v>
       </c>
       <c r="G19" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
@@ -2030,10 +2030,10 @@
         <v>Onder minimum grenswaarde</v>
       </c>
       <c r="I19" t="str">
-        <v>Het waswaterdebiet van de bevloeiing wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het waswaterdebiet van de voorbevochtiging wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="J19" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)|Het waswaterdebiet van de bevloeiing wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)|Het waswaterdebiet van de voorbevochtiging wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="K19" t="str">
         <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
@@ -2042,7 +2042,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
       </c>
       <c r="M19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietbevloeiing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietvoorbevochtiging</v>
       </c>
       <c r="N19" t="str">
         <v>0.8</v>
@@ -2095,7 +2095,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_16</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_15</v>
       </c>
       <c r="B20" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2110,37 +2110,37 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F20" t="str">
-        <v>Drukval afwijking naar boven &gt; 50 Pa (S3 systeem)</v>
+        <v>Waswaterdebiet bevloeiing afwijking naar beneden &gt; 20% (S3 systeem)</v>
       </c>
       <c r="G20" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="H20" t="str">
-        <v>Boven maximum grenswaarde</v>
+        <v>Onder minimum grenswaarde</v>
       </c>
       <c r="I20" t="str">
-        <v>De drukval wijkt meer dan 50 Pa naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het waswaterdebiet van de bevloeiing wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="J20" t="str">
-        <v>De drukval wijkt meer dan 50 Pa naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 50 Pa + waarde technische fiche (afwijking &gt; 50 Pa)</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)|Het waswaterdebiet van de bevloeiing wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="K20" t="str">
-        <v>&gt; 50 Pa + waarde technische fiche (afwijking &gt; 50 Pa)</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="L20" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
       </c>
       <c r="M20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietbevloeiing</v>
       </c>
       <c r="N20" t="str">
-        <v>null</v>
+        <v>0.8</v>
       </c>
       <c r="O20" t="str">
-        <v>som</v>
+        <v>product</v>
       </c>
       <c r="P20" t="str">
-        <v>50</v>
+        <v>null</v>
       </c>
       <c r="Q20" t="str">
         <v>null</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_16</v>
       </c>
       <c r="B21" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2199,7 +2199,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F21" t="str">
-        <v>Zuurtegraad waswater &gt; 8,5 (S1 systeem)</v>
+        <v>Drukval afwijking naar boven &gt; 50 Pa (S3 systeem)</v>
       </c>
       <c r="G21" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
@@ -2208,28 +2208,28 @@
         <v>Boven maximum grenswaarde</v>
       </c>
       <c r="I21" t="str">
-        <v>De zuurtegraad van het waswater is groter dan 8,5</v>
+        <v>De drukval wijkt meer dan 50 Pa naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="J21" t="str">
-        <v>De zuurtegraad van het waswater is groter dan 8,5|&gt; 8,5</v>
+        <v>De drukval wijkt meer dan 50 Pa naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 50 Pa + waarde technische fiche (afwijking &gt; 50 Pa)</v>
       </c>
       <c r="K21" t="str">
-        <v>&gt; 8,5</v>
+        <v>&gt; 50 Pa + waarde technische fiche (afwijking &gt; 50 Pa)</v>
       </c>
       <c r="L21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
       </c>
       <c r="M21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
       </c>
       <c r="N21" t="str">
         <v>null</v>
       </c>
       <c r="O21" t="str">
-        <v>null</v>
+        <v>som</v>
       </c>
       <c r="P21" t="str">
-        <v>8.5</v>
+        <v>50</v>
       </c>
       <c r="Q21" t="str">
         <v>null</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_2</v>
       </c>
       <c r="B22" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2288,7 +2288,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F22" t="str">
-        <v>Geleidbaarheid waswater &gt; maximale waarde (S1 systeem)</v>
+        <v>Zuurtegraad waswater &gt; 8,5 (S1 systeem)</v>
       </c>
       <c r="G22" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
@@ -2297,28 +2297,28 @@
         <v>Boven maximum grenswaarde</v>
       </c>
       <c r="I22" t="str">
-        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De zuurtegraad van het waswater is groter dan 8,5</v>
       </c>
       <c r="J22" t="str">
-        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.|&gt; waarde technische fiche</v>
+        <v>De zuurtegraad van het waswater is groter dan 8,5|&gt; 8,5</v>
       </c>
       <c r="K22" t="str">
-        <v>&gt; waarde technische fiche</v>
+        <v>&gt; 8,5</v>
       </c>
       <c r="L22" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater</v>
       </c>
       <c r="N22" t="str">
         <v>null</v>
       </c>
       <c r="O22" t="str">
-        <v>som</v>
+        <v>null</v>
       </c>
       <c r="P22" t="str">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="Q22" t="str">
         <v>null</v>
@@ -2362,7 +2362,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_4</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_3</v>
       </c>
       <c r="B23" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2377,37 +2377,37 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F23" t="str">
-        <v>Waswaterdebiet afwijking naar beneden &gt; 20% (S1 systeem)</v>
+        <v>Geleidbaarheid waswater &gt; maximale waarde (S1 systeem)</v>
       </c>
       <c r="G23" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="H23" t="str">
-        <v>Onder minimum grenswaarde</v>
+        <v>Boven maximum grenswaarde</v>
       </c>
       <c r="I23" t="str">
-        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="J23" t="str">
-        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.|&gt; waarde technische fiche</v>
       </c>
       <c r="K23" t="str">
-        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
+        <v>&gt; waarde technische fiche</v>
       </c>
       <c r="L23" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="N23" t="str">
-        <v>0.8</v>
+        <v>null</v>
       </c>
       <c r="O23" t="str">
-        <v>product</v>
+        <v>som</v>
       </c>
       <c r="P23" t="str">
-        <v>null</v>
+        <v>0</v>
       </c>
       <c r="Q23" t="str">
         <v>null</v>
@@ -2451,7 +2451,7 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_5</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_4</v>
       </c>
       <c r="B24" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2466,7 +2466,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F24" t="str">
-        <v>Spuiwaterdebiet afwijking naar beneden &gt; 10% (S1 systeem)</v>
+        <v>Waswaterdebiet afwijking naar beneden &gt; 20% (S1 systeem)</v>
       </c>
       <c r="G24" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
@@ -2475,22 +2475,22 @@
         <v>Onder minimum grenswaarde</v>
       </c>
       <c r="I24" t="str">
-        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="J24" t="str">
-        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
+        <v>Het waswaterdebiet wijkt meer dan 20% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="K24" t="str">
-        <v>&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
+        <v>&lt; 0,8 x waarde technische fiche (afwijking &gt; 20%)</v>
       </c>
       <c r="L24" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet</v>
       </c>
       <c r="N24" t="str">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="O24" t="str">
         <v>product</v>
@@ -2540,7 +2540,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_6</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_5</v>
       </c>
       <c r="B25" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2555,7 +2555,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F25" t="str">
-        <v>Drukval afwijking naar beneden &gt; 40% (S1 systeem)</v>
+        <v>Spuiwaterdebiet afwijking naar beneden &gt; 10% (S1 systeem)</v>
       </c>
       <c r="G25" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
@@ -2564,22 +2564,22 @@
         <v>Onder minimum grenswaarde</v>
       </c>
       <c r="I25" t="str">
-        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="J25" t="str">
-        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>Het spuiwaterdebiet wijkt meer dan 10% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
       </c>
       <c r="K25" t="str">
-        <v>&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>&lt; 0,9 x waarde technische fiche (afwijking &gt; 10%)</v>
       </c>
       <c r="L25" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M25" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie</v>
       </c>
       <c r="N25" t="str">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="O25" t="str">
         <v>product</v>
@@ -2629,7 +2629,7 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_7</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_6</v>
       </c>
       <c r="B26" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2644,22 +2644,22 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F26" t="str">
-        <v>Drukval afwijking naar boven &gt; 40% (S1 systeem)</v>
+        <v>Drukval afwijking naar beneden &gt; 40% (S1 systeem)</v>
       </c>
       <c r="G26" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="H26" t="str">
-        <v>Boven maximum grenswaarde</v>
+        <v>Onder minimum grenswaarde</v>
       </c>
       <c r="I26" t="str">
-        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="J26" t="str">
-        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>De drukval wijkt meer dan 40% naar beneden af van de operationele waarde die op de technische fiche vermeld staat.|&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="K26" t="str">
-        <v>&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
+        <v>&lt; 0,6 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="L26" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
@@ -2668,13 +2668,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
       </c>
       <c r="N26" t="str">
-        <v>null</v>
+        <v>0.6</v>
       </c>
       <c r="O26" t="str">
         <v>product</v>
       </c>
       <c r="P26" t="str">
-        <v>1.4</v>
+        <v>null</v>
       </c>
       <c r="Q26" t="str">
         <v>null</v>
@@ -2718,7 +2718,7 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_8</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_7</v>
       </c>
       <c r="B27" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2733,7 +2733,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F27" t="str">
-        <v>Zuurtegraad waswater afwijking naar boven &gt; 1 pH-eenheid (S2 systeem)</v>
+        <v>Drukval afwijking naar boven &gt; 40% (S1 systeem)</v>
       </c>
       <c r="G27" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
@@ -2742,28 +2742,28 @@
         <v>Boven maximum grenswaarde</v>
       </c>
       <c r="I27" t="str">
-        <v>De zuurtegraad van het waswater wijkt meer dan 1 pH-eenheid naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="J27" t="str">
-        <v>De zuurtegraad van het waswater wijkt meer dan 1 pH-eenheid naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1 pH + waarde technische fiche (afwijking &gt; 1pH)</v>
+        <v>De drukval wijkt meer dan 40% naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="K27" t="str">
-        <v>&gt; 1 pH + waarde technische fiche (afwijking &gt; 1pH)</v>
+        <v>&gt; 1,4 x waarde technische fiche (afwijking &gt; 40%)</v>
       </c>
       <c r="L27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
       </c>
       <c r="N27" t="str">
         <v>null</v>
       </c>
       <c r="O27" t="str">
-        <v>som</v>
+        <v>product</v>
       </c>
       <c r="P27" t="str">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="Q27" t="str">
         <v>null</v>
@@ -2807,7 +2807,7 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_9</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_8</v>
       </c>
       <c r="B28" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2822,7 +2822,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F28" t="str">
-        <v>Geleidbaarheid waswater &gt; maximale waarde (S2 systeem)</v>
+        <v>Zuurtegraad waswater afwijking naar boven &gt; 1 pH-eenheid (S2 systeem)</v>
       </c>
       <c r="G28" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
@@ -2831,19 +2831,19 @@
         <v>Boven maximum grenswaarde</v>
       </c>
       <c r="I28" t="str">
-        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.</v>
+        <v>De zuurtegraad van het waswater wijkt meer dan 1 pH-eenheid naar boven af van de operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="J28" t="str">
-        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.|&gt; waarde technische fiche</v>
+        <v>De zuurtegraad van het waswater wijkt meer dan 1 pH-eenheid naar boven af van de operationele waarde die op de technische fiche vermeld staat.|&gt; 1 pH + waarde technische fiche (afwijking &gt; 1pH)</v>
       </c>
       <c r="K28" t="str">
-        <v>&gt; waarde technische fiche</v>
+        <v>&gt; 1 pH + waarde technische fiche (afwijking &gt; 1pH)</v>
       </c>
       <c r="L28" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
       </c>
       <c r="M28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater</v>
       </c>
       <c r="N28" t="str">
         <v>null</v>
@@ -2852,7 +2852,7 @@
         <v>som</v>
       </c>
       <c r="P28" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q28" t="str">
         <v>null</v>
@@ -2896,10 +2896,10 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspoelwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_9</v>
       </c>
       <c r="B29" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C29" t="str">
         <v>null</v>
@@ -2908,49 +2908,49 @@
         <v>null</v>
       </c>
       <c r="E29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="F29" t="str">
-        <v>Biobedspoelwaterproductie</v>
+        <v>Geleidbaarheid waswater &gt; maximale waarde (S2 systeem)</v>
       </c>
       <c r="G29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
       </c>
       <c r="H29" t="str">
-        <v>null</v>
+        <v>Boven maximum grenswaarde</v>
       </c>
       <c r="I29" t="str">
-        <v>null</v>
+        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.</v>
       </c>
       <c r="J29" t="str">
-        <v>null</v>
+        <v>De geleidbaarheid is groter dan de maximale operationele waarde die op de technische fiche vermeld staat.|&gt; waarde technische fiche</v>
       </c>
       <c r="K29" t="str">
-        <v>null</v>
+        <v>&gt; waarde technische fiche</v>
       </c>
       <c r="L29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
       </c>
       <c r="M29" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="N29" t="str">
         <v>null</v>
       </c>
       <c r="O29" t="str">
-        <v>null</v>
+        <v>som</v>
       </c>
       <c r="P29" t="str">
-        <v>null</v>
+        <v>0</v>
       </c>
       <c r="Q29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/waswater</v>
+        <v>null</v>
       </c>
       <c r="R29" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Volume</v>
+        <v>null</v>
       </c>
       <c r="S29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
+        <v>null</v>
       </c>
       <c r="T29" t="str">
         <v>null</v>
@@ -2985,7 +2985,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspoelwaterproductie</v>
       </c>
       <c r="B30" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -3000,7 +3000,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
       </c>
       <c r="F30" t="str">
-        <v>Biobedspuiwaterproductie</v>
+        <v>Biobedspoelwaterproductie</v>
       </c>
       <c r="G30" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
@@ -3033,13 +3033,13 @@
         <v>null</v>
       </c>
       <c r="Q30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/spuiwater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/waswater</v>
       </c>
       <c r="R30" t="str">
         <v>http://qudt.org/vocab/quantitykind/Volume</v>
       </c>
       <c r="S30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0050</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
       </c>
       <c r="T30" t="str">
         <v>null</v>
@@ -3074,7 +3074,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspuiwaterproductie</v>
       </c>
       <c r="B31" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -3089,7 +3089,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
       </c>
       <c r="F31" t="str">
-        <v>Drukval over het systeem</v>
+        <v>Biobedspuiwaterproductie</v>
       </c>
       <c r="G31" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
@@ -3107,7 +3107,7 @@
         <v>null</v>
       </c>
       <c r="L31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
       </c>
       <c r="M31" t="str">
         <v>null</v>
@@ -3122,13 +3122,13 @@
         <v>null</v>
       </c>
       <c r="Q31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/lucht</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/spuiwater</v>
       </c>
       <c r="R31" t="str">
-        <v>http://qudt.org/vocab/quantitykind/VaporPressure</v>
+        <v>http://qudt.org/vocab/quantitykind/Volume</v>
       </c>
       <c r="S31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0329</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0050</v>
       </c>
       <c r="T31" t="str">
         <v>null</v>
@@ -3163,7 +3163,7 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
       </c>
       <c r="B32" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -3178,7 +3178,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
       </c>
       <c r="F32" t="str">
-        <v>Geleidbaarheid van het waswater</v>
+        <v>Drukval over het systeem</v>
       </c>
       <c r="G32" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
@@ -3196,7 +3196,7 @@
         <v>null</v>
       </c>
       <c r="L32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M32" t="str">
         <v>null</v>
@@ -3211,13 +3211,13 @@
         <v>null</v>
       </c>
       <c r="Q32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/waswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/lucht</v>
       </c>
       <c r="R32" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Conductivity</v>
+        <v>http://qudt.org/vocab/quantitykind/VaporPressure</v>
       </c>
       <c r="S32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0010</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0329</v>
       </c>
       <c r="T32" t="str">
         <v>null</v>
@@ -3252,7 +3252,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/elektriciteitsverbruikwaterpompen</v>
       </c>
       <c r="B33" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -3267,7 +3267,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
       </c>
       <c r="F33" t="str">
-        <v>Spuiwaterproductie</v>
+        <v>Elektriciteitsverbruik van de waswaterpomp(en)</v>
       </c>
       <c r="G33" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
@@ -3285,7 +3285,7 @@
         <v>null</v>
       </c>
       <c r="L33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/lelysphere</v>
       </c>
       <c r="M33" t="str">
         <v>null</v>
@@ -3300,13 +3300,13 @@
         <v>null</v>
       </c>
       <c r="Q33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/spuiwater</v>
+        <v>null</v>
       </c>
       <c r="R33" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Volume</v>
+        <v>http://qudt.org/vocab/quantitykind/Energy</v>
       </c>
       <c r="S33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0050</v>
+        <v>null</v>
       </c>
       <c r="T33" t="str">
         <v>null</v>
@@ -3341,7 +3341,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/stalbezetting</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="B34" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -3356,7 +3356,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
       </c>
       <c r="F34" t="str">
-        <v>Stalbezetting</v>
+        <v>Geleidbaarheid van het waswater</v>
       </c>
       <c r="G34" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
@@ -3374,7 +3374,7 @@
         <v>null</v>
       </c>
       <c r="L34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/lelysphere</v>
       </c>
       <c r="M34" t="str">
         <v>null</v>
@@ -3389,16 +3389,16 @@
         <v>null</v>
       </c>
       <c r="Q34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/stal</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/waswater</v>
       </c>
       <c r="R34" t="str">
-        <v>null</v>
+        <v>http://qudt.org/vocab/quantitykind/Conductivity</v>
       </c>
       <c r="S34" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0010</v>
       </c>
       <c r="T34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/stalbezetting</v>
+        <v>null</v>
       </c>
       <c r="U34" t="str">
         <v>null</v>
@@ -3430,7 +3430,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/systeemstatus</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie</v>
       </c>
       <c r="B35" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -3445,7 +3445,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
       </c>
       <c r="F35" t="str">
-        <v>SysteemStatus</v>
+        <v>Spuiwaterproductie</v>
       </c>
       <c r="G35" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
@@ -3463,7 +3463,7 @@
         <v>null</v>
       </c>
       <c r="L35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/lelysphere</v>
       </c>
       <c r="M35" t="str">
         <v>null</v>
@@ -3478,16 +3478,16 @@
         <v>null</v>
       </c>
       <c r="Q35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/hetelektronischmonitoringssysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/spuiwater</v>
       </c>
       <c r="R35" t="str">
-        <v>null</v>
+        <v>http://qudt.org/vocab/quantitykind/Volume</v>
       </c>
       <c r="S35" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0050</v>
       </c>
       <c r="T35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
+        <v>null</v>
       </c>
       <c r="U35" t="str">
         <v>null</v>
@@ -3519,7 +3519,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/stalbezetting</v>
       </c>
       <c r="B36" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -3534,7 +3534,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
       </c>
       <c r="F36" t="str">
-        <v>Waswaterdebiet over het waspakket</v>
+        <v>Stalbezetting</v>
       </c>
       <c r="G36" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
@@ -3552,7 +3552,7 @@
         <v>null</v>
       </c>
       <c r="L36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M36" t="str">
         <v>null</v>
@@ -3567,16 +3567,16 @@
         <v>null</v>
       </c>
       <c r="Q36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/waswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/stal</v>
       </c>
       <c r="R36" t="str">
-        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate</v>
+        <v>null</v>
       </c>
       <c r="S36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
+        <v>null</v>
       </c>
       <c r="T36" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/stalbezetting</v>
       </c>
       <c r="U36" t="str">
         <v>null</v>
@@ -3608,7 +3608,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietbevloeiing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/systeemstatus</v>
       </c>
       <c r="B37" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -3623,7 +3623,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
       </c>
       <c r="F37" t="str">
-        <v>Waswaterdebiet van de bevloeiing van het vulmateriaal</v>
+        <v>SysteemStatus</v>
       </c>
       <c r="G37" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
@@ -3641,7 +3641,7 @@
         <v>null</v>
       </c>
       <c r="L37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M37" t="str">
         <v>null</v>
@@ -3656,16 +3656,16 @@
         <v>null</v>
       </c>
       <c r="Q37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/waswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/hetelektronischmonitoringssysteem</v>
       </c>
       <c r="R37" t="str">
-        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate</v>
+        <v>null</v>
       </c>
       <c r="S37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
+        <v>null</v>
       </c>
       <c r="T37" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
       </c>
       <c r="U37" t="str">
         <v>null</v>
@@ -3697,7 +3697,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietvoorbevochtiging</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet</v>
       </c>
       <c r="B38" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -3712,7 +3712,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
       </c>
       <c r="F38" t="str">
-        <v>Waswaterdebiet van de voorbevochtiging van de ingaande stallucht</v>
+        <v>Waswaterdebiet over het waspakket</v>
       </c>
       <c r="G38" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
@@ -3730,7 +3730,7 @@
         <v>null</v>
       </c>
       <c r="L38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/lelysphere</v>
       </c>
       <c r="M38" t="str">
         <v>null</v>
@@ -3786,7 +3786,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietbevloeiing</v>
       </c>
       <c r="B39" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
@@ -3801,7 +3801,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
       </c>
       <c r="F39" t="str">
-        <v>Zuurtegraad van het waswater</v>
+        <v>Waswaterdebiet van de bevloeiing van het vulmateriaal</v>
       </c>
       <c r="G39" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
@@ -3819,7 +3819,7 @@
         <v>null</v>
       </c>
       <c r="L39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
       </c>
       <c r="M39" t="str">
         <v>null</v>
@@ -3837,10 +3837,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/waswater</v>
       </c>
       <c r="R39" t="str">
-        <v>http://qudt.org/vocab/quantitykind/Acidity</v>
+        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate</v>
       </c>
       <c r="S39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0076</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
       </c>
       <c r="T39" t="str">
         <v>null</v>
@@ -3875,10 +3875,10 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietvoorbevochtiging</v>
       </c>
       <c r="B40" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
       </c>
       <c r="C40" t="str">
         <v>null</v>
@@ -3887,13 +3887,13 @@
         <v>null</v>
       </c>
       <c r="E40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
       </c>
       <c r="F40" t="str">
-        <v>Zuurtegraad waswater S1 systeem</v>
+        <v>Waswaterdebiet van de voorbevochtiging van de ingaande stallucht</v>
       </c>
       <c r="G40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
       </c>
       <c r="H40" t="str">
         <v>null</v>
@@ -3908,10 +3908,10 @@
         <v>null</v>
       </c>
       <c r="L40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
       </c>
       <c r="M40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater</v>
+        <v>null</v>
       </c>
       <c r="N40" t="str">
         <v>null</v>
@@ -3923,19 +3923,19 @@
         <v>null</v>
       </c>
       <c r="Q40" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/waswater</v>
       </c>
       <c r="R40" t="str">
-        <v>null</v>
+        <v>http://qudt.org/vocab/quantitykind/VolumeFlowRate</v>
       </c>
       <c r="S40" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0053</v>
       </c>
       <c r="T40" t="str">
         <v>null</v>
       </c>
       <c r="U40" t="str">
-        <v>false</v>
+        <v>null</v>
       </c>
       <c r="V40" t="str">
         <v>null</v>
@@ -3964,10 +3964,10 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_10</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater</v>
       </c>
       <c r="B41" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept|http://www.w3.org/ns/ssn/Property</v>
       </c>
       <c r="C41" t="str">
         <v>null</v>
@@ -3976,13 +3976,13 @@
         <v>null</v>
       </c>
       <c r="E41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
       </c>
       <c r="F41" t="str">
-        <v>Drukval S2 systeem</v>
+        <v>Zuurtegraad van het waswater</v>
       </c>
       <c r="G41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
       </c>
       <c r="H41" t="str">
         <v>null</v>
@@ -3997,10 +3997,10 @@
         <v>null</v>
       </c>
       <c r="L41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
+        <v>null</v>
       </c>
       <c r="N41" t="str">
         <v>null</v>
@@ -4012,22 +4012,22 @@
         <v>null</v>
       </c>
       <c r="Q41" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/waswater</v>
       </c>
       <c r="R41" t="str">
-        <v>null</v>
+        <v>http://qudt.org/vocab/quantitykind/Acidity</v>
       </c>
       <c r="S41" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/fysico-chemisch/0076</v>
       </c>
       <c r="T41" t="str">
         <v>null</v>
       </c>
       <c r="U41" t="str">
-        <v>true</v>
+        <v>null</v>
       </c>
       <c r="V41" t="str">
-        <v>exact</v>
+        <v>null</v>
       </c>
       <c r="W41" t="str">
         <v>null</v>
@@ -4053,7 +4053,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_11</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_1</v>
       </c>
       <c r="B42" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4068,7 +4068,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F42" t="str">
-        <v>Waswaterdebiet voorbevochtiging S3 systeem</v>
+        <v>Zuurtegraad waswater S1 systeem</v>
       </c>
       <c r="G42" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
@@ -4086,19 +4086,19 @@
         <v>null</v>
       </c>
       <c r="L42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietvoorbevochtiging</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater</v>
       </c>
       <c r="N42" t="str">
-        <v>null</v>
+        <v>8.5</v>
       </c>
       <c r="O42" t="str">
         <v>null</v>
       </c>
       <c r="P42" t="str">
-        <v>null</v>
+        <v>6</v>
       </c>
       <c r="Q42" t="str">
         <v>null</v>
@@ -4113,10 +4113,10 @@
         <v>null</v>
       </c>
       <c r="U42" t="str">
+        <v>maximum</v>
+      </c>
+      <c r="V42" t="str">
         <v>true</v>
-      </c>
-      <c r="V42" t="str">
-        <v>minimum</v>
       </c>
       <c r="W42" t="str">
         <v>null</v>
@@ -4142,7 +4142,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_12</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_10</v>
       </c>
       <c r="B43" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4157,7 +4157,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F43" t="str">
-        <v>Waswaterdebiet bevloeiing S3 systeem</v>
+        <v>Drukval S2 systeem</v>
       </c>
       <c r="G43" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
@@ -4175,19 +4175,19 @@
         <v>null</v>
       </c>
       <c r="L43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
       </c>
       <c r="M43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietbevloeiing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
       </c>
       <c r="N43" t="str">
-        <v>null</v>
+        <v>500</v>
       </c>
       <c r="O43" t="str">
         <v>null</v>
       </c>
       <c r="P43" t="str">
-        <v>null</v>
+        <v>0</v>
       </c>
       <c r="Q43" t="str">
         <v>null</v>
@@ -4202,10 +4202,10 @@
         <v>null</v>
       </c>
       <c r="U43" t="str">
+        <v>exact</v>
+      </c>
+      <c r="V43" t="str">
         <v>true</v>
-      </c>
-      <c r="V43" t="str">
-        <v>minimum</v>
       </c>
       <c r="W43" t="str">
         <v>null</v>
@@ -4231,7 +4231,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_13</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_11</v>
       </c>
       <c r="B44" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4246,7 +4246,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F44" t="str">
-        <v>Biobedspuiwaterproductie S3 systeem</v>
+        <v>Waswaterdebiet voorbevochtiging S3 systeem</v>
       </c>
       <c r="G44" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
@@ -4267,7 +4267,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
       </c>
       <c r="M44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietvoorbevochtiging</v>
       </c>
       <c r="N44" t="str">
         <v>null</v>
@@ -4291,10 +4291,10 @@
         <v>null</v>
       </c>
       <c r="U44" t="str">
+        <v>minimum</v>
+      </c>
+      <c r="V44" t="str">
         <v>true</v>
-      </c>
-      <c r="V44" t="str">
-        <v>minimum</v>
       </c>
       <c r="W44" t="str">
         <v>null</v>
@@ -4320,7 +4320,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_14</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_12</v>
       </c>
       <c r="B45" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4335,7 +4335,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F45" t="str">
-        <v>Biobedspoelwaterproductie S3 systeem</v>
+        <v>Waswaterdebiet bevloeiing S3 systeem</v>
       </c>
       <c r="G45" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
@@ -4356,7 +4356,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
       </c>
       <c r="M45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspoelwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietbevloeiing</v>
       </c>
       <c r="N45" t="str">
         <v>null</v>
@@ -4380,10 +4380,10 @@
         <v>null</v>
       </c>
       <c r="U45" t="str">
+        <v>minimum</v>
+      </c>
+      <c r="V45" t="str">
         <v>true</v>
-      </c>
-      <c r="V45" t="str">
-        <v>minimum</v>
       </c>
       <c r="W45" t="str">
         <v>null</v>
@@ -4409,7 +4409,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_15</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_13</v>
       </c>
       <c r="B46" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4424,7 +4424,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F46" t="str">
-        <v>Drukval S3 systeem</v>
+        <v>Biobedspuiwaterproductie S3 systeem</v>
       </c>
       <c r="G46" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
@@ -4445,7 +4445,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
       </c>
       <c r="M46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspuiwaterproductie</v>
       </c>
       <c r="N46" t="str">
         <v>null</v>
@@ -4469,10 +4469,10 @@
         <v>null</v>
       </c>
       <c r="U46" t="str">
+        <v>minimum</v>
+      </c>
+      <c r="V46" t="str">
         <v>true</v>
-      </c>
-      <c r="V46" t="str">
-        <v>maximum</v>
       </c>
       <c r="W46" t="str">
         <v>null</v>
@@ -4498,7 +4498,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_14</v>
       </c>
       <c r="B47" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4513,7 +4513,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F47" t="str">
-        <v>Geleidbaarheid waswater S1 systeem</v>
+        <v>Biobedspoelwaterproductie S3 systeem</v>
       </c>
       <c r="G47" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
@@ -4531,10 +4531,10 @@
         <v>null</v>
       </c>
       <c r="L47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
       </c>
       <c r="M47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspoelwaterproductie</v>
       </c>
       <c r="N47" t="str">
         <v>null</v>
@@ -4558,10 +4558,10 @@
         <v>null</v>
       </c>
       <c r="U47" t="str">
+        <v>minimum</v>
+      </c>
+      <c r="V47" t="str">
         <v>true</v>
-      </c>
-      <c r="V47" t="str">
-        <v>maximum</v>
       </c>
       <c r="W47" t="str">
         <v>null</v>
@@ -4587,7 +4587,7 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_15</v>
       </c>
       <c r="B48" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4602,7 +4602,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F48" t="str">
-        <v>Waswaterdebiet S1 systeem</v>
+        <v>Drukval S3 systeem</v>
       </c>
       <c r="G48" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
@@ -4620,19 +4620,19 @@
         <v>null</v>
       </c>
       <c r="L48" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
       </c>
       <c r="M48" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
       </c>
       <c r="N48" t="str">
-        <v>null</v>
+        <v>500</v>
       </c>
       <c r="O48" t="str">
         <v>null</v>
       </c>
       <c r="P48" t="str">
-        <v>null</v>
+        <v>0</v>
       </c>
       <c r="Q48" t="str">
         <v>null</v>
@@ -4647,10 +4647,10 @@
         <v>null</v>
       </c>
       <c r="U48" t="str">
+        <v>maximum</v>
+      </c>
+      <c r="V48" t="str">
         <v>true</v>
-      </c>
-      <c r="V48" t="str">
-        <v>minimum</v>
       </c>
       <c r="W48" t="str">
         <v>null</v>
@@ -4676,7 +4676,7 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_4</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_16</v>
       </c>
       <c r="B49" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4691,7 +4691,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F49" t="str">
-        <v>Spuiwaterdebiet S1 systeem</v>
+        <v>Geleidbaarheid waswater Lely Sphere systeem</v>
       </c>
       <c r="G49" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
@@ -4709,10 +4709,10 @@
         <v>null</v>
       </c>
       <c r="L49" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/lelysphere</v>
       </c>
       <c r="M49" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="N49" t="str">
         <v>null</v>
@@ -4736,10 +4736,10 @@
         <v>null</v>
       </c>
       <c r="U49" t="str">
+        <v>maximum</v>
+      </c>
+      <c r="V49" t="str">
         <v>true</v>
-      </c>
-      <c r="V49" t="str">
-        <v>minimum</v>
       </c>
       <c r="W49" t="str">
         <v>null</v>
@@ -4765,7 +4765,7 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_5</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_17</v>
       </c>
       <c r="B50" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4780,7 +4780,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F50" t="str">
-        <v>Drukval S1 systeem</v>
+        <v>Waswaterdebiet Lely Sphere systeem</v>
       </c>
       <c r="G50" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
@@ -4798,10 +4798,10 @@
         <v>null</v>
       </c>
       <c r="L50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/lelysphere</v>
       </c>
       <c r="M50" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet</v>
       </c>
       <c r="N50" t="str">
         <v>null</v>
@@ -4825,10 +4825,10 @@
         <v>null</v>
       </c>
       <c r="U50" t="str">
+        <v>minimum</v>
+      </c>
+      <c r="V50" t="str">
         <v>true</v>
-      </c>
-      <c r="V50" t="str">
-        <v>exact</v>
       </c>
       <c r="W50" t="str">
         <v>null</v>
@@ -4854,7 +4854,7 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_6</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_18</v>
       </c>
       <c r="B51" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4869,7 +4869,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F51" t="str">
-        <v>Zuurtegraad waswater S2 systeem</v>
+        <v>Spuiwaterdebiet Lely Sphere systeem</v>
       </c>
       <c r="G51" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
@@ -4887,10 +4887,10 @@
         <v>null</v>
       </c>
       <c r="L51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/lelysphere</v>
       </c>
       <c r="M51" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie</v>
       </c>
       <c r="N51" t="str">
         <v>null</v>
@@ -4914,10 +4914,10 @@
         <v>null</v>
       </c>
       <c r="U51" t="str">
+        <v>minimum</v>
+      </c>
+      <c r="V51" t="str">
         <v>true</v>
-      </c>
-      <c r="V51" t="str">
-        <v>maximum</v>
       </c>
       <c r="W51" t="str">
         <v>null</v>
@@ -4943,7 +4943,7 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_7</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_19</v>
       </c>
       <c r="B52" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -4958,7 +4958,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F52" t="str">
-        <v>Geleidbaarheid waswater S2 systeem</v>
+        <v>Elektriciteitsverbruik van de waswaterpomp(en) Lely Sphere systeem</v>
       </c>
       <c r="G52" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
@@ -4976,10 +4976,10 @@
         <v>null</v>
       </c>
       <c r="L52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/lelysphere</v>
       </c>
       <c r="M52" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/elektriciteitsverbruikwaterpompen</v>
       </c>
       <c r="N52" t="str">
         <v>null</v>
@@ -5003,10 +5003,10 @@
         <v>null</v>
       </c>
       <c r="U52" t="str">
+        <v>minimum</v>
+      </c>
+      <c r="V52" t="str">
         <v>true</v>
-      </c>
-      <c r="V52" t="str">
-        <v>maximum</v>
       </c>
       <c r="W52" t="str">
         <v>null</v>
@@ -5032,7 +5032,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_8</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_2</v>
       </c>
       <c r="B53" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5047,7 +5047,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F53" t="str">
-        <v>Waswaterdebiet S2 systeem</v>
+        <v>Geleidbaarheid waswater S1 systeem</v>
       </c>
       <c r="G53" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
@@ -5065,19 +5065,19 @@
         <v>null</v>
       </c>
       <c r="L53" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M53" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="N53" t="str">
-        <v>null</v>
+        <v>30</v>
       </c>
       <c r="O53" t="str">
         <v>null</v>
       </c>
       <c r="P53" t="str">
-        <v>null</v>
+        <v>0</v>
       </c>
       <c r="Q53" t="str">
         <v>null</v>
@@ -5092,10 +5092,10 @@
         <v>null</v>
       </c>
       <c r="U53" t="str">
+        <v>maximum</v>
+      </c>
+      <c r="V53" t="str">
         <v>true</v>
-      </c>
-      <c r="V53" t="str">
-        <v>minimum</v>
       </c>
       <c r="W53" t="str">
         <v>null</v>
@@ -5121,7 +5121,7 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_9</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_3</v>
       </c>
       <c r="B54" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5136,7 +5136,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F54" t="str">
-        <v>Spuiwaterdebiet S2 systeem</v>
+        <v>Waswaterdebiet S1 systeem</v>
       </c>
       <c r="G54" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
@@ -5154,10 +5154,10 @@
         <v>null</v>
       </c>
       <c r="L54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M54" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet</v>
       </c>
       <c r="N54" t="str">
         <v>null</v>
@@ -5181,10 +5181,10 @@
         <v>null</v>
       </c>
       <c r="U54" t="str">
+        <v>minimum</v>
+      </c>
+      <c r="V54" t="str">
         <v>true</v>
-      </c>
-      <c r="V54" t="str">
-        <v>minimum</v>
       </c>
       <c r="W54" t="str">
         <v>null</v>
@@ -5210,7 +5210,7 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/stalbezetting/in_gebruik</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_4</v>
       </c>
       <c r="B55" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5222,13 +5222,13 @@
         <v>null</v>
       </c>
       <c r="E55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/stalbezetting</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F55" t="str">
-        <v>Stal in gebruik, dieren aanwezig.</v>
+        <v>Spuiwaterdebiet S1 systeem</v>
       </c>
       <c r="G55" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/stalbezetting</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="H55" t="str">
         <v>null</v>
@@ -5243,10 +5243,10 @@
         <v>null</v>
       </c>
       <c r="L55" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M55" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie</v>
       </c>
       <c r="N55" t="str">
         <v>null</v>
@@ -5270,10 +5270,10 @@
         <v>null</v>
       </c>
       <c r="U55" t="str">
-        <v>null</v>
+        <v>minimum</v>
       </c>
       <c r="V55" t="str">
-        <v>null</v>
+        <v>true</v>
       </c>
       <c r="W55" t="str">
         <v>null</v>
@@ -5299,7 +5299,7 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/stalbezetting/leeg</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_5</v>
       </c>
       <c r="B56" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5311,13 +5311,13 @@
         <v>null</v>
       </c>
       <c r="E56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/stalbezetting</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F56" t="str">
-        <v>Lege stal</v>
+        <v>Drukval S1 systeem</v>
       </c>
       <c r="G56" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/stalbezetting</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="H56" t="str">
         <v>null</v>
@@ -5332,19 +5332,19 @@
         <v>null</v>
       </c>
       <c r="L56" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="M56" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem</v>
       </c>
       <c r="N56" t="str">
-        <v>null</v>
+        <v>500</v>
       </c>
       <c r="O56" t="str">
         <v>null</v>
       </c>
       <c r="P56" t="str">
-        <v>null</v>
+        <v>0</v>
       </c>
       <c r="Q56" t="str">
         <v>null</v>
@@ -5359,10 +5359,10 @@
         <v>null</v>
       </c>
       <c r="U56" t="str">
-        <v>null</v>
+        <v>exact</v>
       </c>
       <c r="V56" t="str">
-        <v>null</v>
+        <v>true</v>
       </c>
       <c r="W56" t="str">
         <v>null</v>
@@ -5388,7 +5388,7 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/status/gereinigd</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_6</v>
       </c>
       <c r="B57" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5400,13 +5400,13 @@
         <v>null</v>
       </c>
       <c r="E57" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F57" t="str">
-        <v>Gereinigd</v>
+        <v>Zuurtegraad waswater S2 systeem</v>
       </c>
       <c r="G57" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="H57" t="str">
         <v>null</v>
@@ -5421,19 +5421,19 @@
         <v>null</v>
       </c>
       <c r="L57" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
       </c>
       <c r="M57" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater</v>
       </c>
       <c r="N57" t="str">
-        <v>null</v>
+        <v>14</v>
       </c>
       <c r="O57" t="str">
         <v>null</v>
       </c>
       <c r="P57" t="str">
-        <v>null</v>
+        <v>0</v>
       </c>
       <c r="Q57" t="str">
         <v>null</v>
@@ -5448,10 +5448,10 @@
         <v>null</v>
       </c>
       <c r="U57" t="str">
-        <v>null</v>
+        <v>maximum</v>
       </c>
       <c r="V57" t="str">
-        <v>null</v>
+        <v>true</v>
       </c>
       <c r="W57" t="str">
         <v>null</v>
@@ -5477,7 +5477,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/status/onderhoud</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_7</v>
       </c>
       <c r="B58" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5489,13 +5489,13 @@
         <v>null</v>
       </c>
       <c r="E58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F58" t="str">
-        <v>In onderhoud</v>
+        <v>Geleidbaarheid waswater S2 systeem</v>
       </c>
       <c r="G58" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="H58" t="str">
         <v>null</v>
@@ -5510,19 +5510,19 @@
         <v>null</v>
       </c>
       <c r="L58" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
       </c>
       <c r="M58" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater</v>
       </c>
       <c r="N58" t="str">
-        <v>null</v>
+        <v>500</v>
       </c>
       <c r="O58" t="str">
         <v>null</v>
       </c>
       <c r="P58" t="str">
-        <v>null</v>
+        <v>0</v>
       </c>
       <c r="Q58" t="str">
         <v>null</v>
@@ -5537,10 +5537,10 @@
         <v>null</v>
       </c>
       <c r="U58" t="str">
-        <v>null</v>
+        <v>maximum</v>
       </c>
       <c r="V58" t="str">
-        <v>null</v>
+        <v>true</v>
       </c>
       <c r="W58" t="str">
         <v>null</v>
@@ -5566,7 +5566,7 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/status/operationeel</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_8</v>
       </c>
       <c r="B59" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5578,13 +5578,13 @@
         <v>null</v>
       </c>
       <c r="E59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F59" t="str">
-        <v>Operationeel</v>
+        <v>Waswaterdebiet S2 systeem</v>
       </c>
       <c r="G59" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="H59" t="str">
         <v>null</v>
@@ -5599,10 +5599,10 @@
         <v>null</v>
       </c>
       <c r="L59" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
       </c>
       <c r="M59" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet</v>
       </c>
       <c r="N59" t="str">
         <v>null</v>
@@ -5626,10 +5626,10 @@
         <v>null</v>
       </c>
       <c r="U59" t="str">
-        <v>null</v>
+        <v>minimum</v>
       </c>
       <c r="V59" t="str">
-        <v>null</v>
+        <v>true</v>
       </c>
       <c r="W59" t="str">
         <v>null</v>
@@ -5655,7 +5655,7 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/status/storing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_9</v>
       </c>
       <c r="B60" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5667,13 +5667,13 @@
         <v>null</v>
       </c>
       <c r="E60" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="F60" t="str">
-        <v>Storing</v>
+        <v>Spuiwaterdebiet S2 systeem</v>
       </c>
       <c r="G60" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
       </c>
       <c r="H60" t="str">
         <v>null</v>
@@ -5688,10 +5688,10 @@
         <v>null</v>
       </c>
       <c r="L60" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
       </c>
       <c r="M60" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie</v>
       </c>
       <c r="N60" t="str">
         <v>null</v>
@@ -5715,10 +5715,10 @@
         <v>null</v>
       </c>
       <c r="U60" t="str">
-        <v>null</v>
+        <v>minimum</v>
       </c>
       <c r="V60" t="str">
-        <v>null</v>
+        <v>true</v>
       </c>
       <c r="W60" t="str">
         <v>null</v>
@@ -5744,7 +5744,7 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/stalbezetting/in_gebruik</v>
       </c>
       <c r="B61" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5756,13 +5756,13 @@
         <v>null</v>
       </c>
       <c r="E61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/stalbezetting</v>
       </c>
       <c r="F61" t="str">
-        <v>Luchtwassysteem</v>
+        <v>Stal in gebruik, dieren aanwezig.</v>
       </c>
       <c r="G61" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/stalbezetting</v>
       </c>
       <c r="H61" t="str">
         <v>null</v>
@@ -5810,19 +5810,19 @@
         <v>null</v>
       </c>
       <c r="W61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="X61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="Y61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>null</v>
       </c>
       <c r="Z61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>null</v>
       </c>
       <c r="AA61" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="AB61" t="str">
         <v>null</v>
@@ -5833,7 +5833,7 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/stalbezetting/leeg</v>
       </c>
       <c r="B62" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5845,13 +5845,13 @@
         <v>null</v>
       </c>
       <c r="E62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/stalbezetting</v>
       </c>
       <c r="F62" t="str">
-        <v>Luchtzuiveringssysteem</v>
+        <v>Lege stal</v>
       </c>
       <c r="G62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/stalbezetting</v>
       </c>
       <c r="H62" t="str">
         <v>null</v>
@@ -5905,13 +5905,13 @@
         <v>null</v>
       </c>
       <c r="Y62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="Z62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="AA62" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="AB62" t="str">
         <v>null</v>
@@ -5922,7 +5922,7 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/status/gereinigd</v>
       </c>
       <c r="B63" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -5934,13 +5934,13 @@
         <v>null</v>
       </c>
       <c r="E63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
       </c>
       <c r="F63" t="str">
-        <v>Biologisch luchtwassysteem</v>
+        <v>Gereinigd</v>
       </c>
       <c r="G63" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
       </c>
       <c r="H63" t="str">
         <v>null</v>
@@ -5958,7 +5958,7 @@
         <v>null</v>
       </c>
       <c r="M63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/systeemstatus</v>
+        <v>null</v>
       </c>
       <c r="N63" t="str">
         <v>null</v>
@@ -5988,10 +5988,10 @@
         <v>null</v>
       </c>
       <c r="W63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="X63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="Y63" t="str">
         <v>null</v>
@@ -6000,10 +6000,10 @@
         <v>null</v>
       </c>
       <c r="AA63" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="AB63" t="str">
-        <v>S1</v>
+        <v>null</v>
       </c>
       <c r="AC63" t="str">
         <v>null</v>
@@ -6011,7 +6011,7 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/status/onderhoud</v>
       </c>
       <c r="B64" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -6023,13 +6023,13 @@
         <v>null</v>
       </c>
       <c r="E64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
       </c>
       <c r="F64" t="str">
-        <v>Chemisch luchtwassysteem</v>
+        <v>In onderhoud</v>
       </c>
       <c r="G64" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
       </c>
       <c r="H64" t="str">
         <v>null</v>
@@ -6047,7 +6047,7 @@
         <v>null</v>
       </c>
       <c r="M64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/systeemstatus</v>
+        <v>null</v>
       </c>
       <c r="N64" t="str">
         <v>null</v>
@@ -6077,10 +6077,10 @@
         <v>null</v>
       </c>
       <c r="W64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem</v>
+        <v>null</v>
       </c>
       <c r="X64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="Y64" t="str">
         <v>null</v>
@@ -6089,10 +6089,10 @@
         <v>null</v>
       </c>
       <c r="AA64" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="AB64" t="str">
-        <v>S2</v>
+        <v>null</v>
       </c>
       <c r="AC64" t="str">
         <v>null</v>
@@ -6100,7 +6100,7 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/status/operationeel</v>
       </c>
       <c r="B65" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -6112,13 +6112,13 @@
         <v>null</v>
       </c>
       <c r="E65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
       </c>
       <c r="F65" t="str">
-        <v>Biobed</v>
+        <v>Operationeel</v>
       </c>
       <c r="G65" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
       </c>
       <c r="H65" t="str">
         <v>null</v>
@@ -6136,7 +6136,7 @@
         <v>null</v>
       </c>
       <c r="M65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietvoorbevochtiging|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietbevloeiing|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspoelwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/systeemstatus</v>
+        <v>null</v>
       </c>
       <c r="N65" t="str">
         <v>null</v>
@@ -6166,10 +6166,10 @@
         <v>null</v>
       </c>
       <c r="W65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="X65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="Y65" t="str">
         <v>null</v>
@@ -6178,10 +6178,10 @@
         <v>null</v>
       </c>
       <c r="AA65" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
       <c r="AB65" t="str">
-        <v>S3</v>
+        <v>null</v>
       </c>
       <c r="AC65" t="str">
         <v>null</v>
@@ -6189,7 +6189,7 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k1</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/status/storing</v>
       </c>
       <c r="B66" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -6198,25 +6198,25 @@
         <v>null</v>
       </c>
       <c r="D66" t="str">
-        <v>VLAREM klasse 1</v>
+        <v>null</v>
       </c>
       <c r="E66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
       </c>
       <c r="F66" t="str">
-        <v>Klasse 1</v>
+        <v>Storing</v>
       </c>
       <c r="G66" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
       </c>
       <c r="H66" t="str">
         <v>null</v>
       </c>
       <c r="I66" t="str">
-        <v>Indelingsklasse voor inrichtingen met de grootste milieu-impact. Voor deze activiteiten geldt een omgevingsvergunning klasse 1 (zwaarste procedure).</v>
+        <v>null</v>
       </c>
       <c r="J66" t="str">
-        <v>Indelingsklasse voor inrichtingen met de grootste milieu-impact. Voor deze activiteiten geldt een omgevingsvergunning klasse 1 (zwaarste procedure).</v>
+        <v>null</v>
       </c>
       <c r="K66" t="str">
         <v>null</v>
@@ -6278,7 +6278,7 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/lelysphere</v>
       </c>
       <c r="B67" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -6287,25 +6287,25 @@
         <v>null</v>
       </c>
       <c r="D67" t="str">
-        <v>VLAREM klasse 2</v>
+        <v>null</v>
       </c>
       <c r="E67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
       </c>
       <c r="F67" t="str">
-        <v>Klasse 2</v>
+        <v>Lely Sphere</v>
       </c>
       <c r="G67" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
+        <v>null</v>
       </c>
       <c r="H67" t="str">
         <v>null</v>
       </c>
       <c r="I67" t="str">
-        <v>Indelingsklasse voor inrichtingen met een middelgrote milieu-impact. Voor deze activiteiten geldt een omgevingsvergunning klasse 2.</v>
+        <v>null</v>
       </c>
       <c r="J67" t="str">
-        <v>Indelingsklasse voor inrichtingen met een middelgrote milieu-impact. Voor deze activiteiten geldt een omgevingsvergunning klasse 2.</v>
+        <v>null</v>
       </c>
       <c r="K67" t="str">
         <v>null</v>
@@ -6314,7 +6314,7 @@
         <v>null</v>
       </c>
       <c r="M67" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/elektriciteitsverbruikwaterpompen</v>
       </c>
       <c r="N67" t="str">
         <v>null</v>
@@ -6344,16 +6344,16 @@
         <v>null</v>
       </c>
       <c r="W67" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem</v>
       </c>
       <c r="X67" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
       </c>
       <c r="Y67" t="str">
-        <v>null</v>
+        <v>Lelysphere</v>
       </c>
       <c r="Z67" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
       </c>
       <c r="AA67" t="str">
         <v>null</v>
@@ -6367,7 +6367,7 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k3</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem</v>
       </c>
       <c r="B68" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -6376,25 +6376,25 @@
         <v>null</v>
       </c>
       <c r="D68" t="str">
-        <v>VLAREM klasse 3</v>
+        <v>null</v>
       </c>
       <c r="E68" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
       </c>
       <c r="F68" t="str">
-        <v>Klasse 3</v>
+        <v>Luchtwassysteem</v>
       </c>
       <c r="G68" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
+        <v>null</v>
       </c>
       <c r="H68" t="str">
         <v>null</v>
       </c>
       <c r="I68" t="str">
-        <v>Indelingsklasse voor inrichtingen met een beperkte milieu-impact. Voor deze activiteiten geldt een meldingsplicht (klasse 3).</v>
+        <v>null</v>
       </c>
       <c r="J68" t="str">
-        <v>Indelingsklasse voor inrichtingen met een beperkte milieu-impact. Voor deze activiteiten geldt een meldingsplicht (klasse 3).</v>
+        <v>null</v>
       </c>
       <c r="K68" t="str">
         <v>null</v>
@@ -6433,22 +6433,22 @@
         <v>null</v>
       </c>
       <c r="W68" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
       </c>
       <c r="X68" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
       </c>
       <c r="Y68" t="str">
         <v>null</v>
       </c>
       <c r="Z68" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/lelysphere|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
       </c>
       <c r="AA68" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/lelysphere</v>
       </c>
       <c r="AB68" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/lelysphere</v>
       </c>
       <c r="AC68" t="str">
         <v>null</v>
@@ -6456,10 +6456,10 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/medium</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
       </c>
       <c r="B69" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C69" t="str">
         <v>null</v>
@@ -6468,13 +6468,13 @@
         <v>null</v>
       </c>
       <c r="E69" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
       </c>
       <c r="F69" t="str">
-        <v>conceptschema luchtzuiveringssysteem medium</v>
+        <v>Luchtzuiveringssysteem</v>
       </c>
       <c r="G69" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
       </c>
       <c r="H69" t="str">
         <v>null</v>
@@ -6531,36 +6531,36 @@
         <v>null</v>
       </c>
       <c r="Z69" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/lelysphere|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem</v>
       </c>
       <c r="AA69" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem</v>
       </c>
       <c r="AB69" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/lelysphere|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem</v>
       </c>
       <c r="AC69" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/hetelektronischmonitoringssysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/lucht|https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/spuiwater|https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/stal|https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/waswater</v>
+        <v>null</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s1</v>
       </c>
       <c r="B70" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C70" t="str">
         <v>null</v>
       </c>
       <c r="D70" t="str">
-        <v>Ranges</v>
+        <v>null</v>
       </c>
       <c r="E70" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
       </c>
       <c r="F70" t="str">
-        <v>conceptschema luchtzuiveringssysteem normbandbreedte</v>
+        <v>Biologisch luchtwassysteem</v>
       </c>
       <c r="G70" t="str">
         <v>null</v>
@@ -6581,7 +6581,7 @@
         <v>null</v>
       </c>
       <c r="M70" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/systeemstatus</v>
       </c>
       <c r="N70" t="str">
         <v>null</v>
@@ -6611,16 +6611,16 @@
         <v>null</v>
       </c>
       <c r="W70" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem</v>
       </c>
       <c r="X70" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
       </c>
       <c r="Y70" t="str">
-        <v>null</v>
+        <v>S1</v>
       </c>
       <c r="Z70" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
       </c>
       <c r="AA70" t="str">
         <v>null</v>
@@ -6629,15 +6629,15 @@
         <v>null</v>
       </c>
       <c r="AC70" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_10|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_11|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_12|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_13|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_14|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_15|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_16|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_1|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_2|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_3|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_4|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_5|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_6|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_7|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_8|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_9</v>
+        <v>null</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s2</v>
       </c>
       <c r="B71" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C71" t="str">
         <v>null</v>
@@ -6646,10 +6646,10 @@
         <v>null</v>
       </c>
       <c r="E71" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
       </c>
       <c r="F71" t="str">
-        <v>conceptschema luchtzuiveringssysteem eigenschap</v>
+        <v>Chemisch luchtwassysteem</v>
       </c>
       <c r="G71" t="str">
         <v>null</v>
@@ -6670,7 +6670,7 @@
         <v>null</v>
       </c>
       <c r="M71" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/systeemstatus</v>
       </c>
       <c r="N71" t="str">
         <v>null</v>
@@ -6700,16 +6700,16 @@
         <v>null</v>
       </c>
       <c r="W71" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem</v>
       </c>
       <c r="X71" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
       </c>
       <c r="Y71" t="str">
-        <v>null</v>
+        <v>S2</v>
       </c>
       <c r="Z71" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtwassysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
       </c>
       <c r="AA71" t="str">
         <v>null</v>
@@ -6718,15 +6718,15 @@
         <v>null</v>
       </c>
       <c r="AC71" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietvoorbevochtiging|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietbevloeiing|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspoelwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/systeemstatus</v>
+        <v>null</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/s3</v>
       </c>
       <c r="B72" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C72" t="str">
         <v>null</v>
@@ -6735,10 +6735,10 @@
         <v>null</v>
       </c>
       <c r="E72" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
       </c>
       <c r="F72" t="str">
-        <v>conceptschema luchtzuiveringssysteem parameter specificatie</v>
+        <v>Biobed</v>
       </c>
       <c r="G72" t="str">
         <v>null</v>
@@ -6747,10 +6747,10 @@
         <v>null</v>
       </c>
       <c r="I72" t="str">
-        <v>Het schema van indelingsklassen (1, 2, 3) zoals vastgelegd in de Vlaamse milieuregelgeving (VLAREM).</v>
+        <v>null</v>
       </c>
       <c r="J72" t="str">
-        <v>Het schema van indelingsklassen (1, 2, 3) zoals vastgelegd in de Vlaamse milieuregelgeving (VLAREM).</v>
+        <v>null</v>
       </c>
       <c r="K72" t="str">
         <v>null</v>
@@ -6759,7 +6759,7 @@
         <v>null</v>
       </c>
       <c r="M72" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietvoorbevochtiging|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietbevloeiing|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspoelwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/systeemstatus</v>
       </c>
       <c r="N72" t="str">
         <v>null</v>
@@ -6789,16 +6789,16 @@
         <v>null</v>
       </c>
       <c r="W72" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
       </c>
       <c r="X72" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
       </c>
       <c r="Y72" t="str">
-        <v>null</v>
+        <v>S3</v>
       </c>
       <c r="Z72" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
       </c>
       <c r="AA72" t="str">
         <v>null</v>
@@ -6807,39 +6807,39 @@
         <v>null</v>
       </c>
       <c r="AC72" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_10|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_11|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_12|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_13|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_14|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_15|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_1|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_2|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_3|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_4|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_5|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_6|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_7|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_8|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_9</v>
+        <v>null</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/stalbezetting</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k1</v>
       </c>
       <c r="B73" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C73" t="str">
         <v>null</v>
       </c>
       <c r="D73" t="str">
-        <v>null</v>
+        <v>VLAREM klasse 1</v>
       </c>
       <c r="E73" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
       </c>
       <c r="F73" t="str">
-        <v>conceptschema luchtzuiveringssysteem stalbezetting</v>
+        <v>Klasse 1</v>
       </c>
       <c r="G73" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
       </c>
       <c r="H73" t="str">
         <v>null</v>
       </c>
       <c r="I73" t="str">
-        <v>null</v>
+        <v>Indelingsklasse voor inrichtingen met de grootste milieu-impact. Voor deze activiteiten geldt een omgevingsvergunning klasse 1 (zwaarste procedure).</v>
       </c>
       <c r="J73" t="str">
-        <v>null</v>
+        <v>Indelingsklasse voor inrichtingen met de grootste milieu-impact. Voor deze activiteiten geldt een omgevingsvergunning klasse 1 (zwaarste procedure).</v>
       </c>
       <c r="K73" t="str">
         <v>null</v>
@@ -6896,39 +6896,39 @@
         <v>null</v>
       </c>
       <c r="AC73" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/stalbezetting/in_gebruik|https://data.omgeving.vlaanderen.be/id/concept/lzs/stalbezetting/leeg</v>
+        <v>null</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k2</v>
       </c>
       <c r="B74" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C74" t="str">
         <v>null</v>
       </c>
       <c r="D74" t="str">
-        <v>null</v>
+        <v>VLAREM klasse 2</v>
       </c>
       <c r="E74" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
       </c>
       <c r="F74" t="str">
-        <v>conceptschema luchtzuiveringssysteem status</v>
+        <v>Klasse 2</v>
       </c>
       <c r="G74" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
       </c>
       <c r="H74" t="str">
         <v>null</v>
       </c>
       <c r="I74" t="str">
-        <v>null</v>
+        <v>Indelingsklasse voor inrichtingen met een middelgrote milieu-impact. Voor deze activiteiten geldt een omgevingsvergunning klasse 2.</v>
       </c>
       <c r="J74" t="str">
-        <v>null</v>
+        <v>Indelingsklasse voor inrichtingen met een middelgrote milieu-impact. Voor deze activiteiten geldt een omgevingsvergunning klasse 2.</v>
       </c>
       <c r="K74" t="str">
         <v>null</v>
@@ -6985,39 +6985,39 @@
         <v>null</v>
       </c>
       <c r="AC74" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/status/gereinigd|https://data.omgeving.vlaanderen.be/id/concept/lzs/status/onderhoud|https://data.omgeving.vlaanderen.be/id/concept/lzs/status/operationeel|https://data.omgeving.vlaanderen.be/id/concept/lzs/status/storing</v>
+        <v>null</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k3</v>
       </c>
       <c r="B75" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C75" t="str">
         <v>null</v>
       </c>
       <c r="D75" t="str">
-        <v>null</v>
+        <v>VLAREM klasse 3</v>
       </c>
       <c r="E75" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
       </c>
       <c r="F75" t="str">
-        <v>conceptschema luchtzuiveringssysteem</v>
+        <v>Klasse 3</v>
       </c>
       <c r="G75" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
       </c>
       <c r="H75" t="str">
         <v>null</v>
       </c>
       <c r="I75" t="str">
-        <v>null</v>
+        <v>Indelingsklasse voor inrichtingen met een beperkte milieu-impact. Voor deze activiteiten geldt een meldingsplicht (klasse 3).</v>
       </c>
       <c r="J75" t="str">
-        <v>null</v>
+        <v>Indelingsklasse voor inrichtingen met een beperkte milieu-impact. Voor deze activiteiten geldt een meldingsplicht (klasse 3).</v>
       </c>
       <c r="K75" t="str">
         <v>null</v>
@@ -7074,12 +7074,12 @@
         <v>null</v>
       </c>
       <c r="AC75" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
+        <v>null</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/medium</v>
       </c>
       <c r="B76" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -7094,81 +7094,704 @@
         <v>null</v>
       </c>
       <c r="F76" t="str">
+        <v>conceptschema luchtzuiveringssysteem medium</v>
+      </c>
+      <c r="G76" t="str">
+        <v>null</v>
+      </c>
+      <c r="H76" t="str">
+        <v>null</v>
+      </c>
+      <c r="I76" t="str">
+        <v>null</v>
+      </c>
+      <c r="J76" t="str">
+        <v>null</v>
+      </c>
+      <c r="K76" t="str">
+        <v>null</v>
+      </c>
+      <c r="L76" t="str">
+        <v>null</v>
+      </c>
+      <c r="M76" t="str">
+        <v>null</v>
+      </c>
+      <c r="N76" t="str">
+        <v>null</v>
+      </c>
+      <c r="O76" t="str">
+        <v>null</v>
+      </c>
+      <c r="P76" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q76" t="str">
+        <v>null</v>
+      </c>
+      <c r="R76" t="str">
+        <v>null</v>
+      </c>
+      <c r="S76" t="str">
+        <v>null</v>
+      </c>
+      <c r="T76" t="str">
+        <v>null</v>
+      </c>
+      <c r="U76" t="str">
+        <v>null</v>
+      </c>
+      <c r="V76" t="str">
+        <v>null</v>
+      </c>
+      <c r="W76" t="str">
+        <v>null</v>
+      </c>
+      <c r="X76" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y76" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z76" t="str">
+        <v>null</v>
+      </c>
+      <c r="AA76" t="str">
+        <v>null</v>
+      </c>
+      <c r="AB76" t="str">
+        <v>null</v>
+      </c>
+      <c r="AC76" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/hetelektronischmonitoringssysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/lucht|https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/spuiwater|https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/stal|https://data.omgeving.vlaanderen.be/id/concept/lzs/medium/waswater</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/norm-bandbreedte</v>
+      </c>
+      <c r="B77" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+      </c>
+      <c r="C77" t="str">
+        <v>null</v>
+      </c>
+      <c r="D77" t="str">
+        <v>Ranges</v>
+      </c>
+      <c r="E77" t="str">
+        <v>null</v>
+      </c>
+      <c r="F77" t="str">
+        <v>conceptschema luchtzuiveringssysteem normbandbreedte</v>
+      </c>
+      <c r="G77" t="str">
+        <v>null</v>
+      </c>
+      <c r="H77" t="str">
+        <v>null</v>
+      </c>
+      <c r="I77" t="str">
+        <v>null</v>
+      </c>
+      <c r="J77" t="str">
+        <v>null</v>
+      </c>
+      <c r="K77" t="str">
+        <v>null</v>
+      </c>
+      <c r="L77" t="str">
+        <v>null</v>
+      </c>
+      <c r="M77" t="str">
+        <v>null</v>
+      </c>
+      <c r="N77" t="str">
+        <v>null</v>
+      </c>
+      <c r="O77" t="str">
+        <v>null</v>
+      </c>
+      <c r="P77" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q77" t="str">
+        <v>null</v>
+      </c>
+      <c r="R77" t="str">
+        <v>null</v>
+      </c>
+      <c r="S77" t="str">
+        <v>null</v>
+      </c>
+      <c r="T77" t="str">
+        <v>null</v>
+      </c>
+      <c r="U77" t="str">
+        <v>null</v>
+      </c>
+      <c r="V77" t="str">
+        <v>null</v>
+      </c>
+      <c r="W77" t="str">
+        <v>null</v>
+      </c>
+      <c r="X77" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y77" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z77" t="str">
+        <v>null</v>
+      </c>
+      <c r="AA77" t="str">
+        <v>null</v>
+      </c>
+      <c r="AB77" t="str">
+        <v>null</v>
+      </c>
+      <c r="AC77" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_10|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_11|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_12|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_13|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_14|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_15|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_16|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_1|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_2|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_3|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_4|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_5|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_6|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_7|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_8|https://data.omgeving.vlaanderen.be/id/concept/lzs/norm_bandbreedte/_9</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter</v>
+      </c>
+      <c r="B78" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+      </c>
+      <c r="C78" t="str">
+        <v>null</v>
+      </c>
+      <c r="D78" t="str">
+        <v>null</v>
+      </c>
+      <c r="E78" t="str">
+        <v>null</v>
+      </c>
+      <c r="F78" t="str">
+        <v>conceptschema luchtzuiveringssysteem eigenschap</v>
+      </c>
+      <c r="G78" t="str">
+        <v>null</v>
+      </c>
+      <c r="H78" t="str">
+        <v>null</v>
+      </c>
+      <c r="I78" t="str">
+        <v>null</v>
+      </c>
+      <c r="J78" t="str">
+        <v>null</v>
+      </c>
+      <c r="K78" t="str">
+        <v>null</v>
+      </c>
+      <c r="L78" t="str">
+        <v>null</v>
+      </c>
+      <c r="M78" t="str">
+        <v>null</v>
+      </c>
+      <c r="N78" t="str">
+        <v>null</v>
+      </c>
+      <c r="O78" t="str">
+        <v>null</v>
+      </c>
+      <c r="P78" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q78" t="str">
+        <v>null</v>
+      </c>
+      <c r="R78" t="str">
+        <v>null</v>
+      </c>
+      <c r="S78" t="str">
+        <v>null</v>
+      </c>
+      <c r="T78" t="str">
+        <v>null</v>
+      </c>
+      <c r="U78" t="str">
+        <v>null</v>
+      </c>
+      <c r="V78" t="str">
+        <v>null</v>
+      </c>
+      <c r="W78" t="str">
+        <v>null</v>
+      </c>
+      <c r="X78" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y78" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z78" t="str">
+        <v>null</v>
+      </c>
+      <c r="AA78" t="str">
+        <v>null</v>
+      </c>
+      <c r="AB78" t="str">
+        <v>null</v>
+      </c>
+      <c r="AC78" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebiet|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/spuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/drukvaloverhetsysteem|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietvoorbevochtiging|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/waswaterdebietbevloeiing|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/zuurtegraadwaswater|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/geleidbaarheidvanhetwaswater|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspoelwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/biobedspuiwaterproductie|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/elektriciteitsverbruikwaterpompen|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/stalbezetting|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter/systeemstatus</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/parameter-norm</v>
+      </c>
+      <c r="B79" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+      </c>
+      <c r="C79" t="str">
+        <v>null</v>
+      </c>
+      <c r="D79" t="str">
+        <v>null</v>
+      </c>
+      <c r="E79" t="str">
+        <v>null</v>
+      </c>
+      <c r="F79" t="str">
+        <v>conceptschema luchtzuiveringssysteem parameter specificatie</v>
+      </c>
+      <c r="G79" t="str">
+        <v>null</v>
+      </c>
+      <c r="H79" t="str">
+        <v>null</v>
+      </c>
+      <c r="I79" t="str">
+        <v>Het schema van indelingsklassen (1, 2, 3) zoals vastgelegd in de Vlaamse milieuregelgeving (VLAREM).</v>
+      </c>
+      <c r="J79" t="str">
+        <v>Het schema van indelingsklassen (1, 2, 3) zoals vastgelegd in de Vlaamse milieuregelgeving (VLAREM).</v>
+      </c>
+      <c r="K79" t="str">
+        <v>null</v>
+      </c>
+      <c r="L79" t="str">
+        <v>null</v>
+      </c>
+      <c r="M79" t="str">
+        <v>null</v>
+      </c>
+      <c r="N79" t="str">
+        <v>null</v>
+      </c>
+      <c r="O79" t="str">
+        <v>null</v>
+      </c>
+      <c r="P79" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q79" t="str">
+        <v>null</v>
+      </c>
+      <c r="R79" t="str">
+        <v>null</v>
+      </c>
+      <c r="S79" t="str">
+        <v>null</v>
+      </c>
+      <c r="T79" t="str">
+        <v>null</v>
+      </c>
+      <c r="U79" t="str">
+        <v>null</v>
+      </c>
+      <c r="V79" t="str">
+        <v>null</v>
+      </c>
+      <c r="W79" t="str">
+        <v>null</v>
+      </c>
+      <c r="X79" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y79" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z79" t="str">
+        <v>null</v>
+      </c>
+      <c r="AA79" t="str">
+        <v>null</v>
+      </c>
+      <c r="AB79" t="str">
+        <v>null</v>
+      </c>
+      <c r="AC79" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_10|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_11|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_12|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_13|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_14|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_15|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_16|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_17|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_18|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_19|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_1|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_2|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_3|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_4|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_5|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_6|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_7|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_8|https://data.omgeving.vlaanderen.be/id/concept/lzs/parameter_norm/_9</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/stalbezetting</v>
+      </c>
+      <c r="B80" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+      </c>
+      <c r="C80" t="str">
+        <v>null</v>
+      </c>
+      <c r="D80" t="str">
+        <v>null</v>
+      </c>
+      <c r="E80" t="str">
+        <v>null</v>
+      </c>
+      <c r="F80" t="str">
+        <v>conceptschema luchtzuiveringssysteem stalbezetting</v>
+      </c>
+      <c r="G80" t="str">
+        <v>null</v>
+      </c>
+      <c r="H80" t="str">
+        <v>null</v>
+      </c>
+      <c r="I80" t="str">
+        <v>null</v>
+      </c>
+      <c r="J80" t="str">
+        <v>null</v>
+      </c>
+      <c r="K80" t="str">
+        <v>null</v>
+      </c>
+      <c r="L80" t="str">
+        <v>null</v>
+      </c>
+      <c r="M80" t="str">
+        <v>null</v>
+      </c>
+      <c r="N80" t="str">
+        <v>null</v>
+      </c>
+      <c r="O80" t="str">
+        <v>null</v>
+      </c>
+      <c r="P80" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q80" t="str">
+        <v>null</v>
+      </c>
+      <c r="R80" t="str">
+        <v>null</v>
+      </c>
+      <c r="S80" t="str">
+        <v>null</v>
+      </c>
+      <c r="T80" t="str">
+        <v>null</v>
+      </c>
+      <c r="U80" t="str">
+        <v>null</v>
+      </c>
+      <c r="V80" t="str">
+        <v>null</v>
+      </c>
+      <c r="W80" t="str">
+        <v>null</v>
+      </c>
+      <c r="X80" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y80" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z80" t="str">
+        <v>null</v>
+      </c>
+      <c r="AA80" t="str">
+        <v>null</v>
+      </c>
+      <c r="AB80" t="str">
+        <v>null</v>
+      </c>
+      <c r="AC80" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/stalbezetting/in_gebruik|https://data.omgeving.vlaanderen.be/id/concept/lzs/stalbezetting/leeg</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemstatus</v>
+      </c>
+      <c r="B81" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+      </c>
+      <c r="C81" t="str">
+        <v>null</v>
+      </c>
+      <c r="D81" t="str">
+        <v>null</v>
+      </c>
+      <c r="E81" t="str">
+        <v>null</v>
+      </c>
+      <c r="F81" t="str">
+        <v>conceptschema luchtzuiveringssysteem status</v>
+      </c>
+      <c r="G81" t="str">
+        <v>null</v>
+      </c>
+      <c r="H81" t="str">
+        <v>null</v>
+      </c>
+      <c r="I81" t="str">
+        <v>null</v>
+      </c>
+      <c r="J81" t="str">
+        <v>null</v>
+      </c>
+      <c r="K81" t="str">
+        <v>null</v>
+      </c>
+      <c r="L81" t="str">
+        <v>null</v>
+      </c>
+      <c r="M81" t="str">
+        <v>null</v>
+      </c>
+      <c r="N81" t="str">
+        <v>null</v>
+      </c>
+      <c r="O81" t="str">
+        <v>null</v>
+      </c>
+      <c r="P81" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q81" t="str">
+        <v>null</v>
+      </c>
+      <c r="R81" t="str">
+        <v>null</v>
+      </c>
+      <c r="S81" t="str">
+        <v>null</v>
+      </c>
+      <c r="T81" t="str">
+        <v>null</v>
+      </c>
+      <c r="U81" t="str">
+        <v>null</v>
+      </c>
+      <c r="V81" t="str">
+        <v>null</v>
+      </c>
+      <c r="W81" t="str">
+        <v>null</v>
+      </c>
+      <c r="X81" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y81" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z81" t="str">
+        <v>null</v>
+      </c>
+      <c r="AA81" t="str">
+        <v>null</v>
+      </c>
+      <c r="AB81" t="str">
+        <v>null</v>
+      </c>
+      <c r="AC81" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/status/gereinigd|https://data.omgeving.vlaanderen.be/id/concept/lzs/status/onderhoud|https://data.omgeving.vlaanderen.be/id/concept/lzs/status/operationeel|https://data.omgeving.vlaanderen.be/id/concept/lzs/status/storing</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/lzs/systeemtype</v>
+      </c>
+      <c r="B82" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+      </c>
+      <c r="C82" t="str">
+        <v>null</v>
+      </c>
+      <c r="D82" t="str">
+        <v>null</v>
+      </c>
+      <c r="E82" t="str">
+        <v>null</v>
+      </c>
+      <c r="F82" t="str">
+        <v>conceptschema luchtzuiveringssysteem</v>
+      </c>
+      <c r="G82" t="str">
+        <v>null</v>
+      </c>
+      <c r="H82" t="str">
+        <v>null</v>
+      </c>
+      <c r="I82" t="str">
+        <v>null</v>
+      </c>
+      <c r="J82" t="str">
+        <v>null</v>
+      </c>
+      <c r="K82" t="str">
+        <v>null</v>
+      </c>
+      <c r="L82" t="str">
+        <v>null</v>
+      </c>
+      <c r="M82" t="str">
+        <v>null</v>
+      </c>
+      <c r="N82" t="str">
+        <v>null</v>
+      </c>
+      <c r="O82" t="str">
+        <v>null</v>
+      </c>
+      <c r="P82" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q82" t="str">
+        <v>null</v>
+      </c>
+      <c r="R82" t="str">
+        <v>null</v>
+      </c>
+      <c r="S82" t="str">
+        <v>null</v>
+      </c>
+      <c r="T82" t="str">
+        <v>null</v>
+      </c>
+      <c r="U82" t="str">
+        <v>null</v>
+      </c>
+      <c r="V82" t="str">
+        <v>null</v>
+      </c>
+      <c r="W82" t="str">
+        <v>null</v>
+      </c>
+      <c r="X82" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y82" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z82" t="str">
+        <v>null</v>
+      </c>
+      <c r="AA82" t="str">
+        <v>null</v>
+      </c>
+      <c r="AB82" t="str">
+        <v>null</v>
+      </c>
+      <c r="AC82" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/lzs/type/luchtzuiveringssysteem</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/vlarem-klasse</v>
+      </c>
+      <c r="B83" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+      </c>
+      <c r="C83" t="str">
+        <v>null</v>
+      </c>
+      <c r="D83" t="str">
+        <v>null</v>
+      </c>
+      <c r="E83" t="str">
+        <v>null</v>
+      </c>
+      <c r="F83" t="str">
         <v>VLAREM indelingsklassen</v>
       </c>
-      <c r="G76" t="str">
-        <v>null</v>
-      </c>
-      <c r="H76" t="str">
-        <v>null</v>
-      </c>
-      <c r="I76" t="str">
-        <v>null</v>
-      </c>
-      <c r="J76" t="str">
-        <v>null</v>
-      </c>
-      <c r="K76" t="str">
-        <v>null</v>
-      </c>
-      <c r="L76" t="str">
-        <v>null</v>
-      </c>
-      <c r="M76" t="str">
-        <v>null</v>
-      </c>
-      <c r="N76" t="str">
-        <v>null</v>
-      </c>
-      <c r="O76" t="str">
-        <v>null</v>
-      </c>
-      <c r="P76" t="str">
-        <v>null</v>
-      </c>
-      <c r="Q76" t="str">
-        <v>null</v>
-      </c>
-      <c r="R76" t="str">
-        <v>null</v>
-      </c>
-      <c r="S76" t="str">
-        <v>null</v>
-      </c>
-      <c r="T76" t="str">
-        <v>null</v>
-      </c>
-      <c r="U76" t="str">
-        <v>null</v>
-      </c>
-      <c r="V76" t="str">
-        <v>null</v>
-      </c>
-      <c r="W76" t="str">
-        <v>null</v>
-      </c>
-      <c r="X76" t="str">
-        <v>null</v>
-      </c>
-      <c r="Y76" t="str">
-        <v>null</v>
-      </c>
-      <c r="Z76" t="str">
-        <v>null</v>
-      </c>
-      <c r="AA76" t="str">
-        <v>null</v>
-      </c>
-      <c r="AB76" t="str">
-        <v>null</v>
-      </c>
-      <c r="AC76" t="str">
+      <c r="G83" t="str">
+        <v>null</v>
+      </c>
+      <c r="H83" t="str">
+        <v>null</v>
+      </c>
+      <c r="I83" t="str">
+        <v>null</v>
+      </c>
+      <c r="J83" t="str">
+        <v>null</v>
+      </c>
+      <c r="K83" t="str">
+        <v>null</v>
+      </c>
+      <c r="L83" t="str">
+        <v>null</v>
+      </c>
+      <c r="M83" t="str">
+        <v>null</v>
+      </c>
+      <c r="N83" t="str">
+        <v>null</v>
+      </c>
+      <c r="O83" t="str">
+        <v>null</v>
+      </c>
+      <c r="P83" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q83" t="str">
+        <v>null</v>
+      </c>
+      <c r="R83" t="str">
+        <v>null</v>
+      </c>
+      <c r="S83" t="str">
+        <v>null</v>
+      </c>
+      <c r="T83" t="str">
+        <v>null</v>
+      </c>
+      <c r="U83" t="str">
+        <v>null</v>
+      </c>
+      <c r="V83" t="str">
+        <v>null</v>
+      </c>
+      <c r="W83" t="str">
+        <v>null</v>
+      </c>
+      <c r="X83" t="str">
+        <v>null</v>
+      </c>
+      <c r="Y83" t="str">
+        <v>null</v>
+      </c>
+      <c r="Z83" t="str">
+        <v>null</v>
+      </c>
+      <c r="AA83" t="str">
+        <v>null</v>
+      </c>
+      <c r="AB83" t="str">
+        <v>null</v>
+      </c>
+      <c r="AC83" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k1|https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k2|https://data.omgeving.vlaanderen.be/id/concept/vlarem-klasse/k3</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AC76"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AC83"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>